<commit_message>
feat– firstname length validation testcases have been added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -101,6 +101,81 @@
   </si>
   <si>
     <t xml:space="preserve">firstname equal to max range 80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRSTNAME_EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{    "errors": [        "size must be between 3 and 18",        "Firstname should not be blank"    ] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRSTNAME_PARAM_MISS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRSTNAME_SPACES_ONLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{    "errors": [        "Firstname should not be blank",        "size must be between 3 and 18"    ]} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRSTNAME_NUMERIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Booking should be created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRSTNAME_SPECIAL_CHARS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~`!@#^&amp;*()_+{}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRSTNAME_ALPHANUMERIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John123 @34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRSTNAME_LEADING_TRAILING_SPACES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Saravanans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_VALID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_LT_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_EQ_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_GT_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_EQ_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_PARAM_MISS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_SPACES_ONLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_NUMERIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_ALPHANUMERIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTNAME_LEADING_TRAILING_SPACES</t>
   </si>
 </sst>
 </file>
@@ -111,7 +186,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -139,6 +214,20 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -203,7 +292,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,6 +305,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,6 +319,22 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -478,7 +587,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -486,14 +595,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="33.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="44.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,227 +633,825 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
+        <v>201</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G2" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>202</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>203</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>204</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="n">
         <v>205</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>206</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>207</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>208</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>209</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>211</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>212</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>201</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>46013</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>46021</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3" t="n">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>202</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>203</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>204</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>205</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="4" t="n">
         <v>206</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>46013</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>46021</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="n">
+      <c r="C20" s="5"/>
+      <c r="D20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="4" t="n">
         <v>207</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>46013</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>46021</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="n">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="4" t="n">
         <v>208</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>46013</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>46021</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3" t="n">
+      <c r="C22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G22" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="4" t="n">
         <v>209</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>46013</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>46021</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="C23" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G23" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G24" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>211</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G25" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>212</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="6" t="n">
+        <v>46013</v>
+      </c>
+      <c r="G26" s="6" t="n">
+        <v>46021</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="4" t="n">
+        <f aca="false">919710288425</f>
+        <v>919710288425</v>
+      </c>
+      <c r="J26" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: add e-mail validation test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="118">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">FIRSTNAME_VALID</t>
   </si>
   <si>
-    <t xml:space="preserve">274</t>
+    <t xml:space="preserve">110</t>
   </si>
   <si>
     <t xml:space="preserve">SaravananSubbu</t>
@@ -79,6 +79,9 @@
     <t xml:space="preserve">subbusrvn@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">+91 9710288425</t>
+  </si>
+  <si>
     <t xml:space="preserve">firstname with in the range 3~ 18</t>
   </si>
   <si>
@@ -88,7 +91,7 @@
     <t xml:space="preserve">FIRSTNAME_LT_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">275</t>
+    <t xml:space="preserve">111</t>
   </si>
   <si>
     <t xml:space="preserve">sa</t>
@@ -103,7 +106,7 @@
     <t xml:space="preserve">FIRSTNAME_EQ_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">276</t>
+    <t xml:space="preserve">112</t>
   </si>
   <si>
     <t xml:space="preserve">Sar</t>
@@ -115,7 +118,7 @@
     <t xml:space="preserve">FIRSTNAME_GT_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">277</t>
+    <t xml:space="preserve">113</t>
   </si>
   <si>
     <t xml:space="preserve">SaravananSubramaniyan</t>
@@ -127,7 +130,7 @@
     <t xml:space="preserve">FIRSTNAME_EQ_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">278</t>
+    <t xml:space="preserve">114</t>
   </si>
   <si>
     <t xml:space="preserve">SaravananSubramani</t>
@@ -139,7 +142,7 @@
     <t xml:space="preserve">FIRSTNAME_EMPTY</t>
   </si>
   <si>
-    <t xml:space="preserve">279</t>
+    <t xml:space="preserve">115</t>
   </si>
   <si>
     <t xml:space="preserve">{    "errors": [        "size must be between 3 and 18",        "Firstname should not be blank"    ] </t>
@@ -148,13 +151,13 @@
     <t xml:space="preserve">FIRSTNAME_PARAM_MISS</t>
   </si>
   <si>
-    <t xml:space="preserve">280</t>
+    <t xml:space="preserve">116</t>
   </si>
   <si>
     <t xml:space="preserve">FIRSTNAME_SPACES_ONLY</t>
   </si>
   <si>
-    <t xml:space="preserve">281</t>
+    <t xml:space="preserve">117</t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
@@ -166,7 +169,7 @@
     <t xml:space="preserve">FIRSTNAME_NUMERIC</t>
   </si>
   <si>
-    <t xml:space="preserve">282</t>
+    <t xml:space="preserve">118</t>
   </si>
   <si>
     <t xml:space="preserve">firstname Numeric value check</t>
@@ -175,7 +178,7 @@
     <t xml:space="preserve">FIRSTNAME_SPECIAL_CHARS</t>
   </si>
   <si>
-    <t xml:space="preserve">283</t>
+    <t xml:space="preserve">119</t>
   </si>
   <si>
     <t xml:space="preserve">~`!@#^&amp;*()_+{}</t>
@@ -187,7 +190,7 @@
     <t xml:space="preserve">FIRSTNAME_ALPHANUMERIC</t>
   </si>
   <si>
-    <t xml:space="preserve">284</t>
+    <t xml:space="preserve">120</t>
   </si>
   <si>
     <t xml:space="preserve">John123 @34</t>
@@ -199,7 +202,7 @@
     <t xml:space="preserve">FIRSTNAME_LEADING_TRAILING_SPACES</t>
   </si>
   <si>
-    <t xml:space="preserve">285</t>
+    <t xml:space="preserve">121</t>
   </si>
   <si>
     <t xml:space="preserve">     Saravanans</t>
@@ -211,7 +214,7 @@
     <t xml:space="preserve">LASTNAME_VALID</t>
   </si>
   <si>
-    <t xml:space="preserve">286</t>
+    <t xml:space="preserve">122</t>
   </si>
   <si>
     <t xml:space="preserve">Saravanan S</t>
@@ -223,7 +226,7 @@
     <t xml:space="preserve">LASTNAME_LT_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">287</t>
+    <t xml:space="preserve">123</t>
   </si>
   <si>
     <t xml:space="preserve">Lastname less then min range 3</t>
@@ -232,7 +235,7 @@
     <t xml:space="preserve">LASTNAME_EQ_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">288</t>
+    <t xml:space="preserve">124</t>
   </si>
   <si>
     <t xml:space="preserve">Lastname equal to the min range 3</t>
@@ -241,7 +244,7 @@
     <t xml:space="preserve">LASTNAME_GT_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">289</t>
+    <t xml:space="preserve">125</t>
   </si>
   <si>
     <t xml:space="preserve">Saravanan Subramaniyan ABCDENTT</t>
@@ -253,7 +256,7 @@
     <t xml:space="preserve">LASTNAME_EQ_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">290</t>
+    <t xml:space="preserve">126</t>
   </si>
   <si>
     <t xml:space="preserve">Saravanan Subramaniyan ABCDENT</t>
@@ -265,25 +268,25 @@
     <t xml:space="preserve">LASTNAME_EMPTY</t>
   </si>
   <si>
-    <t xml:space="preserve">291</t>
+    <t xml:space="preserve">127</t>
   </si>
   <si>
     <t xml:space="preserve">LASTNAME_PARAM_MISS</t>
   </si>
   <si>
-    <t xml:space="preserve">292</t>
+    <t xml:space="preserve">128</t>
   </si>
   <si>
     <t xml:space="preserve">LASTNAME_SPACES_ONLY</t>
   </si>
   <si>
-    <t xml:space="preserve">293</t>
+    <t xml:space="preserve">129</t>
   </si>
   <si>
     <t xml:space="preserve">LASTNAME_NUMERIC</t>
   </si>
   <si>
-    <t xml:space="preserve">294</t>
+    <t xml:space="preserve">130</t>
   </si>
   <si>
     <t xml:space="preserve">Lastname Numeric value check</t>
@@ -292,7 +295,7 @@
     <t xml:space="preserve">LASTNAME_SPECIAL_CHARS</t>
   </si>
   <si>
-    <t xml:space="preserve">295</t>
+    <t xml:space="preserve">131</t>
   </si>
   <si>
     <t xml:space="preserve">L astnamespecial character value check</t>
@@ -301,7 +304,7 @@
     <t xml:space="preserve">LASTNAME_ALPHANUMERIC</t>
   </si>
   <si>
-    <t xml:space="preserve">296</t>
+    <t xml:space="preserve">132</t>
   </si>
   <si>
     <t xml:space="preserve">Lastname alpha numeric character value check</t>
@@ -310,10 +313,148 @@
     <t xml:space="preserve">LASTNAME_LEADING_TRAILING_SPACES</t>
   </si>
   <si>
-    <t xml:space="preserve">297</t>
+    <t xml:space="preserve">133</t>
   </si>
   <si>
     <t xml:space="preserve">Lastname trainling space before value check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL_VALID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saravanan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking request with valid e-mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL_EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">booking request with no e-mail
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{    "errors": [        "must not be empty"    ]} </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL_INVALID_FORMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testusergmail.com</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">booking request with invalid e-mail
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{    "errors": [        "must be a well-formed email address"    ]} </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL_NO_DOMAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subbusrvn@</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">booking request with e-mail with no domain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+{    "errors": [        "must be a well-formed email address"    ]} </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL_NO_USERNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@gmail.com</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">booking request with e-mail with no username
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{    "errors": [        "must be a well-formed email address"    ]} </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -324,7 +465,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -357,6 +498,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -429,7 +577,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,6 +620,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -724,7 +876,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -738,7 +890,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="23.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="44.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23"/>
   </cols>
@@ -803,26 +955,25 @@
       <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I2" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>14</v>
@@ -839,26 +990,25 @@
       <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>14</v>
@@ -875,26 +1025,25 @@
       <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>14</v>
@@ -911,26 +1060,25 @@
       <c r="H5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I5" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>14</v>
@@ -947,23 +1095,22 @@
       <c r="H6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I6" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
@@ -981,23 +1128,22 @@
       <c r="H7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="5" t="s">
@@ -1015,26 +1161,25 @@
       <c r="H8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I8" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>14</v>
@@ -1051,23 +1196,22 @@
       <c r="H9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I9" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>123456</v>
@@ -1087,26 +1231,25 @@
       <c r="H10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I10" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>14</v>
@@ -1123,26 +1266,25 @@
       <c r="H11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I11" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>14</v>
@@ -1159,26 +1301,25 @@
       <c r="H12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I12" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>14</v>
@@ -1195,26 +1336,25 @@
       <c r="H13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I13" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>13</v>
@@ -1231,29 +1371,28 @@
       <c r="H14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I14" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>15</v>
@@ -1267,29 +1406,28 @@
       <c r="H15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I15" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>15</v>
@@ -1303,29 +1441,28 @@
       <c r="H16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I16" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>15</v>
@@ -1339,29 +1476,28 @@
       <c r="H17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I17" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>15</v>
@@ -1375,26 +1511,25 @@
       <c r="H18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I18" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="5" t="s">
@@ -1409,26 +1544,25 @@
       <c r="H19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I19" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="5" t="s">
@@ -1443,29 +1577,28 @@
       <c r="H20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I20" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>15</v>
@@ -1479,26 +1612,25 @@
       <c r="H21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I21" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="9" t="n">
         <v>123456</v>
@@ -1515,29 +1647,28 @@
       <c r="H22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I22" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>15</v>
@@ -1551,29 +1682,28 @@
       <c r="H23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I23" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>15</v>
@@ -1587,29 +1717,28 @@
       <c r="H24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I24" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>15</v>
@@ -1623,19 +1752,189 @@
       <c r="H25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="5" t="n">
-        <f aca="false">919710288425</f>
-        <v>919710288425</v>
+      <c r="I25" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat: add checkin, checkout date validation test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="151">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -456,16 +456,116 @@
       <t xml:space="preserve">{    "errors": [        "must be a well-formed email address"    ]} </t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">DATES_VALID_RANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-12-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a valid check-in and check-out date range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Booking should created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_CHECKIN_AFTER_CHECKOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-12-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a check-in date after the check-out date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_SAME_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the same check-in and check-out date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_CHECKIN_IN_PAST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-12-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-12-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a check-in date in the past</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_CHECKIN_MISSING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-12-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a missing check-in date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_CHECKOUT_MISSING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a missing check-out date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_CHECKIN_TOO_FAR_IN_FUTURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_CHECKIN_NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_CHECKOUT_NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATES_TOO_LONG_STAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">329</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -509,8 +609,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF50C91C"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,13 +640,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7FF6BB"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFB0FA6D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEACEF9"/>
-        <bgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFDDB6F8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDF084"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDB6F8"/>
+        <bgColor rgb="FFEACEF9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB0FA6D"/>
+        <bgColor rgb="FF7FF6BB"/>
       </patternFill>
     </fill>
   </fills>
@@ -577,7 +709,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -622,7 +754,39 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -671,15 +835,15 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFB0FA6D"/>
+      <rgbColor rgb="FFFDF084"/>
       <rgbColor rgb="FF7FF6BB"/>
       <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFDDB6F8"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF50C91C"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -876,7 +1040,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -884,7 +1048,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.97"/>
@@ -1784,7 +1948,7 @@
       <c r="G26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="11" t="s">
         <v>18</v>
       </c>
       <c r="I26" s="5" t="s">
@@ -1819,7 +1983,7 @@
       <c r="G27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="4"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="5" t="s">
         <v>19</v>
       </c>
@@ -1852,7 +2016,7 @@
       <c r="G28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="12" t="s">
         <v>108</v>
       </c>
       <c r="I28" s="5" t="s">
@@ -1887,7 +2051,7 @@
       <c r="G29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="13" t="s">
         <v>112</v>
       </c>
       <c r="I29" s="5" t="s">
@@ -1922,7 +2086,7 @@
       <c r="G30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="13" t="s">
         <v>116</v>
       </c>
       <c r="I30" s="5" t="s">
@@ -1933,6 +2097,352 @@
       </c>
       <c r="K30" s="4" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G36" s="15"/>
+      <c r="H36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="18" t="n">
+        <v>46388</v>
+      </c>
+      <c r="G37" s="18" t="n">
+        <v>46397</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="18" t="n">
+        <v>46023</v>
+      </c>
+      <c r="G40" s="18" t="n">
+        <v>46387</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add depostTruu validation test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="168">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -555,6 +555,57 @@
   <si>
     <t xml:space="preserve">329</t>
   </si>
+  <si>
+    <t xml:space="preserve">DEPOSIT_TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking creation with deposit true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPOSIT_FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking creation with deposit false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPOSIT_STRING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“true”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking creation with deposit as string value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPOSIT_NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking creation with deposit as number value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPOSIT_INVALID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!@AS12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking creation with deposit as alpha numeric value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPOSIT_MISSING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking creation without deposit</t>
+  </si>
 </sst>
 </file>
 
@@ -565,7 +616,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -623,8 +674,23 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF50C91C"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Mono;Courier New;DejaVu Sans Mono;Lucida Sans Typewriter"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -640,7 +706,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7FF6BB"/>
-        <bgColor rgb="FFB0FA6D"/>
+        <bgColor rgb="FF9EEFF5"/>
       </patternFill>
     </fill>
     <fill>
@@ -664,6 +730,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB0FA6D"/>
+        <bgColor rgb="FF7FF6BB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9EEFF5"/>
         <bgColor rgb="FF7FF6BB"/>
       </patternFill>
     </fill>
@@ -709,7 +781,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -790,6 +862,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,10 +926,10 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF7FF6BB"/>
       <rgbColor rgb="FFB0FA6D"/>
       <rgbColor rgb="FFFDF084"/>
-      <rgbColor rgb="FF7FF6BB"/>
+      <rgbColor rgb="FF9EEFF5"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFDDB6F8"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -1040,7 +1132,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2441,11 +2533,225 @@
       <c r="J40" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="K40" s="16" t="s">
+      <c r="K40" s="20" t="s">
         <v>122</v>
       </c>
     </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="22" t="n">
+        <v>330</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G41" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="K41" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="22" t="n">
+        <v>331</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G42" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="22" t="n">
+        <v>333</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="F43" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G43" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="22" t="n">
+        <v>334</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="F44" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G44" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="22" t="n">
+        <v>335</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G45" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" s="22" t="n">
+        <v>336</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="F46" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G46" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E45" r:id="rId1" display="!@AS12"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
feat: add phone number validation testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="194">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -644,6 +644,45 @@
   </si>
   <si>
     <t xml:space="preserve">booking creation without deposit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHONE_VALID_MIN_LENGTH_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91971028842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking with valid phone number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHONE_VALID_MAX_LENGTH_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91 971028842523456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHONE_TOO_SHORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9710288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking with invalid phone number(Too short)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHONE_TOO_LONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91 97102884259710288425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booking with invalid phone number(Too lengthy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHONE_EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{    "errors": [        "must not be empty",        "size must be between 11 and 21"    ]} </t>
   </si>
 </sst>
 </file>
@@ -811,7 +850,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -910,6 +949,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1162,9 +1205,9 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1176,7 +1219,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="44.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23"/>
   </cols>
@@ -2452,7 +2495,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
         <v>132</v>
       </c>
@@ -2487,7 +2530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
         <v>136</v>
       </c>
@@ -2522,7 +2565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
         <v>140</v>
       </c>
@@ -2557,7 +2600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
         <v>143</v>
       </c>
@@ -2592,7 +2635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
         <v>148</v>
       </c>
@@ -2625,7 +2668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="18" t="s">
         <v>152</v>
       </c>
@@ -2658,7 +2701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
         <v>155</v>
       </c>
@@ -2693,7 +2736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
         <v>157</v>
       </c>
@@ -2728,7 +2771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
         <v>160</v>
       </c>
@@ -2763,7 +2806,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
         <v>162</v>
       </c>
@@ -2798,7 +2841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="21" t="s">
         <v>164</v>
       </c>
@@ -2833,7 +2876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="21" t="s">
         <v>166</v>
       </c>
@@ -2868,7 +2911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="21" t="s">
         <v>169</v>
       </c>
@@ -2903,7 +2946,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="21" t="s">
         <v>172</v>
       </c>
@@ -2938,7 +2981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="21" t="s">
         <v>175</v>
       </c>
@@ -2973,7 +3016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="21" t="s">
         <v>178</v>
       </c>
@@ -3008,6 +3051,181 @@
         <v>23</v>
       </c>
     </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="22" t="n">
+        <v>340</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G54" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J54" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="22" t="n">
+        <v>341</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G55" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J55" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" s="22" t="n">
+        <v>342</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G56" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="J56" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" s="22" t="n">
+        <v>343</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G57" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J57" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" s="22" t="n">
+        <v>344</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G58" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I58" s="4"/>
+      <c r="J58" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E52" r:id="rId1" display="!@AS12"/>

</xml_diff>

<commit_message>
feat: add end to end cases added and validated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="205">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -695,6 +695,27 @@
   </si>
   <si>
     <t xml:space="preserve">BOOKING_VALID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_E2E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_UPDATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samyuktha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saravanan_Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samsaravanan@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">919710288178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Booking should be updated</t>
   </si>
 </sst>
 </file>
@@ -967,7 +988,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3276,11 +3297,11 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="8" t="s">
         <v>197</v>
       </c>
       <c r="B60" s="22" t="n">
-        <v>356</v>
+        <v>588</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>80</v>
@@ -3310,7 +3331,74 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B61" s="22" t="n">
+        <v>4652</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G61" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="J61" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62" s="22" t="n">
+        <v>5875</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F62" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G62" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J62" s="25"/>
+      <c r="K62" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
refactor – phone, email assertion refactored
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -3301,7 +3301,7 @@
         <v>197</v>
       </c>
       <c r="B60" s="22" t="n">
-        <v>588</v>
+        <v>12323</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>80</v>
@@ -3336,7 +3336,7 @@
         <v>198</v>
       </c>
       <c r="B61" s="22" t="n">
-        <v>4652</v>
+        <v>232</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>80</v>
@@ -3371,7 +3371,7 @@
         <v>199</v>
       </c>
       <c r="B62" s="22" t="n">
-        <v>5875</v>
+        <v>4</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>200</v>

</xml_diff>

<commit_message>
feat: add testcase, response data structure should follow the Swagger booking contract
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="206">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -716,6 +716,9 @@
   </si>
   <si>
     <t xml:space="preserve">Booking should be updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWAGGER_VALIDATION</t>
   </si>
 </sst>
 </file>
@@ -3399,6 +3402,39 @@
         <v>204</v>
       </c>
     </row>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B63" s="22" t="n">
+        <v>5687</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G63" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J63" s="25"/>
+      <c r="K63" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
style – feature file readability improved
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -697,28 +697,28 @@
     <t xml:space="preserve">BOOKING_VALID</t>
   </si>
   <si>
+    <t xml:space="preserve">SWAGGER_VALIDATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samyuktha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samsaravanan@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">919710288178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Booking should be updated</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOOKING_E2E</t>
   </si>
   <si>
     <t xml:space="preserve">BOOKING_UPDATE</t>
   </si>
   <si>
-    <t xml:space="preserve">Samyuktha</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saravanan_Update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">samsaravanan@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">919710288178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Booking should be updated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SWAGGER_VALIDATION</t>
   </si>
 </sst>
 </file>
@@ -3335,17 +3335,17 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="21" t="s">
         <v>198</v>
       </c>
       <c r="B61" s="22" t="n">
-        <v>232</v>
+        <v>5687</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>80</v>
+        <v>199</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>15</v>
@@ -3357,33 +3357,31 @@
         <v>46022</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>18</v>
+        <v>200</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="J61" s="25" t="s">
-        <v>196</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="J61" s="25"/>
       <c r="K61" s="7" t="s">
-        <v>20</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
-        <v>199</v>
+      <c r="A62" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="B62" s="22" t="n">
-        <v>4</v>
+        <v>232</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>167</v>
+        <v>15</v>
       </c>
       <c r="F62" s="24" t="n">
         <v>46019</v>
@@ -3392,31 +3390,33 @@
         <v>46022</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>202</v>
+        <v>18</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="J62" s="25"/>
+        <v>195</v>
+      </c>
+      <c r="J62" s="25" t="s">
+        <v>196</v>
+      </c>
       <c r="K62" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="8" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="21" t="s">
+      <c r="B63" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B63" s="22" t="n">
-        <v>5687</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="E63" s="4" t="s">
-        <v>15</v>
+        <v>167</v>
       </c>
       <c r="F63" s="24" t="n">
         <v>46019</v>
@@ -3425,16 +3425,20 @@
         <v>46022</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J63" s="25"/>
       <c r="K63" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
chore - joson schema validaor dependency version upgrated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -3372,7 +3372,7 @@
         <v>203</v>
       </c>
       <c r="B62" s="22" t="n">
-        <v>232</v>
+        <v>1012</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>80</v>
@@ -3407,7 +3407,7 @@
         <v>204</v>
       </c>
       <c r="B63" s="22" t="n">
-        <v>4</v>
+        <v>1013</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
feat -Patch operation included in the E2E booking process and format done for all the source
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -3372,7 +3372,7 @@
         <v>203</v>
       </c>
       <c r="B62" s="22" t="n">
-        <v>1012</v>
+        <v>1067</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>80</v>
@@ -3407,7 +3407,7 @@
         <v>204</v>
       </c>
       <c r="B63" s="22" t="n">
-        <v>1013</v>
+        <v>1068</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
feat-  Room-Id taken dynamically as random number implemeneted, E2E cases separated as feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="171">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -58,33 +58,33 @@
     <t xml:space="preserve">ROOMID_VALID</t>
   </si>
   <si>
+    <t xml:space="preserve">Saravanan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subramaniyan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-12-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-12-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subbusrvn@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+91 9710288425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Booking should be created</t>
+  </si>
+  <si>
     <t xml:space="preserve">300</t>
   </si>
   <si>
-    <t xml:space="preserve">Saravanan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subramaniyan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-12-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-12-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subbusrvn@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+91 9710288425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Booking should be created</t>
-  </si>
-  <si>
     <t xml:space="preserve">ROOMID_OUT_OF_RANGE</t>
   </si>
   <si>
@@ -109,6 +109,9 @@
     <t xml:space="preserve">ROOMID_ALPHANUMERIC</t>
   </si>
   <si>
+    <t xml:space="preserve">ABC1000</t>
+  </si>
+  <si>
     <t xml:space="preserve">ABC100</t>
   </si>
   <si>
@@ -121,15 +124,15 @@
     <t xml:space="preserve">ROOMID_SPECIAL_CHARS</t>
   </si>
   <si>
+    <t xml:space="preserve">!@!@#$!</t>
+  </si>
+  <si>
     <t xml:space="preserve">!@#$%543</t>
   </si>
   <si>
     <t xml:space="preserve">FIRSTNAME_VALID</t>
   </si>
   <si>
-    <t xml:space="preserve">110</t>
-  </si>
-  <si>
     <t xml:space="preserve">SaravananSubbu</t>
   </si>
   <si>
@@ -139,9 +142,6 @@
     <t xml:space="preserve">FIRSTNAME_LT_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">111</t>
-  </si>
-  <si>
     <t xml:space="preserve">sa</t>
   </si>
   <si>
@@ -151,9 +151,6 @@
     <t xml:space="preserve">FIRSTNAME_EQ_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">112</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sar</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t xml:space="preserve">FIRSTNAME_GT_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">113</t>
-  </si>
-  <si>
     <t xml:space="preserve">SaravananSubramaniyan</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
     <t xml:space="preserve">FIRSTNAME_EQ_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">114</t>
-  </si>
-  <si>
     <t xml:space="preserve">SaravananSubramani</t>
   </si>
   <si>
@@ -187,24 +178,15 @@
     <t xml:space="preserve">FIRSTNAME_EMPTY</t>
   </si>
   <si>
-    <t xml:space="preserve">115</t>
-  </si>
-  <si>
     <t xml:space="preserve">{    "errors": [        "size must be between 3 and 18",        "Firstname should not be blank"    ] </t>
   </si>
   <si>
     <t xml:space="preserve">FIRSTNAME_PARAM_MISS</t>
   </si>
   <si>
-    <t xml:space="preserve">116</t>
-  </si>
-  <si>
     <t xml:space="preserve">FIRSTNAME_SPACES_ONLY</t>
   </si>
   <si>
-    <t xml:space="preserve">117</t>
-  </si>
-  <si>
     <t xml:space="preserve">   </t>
   </si>
   <si>
@@ -214,18 +196,12 @@
     <t xml:space="preserve">FIRSTNAME_NUMERIC</t>
   </si>
   <si>
-    <t xml:space="preserve">118</t>
-  </si>
-  <si>
     <t xml:space="preserve">firstname Numeric value check</t>
   </si>
   <si>
     <t xml:space="preserve">FIRSTNAME_SPECIAL_CHARS</t>
   </si>
   <si>
-    <t xml:space="preserve">119</t>
-  </si>
-  <si>
     <t xml:space="preserve">~`!@#^&amp;*()_+{}</t>
   </si>
   <si>
@@ -235,9 +211,6 @@
     <t xml:space="preserve">FIRSTNAME_ALPHANUMERIC</t>
   </si>
   <si>
-    <t xml:space="preserve">120</t>
-  </si>
-  <si>
     <t xml:space="preserve">John123 @34</t>
   </si>
   <si>
@@ -247,9 +220,6 @@
     <t xml:space="preserve">FIRSTNAME_LEADING_TRAILING_SPACES</t>
   </si>
   <si>
-    <t xml:space="preserve">121</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Saravanans</t>
   </si>
   <si>
@@ -259,9 +229,6 @@
     <t xml:space="preserve">LASTNAME_VALID</t>
   </si>
   <si>
-    <t xml:space="preserve">122</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saravanan S</t>
   </si>
   <si>
@@ -271,27 +238,18 @@
     <t xml:space="preserve">LASTNAME_LT_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">123</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lastname less then min range 3</t>
   </si>
   <si>
     <t xml:space="preserve">LASTNAME_EQ_MIN</t>
   </si>
   <si>
-    <t xml:space="preserve">124</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lastname equal to the min range 3</t>
   </si>
   <si>
     <t xml:space="preserve">LASTNAME_GT_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">125</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saravanan Subramaniyan ABCDENTT</t>
   </si>
   <si>
@@ -301,9 +259,6 @@
     <t xml:space="preserve">LASTNAME_EQ_MAX</t>
   </si>
   <si>
-    <t xml:space="preserve">126</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saravanan Subramaniyan ABCDENT</t>
   </si>
   <si>
@@ -313,70 +268,43 @@
     <t xml:space="preserve">LASTNAME_EMPTY</t>
   </si>
   <si>
-    <t xml:space="preserve">127</t>
-  </si>
-  <si>
     <t xml:space="preserve">LASTNAME_PARAM_MISS</t>
   </si>
   <si>
-    <t xml:space="preserve">128</t>
-  </si>
-  <si>
     <t xml:space="preserve">LASTNAME_SPACES_ONLY</t>
   </si>
   <si>
-    <t xml:space="preserve">129</t>
-  </si>
-  <si>
     <t xml:space="preserve">LASTNAME_NUMERIC</t>
   </si>
   <si>
-    <t xml:space="preserve">130</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lastname Numeric value check</t>
   </si>
   <si>
     <t xml:space="preserve">LASTNAME_SPECIAL_CHARS</t>
   </si>
   <si>
-    <t xml:space="preserve">131</t>
-  </si>
-  <si>
     <t xml:space="preserve">L astnamespecial character value check</t>
   </si>
   <si>
     <t xml:space="preserve">LASTNAME_ALPHANUMERIC</t>
   </si>
   <si>
-    <t xml:space="preserve">132</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lastname alpha numeric character value check</t>
   </si>
   <si>
     <t xml:space="preserve">LASTNAME_LEADING_TRAILING_SPACES</t>
   </si>
   <si>
-    <t xml:space="preserve">133</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lastname trainling space before value check</t>
   </si>
   <si>
     <t xml:space="preserve">EMAIL_VALID</t>
   </si>
   <si>
-    <t xml:space="preserve">134</t>
-  </si>
-  <si>
     <t xml:space="preserve">booking request with valid e-mail</t>
   </si>
   <si>
     <t xml:space="preserve">EMAIL_EMPTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">135</t>
   </si>
   <si>
     <r>
@@ -405,9 +333,6 @@
     <t xml:space="preserve">EMAIL_INVALID_FORMAT</t>
   </si>
   <si>
-    <t xml:space="preserve">136</t>
-  </si>
-  <si>
     <t xml:space="preserve">testusergmail.com</t>
   </si>
   <si>
@@ -435,9 +360,6 @@
   </si>
   <si>
     <t xml:space="preserve">EMAIL_NO_DOMAIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">137</t>
   </si>
   <si>
     <t xml:space="preserve">subbusrvn@</t>
@@ -470,9 +392,6 @@
     <t xml:space="preserve">EMAIL_NO_USERNAME</t>
   </si>
   <si>
-    <t xml:space="preserve">138</t>
-  </si>
-  <si>
     <t xml:space="preserve">@gmail.com</t>
   </si>
   <si>
@@ -502,9 +421,6 @@
     <t xml:space="preserve">DATES_VALID_RANGE</t>
   </si>
   <si>
-    <t xml:space="preserve">320</t>
-  </si>
-  <si>
     <t xml:space="preserve">2025-12-28</t>
   </si>
   <si>
@@ -514,9 +430,6 @@
     <t xml:space="preserve">DATES_CHECKIN_AFTER_CHECKOUT</t>
   </si>
   <si>
-    <t xml:space="preserve">321</t>
-  </si>
-  <si>
     <t xml:space="preserve">2025-12-01</t>
   </si>
   <si>
@@ -526,18 +439,12 @@
     <t xml:space="preserve">DATES_SAME_DAY</t>
   </si>
   <si>
-    <t xml:space="preserve">322</t>
-  </si>
-  <si>
     <t xml:space="preserve">the same check-in and check-out date</t>
   </si>
   <si>
     <t xml:space="preserve">DATES_CHECKIN_IN_PAST</t>
   </si>
   <si>
-    <t xml:space="preserve">323</t>
-  </si>
-  <si>
     <t xml:space="preserve">2025-12-15</t>
   </si>
   <si>
@@ -550,9 +457,6 @@
     <t xml:space="preserve">DATES_CHECKIN_MISSING</t>
   </si>
   <si>
-    <t xml:space="preserve">324</t>
-  </si>
-  <si>
     <t xml:space="preserve">2025-12-31</t>
   </si>
   <si>
@@ -562,39 +466,24 @@
     <t xml:space="preserve">DATES_CHECKOUT_MISSING</t>
   </si>
   <si>
-    <t xml:space="preserve">325</t>
-  </si>
-  <si>
     <t xml:space="preserve">a missing check-out date</t>
   </si>
   <si>
     <t xml:space="preserve">DATES_CHECKIN_TOO_FAR_IN_FUTURE</t>
   </si>
   <si>
-    <t xml:space="preserve">326</t>
-  </si>
-  <si>
     <t xml:space="preserve">DATES_CHECKIN_NULL</t>
   </si>
   <si>
-    <t xml:space="preserve">327</t>
-  </si>
-  <si>
     <t xml:space="preserve">null</t>
   </si>
   <si>
     <t xml:space="preserve">DATES_CHECKOUT_NULL</t>
   </si>
   <si>
-    <t xml:space="preserve">328</t>
-  </si>
-  <si>
     <t xml:space="preserve">DATES_TOO_LONG_STAY</t>
   </si>
   <si>
-    <t xml:space="preserve">329</t>
-  </si>
-  <si>
     <t xml:space="preserve">DEPOSIT_TRUE</t>
   </si>
   <si>
@@ -719,6 +608,12 @@
   </si>
   <si>
     <t xml:space="preserve">Saravanan_Update</t>
+  </si>
+  <si>
+    <t>904291180</t>
+  </si>
+  <si>
+    <t>904294059</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1140,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1253,15 +1148,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="44.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="35.94" collapsed="false" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.74" collapsed="false" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="25.92" collapsed="false" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="34.97" collapsed="false" outlineLevel="0"/>
+    <col min="5" max="7" customWidth="true" hidden="false" style="1" width="11.85" collapsed="false" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="22.44" collapsed="false" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="26.89" collapsed="false" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="44.38" collapsed="false" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="23.0" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,32 +1198,33 @@
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1340,29 +1236,32 @@
         <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,29 +1272,32 @@
         <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,29 +1308,32 @@
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,159 +1344,164 @@
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="L6" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="L7" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="L8" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="B10" s="4"/>
       <c r="C10" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>41</v>
@@ -1604,67 +1514,63 @@
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="4" t="s">
+      <c r="K11" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>23</v>
@@ -1672,67 +1578,63 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="K13" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>55</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="9"/>
       <c r="D14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>23</v>
@@ -1740,32 +1642,30 @@
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B15" s="4"/>
       <c r="C15" s="9"/>
       <c r="D15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>23</v>
@@ -1773,34 +1673,32 @@
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>23</v>
@@ -1808,209 +1706,197 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B17" s="4"/>
       <c r="C17" s="9" t="n">
         <v>123456</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>67</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="9" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>71</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="9" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>75</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="9" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>79</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>83</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>23</v>
@@ -2018,69 +1904,65 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>86</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>23</v>
@@ -2088,67 +1970,63 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>93</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="4" t="s">
+      <c r="K25" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>23</v>
@@ -2156,32 +2034,30 @@
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>23</v>
@@ -2189,34 +2065,32 @@
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>101</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>23</v>
@@ -2224,207 +2098,195 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>103</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D29" s="11" t="n">
         <v>123456</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K29" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>106</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K30" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>109</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K32" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>115</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K33" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>118</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H34" s="14"/>
       <c r="I34" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="K34" s="8" t="s">
         <v>23</v>
@@ -2432,34 +2294,32 @@
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>121</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>23</v>
@@ -2467,34 +2327,32 @@
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>125</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="K36" s="8" t="s">
         <v>23</v>
@@ -2502,34 +2360,32 @@
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>129</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>23</v>
@@ -2537,69 +2393,65 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>133</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K38" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="K38" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>137</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>23</v>
@@ -2607,34 +2459,32 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>141</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="K40" s="8" t="s">
         <v>23</v>
@@ -2642,34 +2492,32 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>144</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B41" s="4"/>
       <c r="C41" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>23</v>
@@ -2677,32 +2525,30 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>149</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="17" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="K42" s="8" t="s">
         <v>23</v>
@@ -2710,32 +2556,30 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>153</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="B43" s="4"/>
       <c r="C43" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="G43" s="17"/>
       <c r="H43" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>23</v>
@@ -2743,19 +2587,17 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>156</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F44" s="19" t="n">
         <v>46388</v>
@@ -2764,48 +2606,46 @@
         <v>46397</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K44" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>158</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B45" s="4"/>
       <c r="C45" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>23</v>
@@ -2813,34 +2653,32 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>161</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B46" s="4"/>
       <c r="C46" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="K46" s="8" t="s">
         <v>23</v>
@@ -2848,19 +2686,17 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>163</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F47" s="19" t="n">
         <v>46023</v>
@@ -2869,33 +2705,31 @@
         <v>46387</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K47" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="K47" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="B48" s="22" t="n">
-        <v>330</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B48" s="22"/>
       <c r="C48" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F48" s="24" t="n">
         <v>46019</v>
@@ -2904,33 +2738,31 @@
         <v>46022</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="K48" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J48" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K48" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="B49" s="22" t="n">
-        <v>331</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="B49" s="22"/>
       <c r="C49" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="F49" s="24" t="n">
         <v>46019</v>
@@ -2939,33 +2771,31 @@
         <v>46022</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I49" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="K49" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K49" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="B50" s="22" t="n">
-        <v>333</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="B50" s="22"/>
       <c r="C50" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="F50" s="24" t="n">
         <v>46019</v>
@@ -2974,13 +2804,13 @@
         <v>46022</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="K50" s="8" t="s">
         <v>23</v>
@@ -2988,19 +2818,17 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="B51" s="22" t="n">
-        <v>334</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="B51" s="22"/>
       <c r="C51" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="F51" s="24" t="n">
         <v>46019</v>
@@ -3009,13 +2837,13 @@
         <v>46022</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J51" s="8" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="K51" s="8" t="s">
         <v>23</v>
@@ -3023,19 +2851,17 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="B52" s="22" t="n">
-        <v>335</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B52" s="22"/>
       <c r="C52" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="F52" s="24" t="n">
         <v>46019</v>
@@ -3044,13 +2870,13 @@
         <v>46022</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J52" s="8" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="K52" s="8" t="s">
         <v>23</v>
@@ -3058,19 +2884,17 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="B53" s="22" t="n">
-        <v>336</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B53" s="22"/>
       <c r="C53" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>179</v>
+        <v>142</v>
       </c>
       <c r="F53" s="24" t="n">
         <v>46019</v>
@@ -3079,13 +2903,13 @@
         <v>46022</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J53" s="8" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="K53" s="8" t="s">
         <v>23</v>
@@ -3093,19 +2917,17 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="B54" s="22" t="n">
-        <v>340</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="B54" s="22"/>
       <c r="C54" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F54" s="24" t="n">
         <v>46019</v>
@@ -3114,33 +2936,31 @@
         <v>46022</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="J54" s="18" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="B55" s="22" t="n">
-        <v>341</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="B55" s="22"/>
       <c r="C55" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F55" s="24" t="n">
         <v>46019</v>
@@ -3149,33 +2969,31 @@
         <v>46022</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>185</v>
+        <v>148</v>
       </c>
       <c r="J55" s="18" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="K55" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="B56" s="22" t="n">
-        <v>342</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="B56" s="22"/>
       <c r="C56" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F56" s="24" t="n">
         <v>46019</v>
@@ -3184,13 +3002,13 @@
         <v>46022</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="J56" s="18" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="K56" s="8" t="s">
         <v>23</v>
@@ -3198,19 +3016,17 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B57" s="22" t="n">
-        <v>343</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="B57" s="22"/>
       <c r="C57" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F57" s="24" t="n">
         <v>46019</v>
@@ -3219,13 +3035,13 @@
         <v>46022</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="J57" s="18" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="K57" s="8" t="s">
         <v>23</v>
@@ -3233,19 +3049,17 @@
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="B58" s="22" t="n">
-        <v>344</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="B58" s="22"/>
       <c r="C58" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F58" s="24" t="n">
         <v>46019</v>
@@ -3254,11 +3068,11 @@
         <v>46022</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="25" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="K58" s="8" t="s">
         <v>23</v>
@@ -3266,19 +3080,17 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="B59" s="22" t="n">
-        <v>355</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="B59" s="22"/>
       <c r="C59" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F59" s="24" t="n">
         <v>46019</v>
@@ -3287,33 +3099,31 @@
         <v>46022</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="J59" s="25" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="B60" s="22" t="n">
-        <v>12323</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="B60" s="22"/>
       <c r="C60" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F60" s="24" t="n">
         <v>46019</v>
@@ -3322,33 +3132,31 @@
         <v>46022</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="J60" s="25" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="K60" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="B61" s="22" t="n">
-        <v>5687</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="B61" s="22"/>
       <c r="C61" s="4" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F61" s="24" t="n">
         <v>46019</v>
@@ -3357,31 +3165,31 @@
         <v>46022</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="J61" s="25"/>
       <c r="K61" s="7" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="B62" s="22" t="n">
-        <v>1067</v>
+        <v>166</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>169</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F62" s="24" t="n">
         <v>46019</v>
@@ -3390,33 +3198,33 @@
         <v>46022</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="J62" s="25" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="K62" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B63" s="22" t="n">
-        <v>1068</v>
+        <v>167</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>170</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="F63" s="24" t="n">
         <v>46019</v>
@@ -3425,14 +3233,14 @@
         <v>46022</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="J63" s="25"/>
       <c r="K63" s="7" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
feat-  Delete End Testcase validation added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="170">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -610,10 +610,7 @@
     <t xml:space="preserve">Saravanan_Update</t>
   </si>
   <si>
-    <t>904291180</t>
-  </si>
-  <si>
-    <t>904294059</t>
+    <t>917421608</t>
   </si>
 </sst>
 </file>
@@ -3115,7 +3112,9 @@
       <c r="A60" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B60" s="22"/>
+      <c r="B60" s="22" t="s">
+        <v>169</v>
+      </c>
       <c r="C60" s="4" t="s">
         <v>69</v>
       </c>
@@ -3179,9 +3178,7 @@
       <c r="A62" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="B62" s="22" t="s">
-        <v>169</v>
-      </c>
+      <c r="B62" s="22"/>
       <c r="C62" s="4" t="s">
         <v>69</v>
       </c>
@@ -3214,9 +3211,7 @@
       <c r="A63" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B63" s="22" t="s">
-        <v>170</v>
-      </c>
+      <c r="B63" s="22"/>
       <c r="C63" s="4" t="s">
         <v>162</v>
       </c>

</xml_diff>

<commit_message>
feat - Update Negative Scenarios are added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="247">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -586,6 +586,30 @@
     <t xml:space="preserve">BOOKING_VALID</t>
   </si>
   <si>
+    <t xml:space="preserve">BOOKING_VALID_UPDATE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_UPDATE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_UPDATE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_UPDATE4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_UPDATE5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_UPDATE6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_UPDATE7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_UPDATE8</t>
+  </si>
+  <si>
     <t xml:space="preserve">SWAGGER_VALIDATION</t>
   </si>
   <si>
@@ -610,7 +634,214 @@
     <t xml:space="preserve">Saravanan_Update</t>
   </si>
   <si>
-    <t>949147798</t>
+    <t xml:space="preserve">BOOKING_VALID_DELETE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_DELETE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOKING_VALID_DELETE3</t>
+  </si>
+  <si>
+    <t>986818883</t>
+  </si>
+  <si>
+    <t>986826080</t>
+  </si>
+  <si>
+    <t>986826815</t>
+  </si>
+  <si>
+    <t>986827521</t>
+  </si>
+  <si>
+    <t>986828657</t>
+  </si>
+  <si>
+    <t>986829421</t>
+  </si>
+  <si>
+    <t>986830168</t>
+  </si>
+  <si>
+    <t>986831218</t>
+  </si>
+  <si>
+    <t>986832408</t>
+  </si>
+  <si>
+    <t>986833186</t>
+  </si>
+  <si>
+    <t>986833991</t>
+  </si>
+  <si>
+    <t>986834750</t>
+  </si>
+  <si>
+    <t>986835521</t>
+  </si>
+  <si>
+    <t>986836297</t>
+  </si>
+  <si>
+    <t>986837099</t>
+  </si>
+  <si>
+    <t>986837883</t>
+  </si>
+  <si>
+    <t>986838938</t>
+  </si>
+  <si>
+    <t>986839728</t>
+  </si>
+  <si>
+    <t>986840543</t>
+  </si>
+  <si>
+    <t>986841505</t>
+  </si>
+  <si>
+    <t>986842825</t>
+  </si>
+  <si>
+    <t>986843655</t>
+  </si>
+  <si>
+    <t>986844484</t>
+  </si>
+  <si>
+    <t>986845314</t>
+  </si>
+  <si>
+    <t>986846378</t>
+  </si>
+  <si>
+    <t>986847249</t>
+  </si>
+  <si>
+    <t>986848301</t>
+  </si>
+  <si>
+    <t>986849155</t>
+  </si>
+  <si>
+    <t>986850231</t>
+  </si>
+  <si>
+    <t>986851109</t>
+  </si>
+  <si>
+    <t>986851994</t>
+  </si>
+  <si>
+    <t>986853444</t>
+  </si>
+  <si>
+    <t>986854721</t>
+  </si>
+  <si>
+    <t>986855612</t>
+  </si>
+  <si>
+    <t>986856668</t>
+  </si>
+  <si>
+    <t>986857576</t>
+  </si>
+  <si>
+    <t>986858892</t>
+  </si>
+  <si>
+    <t>986859819</t>
+  </si>
+  <si>
+    <t>986860733</t>
+  </si>
+  <si>
+    <t>986862113</t>
+  </si>
+  <si>
+    <t>986863149</t>
+  </si>
+  <si>
+    <t>986864078</t>
+  </si>
+  <si>
+    <t>986865006</t>
+  </si>
+  <si>
+    <t>986865945</t>
+  </si>
+  <si>
+    <t>986866879</t>
+  </si>
+  <si>
+    <t>986868128</t>
+  </si>
+  <si>
+    <t>986869535</t>
+  </si>
+  <si>
+    <t>986870482</t>
+  </si>
+  <si>
+    <t>986871449</t>
+  </si>
+  <si>
+    <t>986872473</t>
+  </si>
+  <si>
+    <t>986873699</t>
+  </si>
+  <si>
+    <t>986874649</t>
+  </si>
+  <si>
+    <t>986875934</t>
+  </si>
+  <si>
+    <t>986877852</t>
+  </si>
+  <si>
+    <t>986879849</t>
+  </si>
+  <si>
+    <t>986883192</t>
+  </si>
+  <si>
+    <t>986886851</t>
+  </si>
+  <si>
+    <t>986889031</t>
+  </si>
+  <si>
+    <t>986890472</t>
+  </si>
+  <si>
+    <t>986892053</t>
+  </si>
+  <si>
+    <t>986894690</t>
+  </si>
+  <si>
+    <t>986896784</t>
+  </si>
+  <si>
+    <t>986899122</t>
+  </si>
+  <si>
+    <t>986901899</t>
+  </si>
+  <si>
+    <t>986903363</t>
+  </si>
+  <si>
+    <t>986905499</t>
+  </si>
+  <si>
+    <t>986907984</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1368,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1195,7 +1426,9 @@
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>180</v>
+      </c>
       <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1445,7 +1678,9 @@
       <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="C9" s="9" t="s">
         <v>37</v>
       </c>
@@ -1478,7 +1713,9 @@
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="C10" s="9" t="s">
         <v>40</v>
       </c>
@@ -1511,7 +1748,9 @@
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>183</v>
+      </c>
       <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
@@ -1544,7 +1783,9 @@
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="C12" s="9" t="s">
         <v>46</v>
       </c>
@@ -1577,7 +1818,9 @@
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="C13" s="9" t="s">
         <v>49</v>
       </c>
@@ -1610,7 +1853,9 @@
       <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>186</v>
+      </c>
       <c r="C14" s="9"/>
       <c r="D14" s="4" t="s">
         <v>13</v>
@@ -1641,7 +1886,9 @@
       <c r="A15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="C15" s="9"/>
       <c r="D15" s="4" t="s">
         <v>13</v>
@@ -1672,7 +1919,9 @@
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>188</v>
+      </c>
       <c r="C16" s="9" t="s">
         <v>55</v>
       </c>
@@ -1705,7 +1954,9 @@
       <c r="A17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="C17" s="9" t="n">
         <v>123456</v>
       </c>
@@ -1738,7 +1989,9 @@
       <c r="A18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="C18" s="9" t="s">
         <v>60</v>
       </c>
@@ -1771,7 +2024,9 @@
       <c r="A19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="C19" s="9" t="s">
         <v>63</v>
       </c>
@@ -1804,7 +2059,9 @@
       <c r="A20" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>192</v>
+      </c>
       <c r="C20" s="9" t="s">
         <v>66</v>
       </c>
@@ -1837,7 +2094,9 @@
       <c r="A21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>69</v>
       </c>
@@ -1870,7 +2129,9 @@
       <c r="A22" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>194</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>69</v>
       </c>
@@ -1903,7 +2164,9 @@
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>69</v>
       </c>
@@ -1936,7 +2199,9 @@
       <c r="A24" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>69</v>
       </c>
@@ -1969,7 +2234,9 @@
       <c r="A25" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>69</v>
       </c>
@@ -2002,7 +2269,9 @@
       <c r="A26" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>69</v>
       </c>
@@ -2033,7 +2302,9 @@
       <c r="A27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>199</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>69</v>
       </c>
@@ -2064,7 +2335,9 @@
       <c r="A28" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>69</v>
       </c>
@@ -2097,7 +2370,9 @@
       <c r="A29" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>201</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>69</v>
       </c>
@@ -2130,7 +2405,9 @@
       <c r="A30" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>202</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>69</v>
       </c>
@@ -2163,7 +2440,9 @@
       <c r="A31" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>203</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>69</v>
       </c>
@@ -2196,7 +2475,9 @@
       <c r="A32" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>204</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>69</v>
       </c>
@@ -2229,7 +2510,9 @@
       <c r="A33" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>205</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>12</v>
       </c>
@@ -2262,7 +2545,9 @@
       <c r="A34" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>206</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>12</v>
       </c>
@@ -2293,7 +2578,9 @@
       <c r="A35" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>207</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>12</v>
       </c>
@@ -2326,7 +2613,9 @@
       <c r="A36" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="C36" s="4" t="s">
         <v>12</v>
       </c>
@@ -2359,7 +2648,9 @@
       <c r="A37" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>209</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>12</v>
       </c>
@@ -2392,7 +2683,9 @@
       <c r="A38" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>210</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>69</v>
       </c>
@@ -2425,7 +2718,9 @@
       <c r="A39" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>69</v>
       </c>
@@ -2458,7 +2753,9 @@
       <c r="A40" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4" t="s">
+        <v>212</v>
+      </c>
       <c r="C40" s="4" t="s">
         <v>69</v>
       </c>
@@ -2491,7 +2788,9 @@
       <c r="A41" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>213</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>69</v>
       </c>
@@ -2524,7 +2823,9 @@
       <c r="A42" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>69</v>
       </c>
@@ -2555,7 +2856,9 @@
       <c r="A43" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="C43" s="4" t="s">
         <v>69</v>
       </c>
@@ -2586,7 +2889,9 @@
       <c r="A44" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>216</v>
+      </c>
       <c r="C44" s="4" t="s">
         <v>69</v>
       </c>
@@ -2619,7 +2924,9 @@
       <c r="A45" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B45" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="C45" s="4" t="s">
         <v>69</v>
       </c>
@@ -2652,7 +2959,9 @@
       <c r="A46" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>218</v>
+      </c>
       <c r="C46" s="4" t="s">
         <v>69</v>
       </c>
@@ -2685,7 +2994,9 @@
       <c r="A47" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="C47" s="4" t="s">
         <v>69</v>
       </c>
@@ -2718,7 +3029,9 @@
       <c r="A48" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="B48" s="22"/>
+      <c r="B48" s="22" t="s">
+        <v>220</v>
+      </c>
       <c r="C48" s="4" t="s">
         <v>69</v>
       </c>
@@ -2751,7 +3064,9 @@
       <c r="A49" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="22"/>
+      <c r="B49" s="22" t="s">
+        <v>221</v>
+      </c>
       <c r="C49" s="4" t="s">
         <v>69</v>
       </c>
@@ -2784,7 +3099,9 @@
       <c r="A50" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="B50" s="22"/>
+      <c r="B50" s="22" t="s">
+        <v>223</v>
+      </c>
       <c r="C50" s="4" t="s">
         <v>69</v>
       </c>
@@ -2817,7 +3134,9 @@
       <c r="A51" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="22"/>
+      <c r="B51" s="22" t="s">
+        <v>224</v>
+      </c>
       <c r="C51" s="4" t="s">
         <v>69</v>
       </c>
@@ -2850,7 +3169,9 @@
       <c r="A52" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="B52" s="22"/>
+      <c r="B52" s="22" t="s">
+        <v>225</v>
+      </c>
       <c r="C52" s="4" t="s">
         <v>69</v>
       </c>
@@ -2883,7 +3204,9 @@
       <c r="A53" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B53" s="22"/>
+      <c r="B53" s="22" t="s">
+        <v>222</v>
+      </c>
       <c r="C53" s="4" t="s">
         <v>69</v>
       </c>
@@ -2916,7 +3239,9 @@
       <c r="A54" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="22"/>
+      <c r="B54" s="22" t="s">
+        <v>226</v>
+      </c>
       <c r="C54" s="4" t="s">
         <v>69</v>
       </c>
@@ -2949,7 +3274,9 @@
       <c r="A55" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B55" s="22"/>
+      <c r="B55" s="22" t="s">
+        <v>227</v>
+      </c>
       <c r="C55" s="4" t="s">
         <v>69</v>
       </c>
@@ -2982,7 +3309,9 @@
       <c r="A56" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B56" s="22"/>
+      <c r="B56" s="22" t="s">
+        <v>228</v>
+      </c>
       <c r="C56" s="4" t="s">
         <v>69</v>
       </c>
@@ -3015,7 +3344,9 @@
       <c r="A57" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="22"/>
+      <c r="B57" s="22" t="s">
+        <v>229</v>
+      </c>
       <c r="C57" s="4" t="s">
         <v>69</v>
       </c>
@@ -3048,7 +3379,9 @@
       <c r="A58" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="B58" s="22"/>
+      <c r="B58" s="22" t="s">
+        <v>230</v>
+      </c>
       <c r="C58" s="4" t="s">
         <v>69</v>
       </c>
@@ -3079,7 +3412,9 @@
       <c r="A59" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B59" s="22"/>
+      <c r="B59" s="22" t="s">
+        <v>231</v>
+      </c>
       <c r="C59" s="4" t="s">
         <v>69</v>
       </c>
@@ -3113,7 +3448,7 @@
         <v>160</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>69</v>
@@ -3136,23 +3471,21 @@
       <c r="I60" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="J60" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="K60" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="J60" s="25"/>
+      <c r="K60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B61" s="22"/>
+      <c r="B61" s="22" t="s">
+        <v>239</v>
+      </c>
       <c r="C61" s="4" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>14</v>
@@ -3164,21 +3497,25 @@
         <v>46022</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>163</v>
+        <v>17</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="J61" s="25"/>
+        <v>158</v>
+      </c>
+      <c r="J61" s="25" t="s">
+        <v>159</v>
+      </c>
       <c r="K61" s="7" t="s">
-        <v>165</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="B62" s="22"/>
+      <c r="A62" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>240</v>
+      </c>
       <c r="C62" s="4" t="s">
         <v>69</v>
       </c>
@@ -3200,26 +3537,24 @@
       <c r="I62" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="J62" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="K62" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="J62" s="25"/>
+      <c r="K62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B63" s="22"/>
+        <v>163</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>241</v>
+      </c>
       <c r="C63" s="4" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="F63" s="24" t="n">
         <v>46019</v>
@@ -3228,21 +3563,369 @@
         <v>46022</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>163</v>
+        <v>17</v>
       </c>
       <c r="I63" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J63" s="25"/>
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J63" s="25"/>
-      <c r="K63" s="7" t="s">
+      <c r="B64" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G64" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J64" s="25"/>
+      <c r="K64" s="7"/>
+    </row>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="8" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B65" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G65" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J65" s="25"/>
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G66" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J66" s="25"/>
+      <c r="K66" s="7"/>
+    </row>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G67" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J67" s="25"/>
+      <c r="K67" s="7"/>
+    </row>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G68" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J68" s="25"/>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G69" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J69" s="25"/>
+      <c r="K69" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G70" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="J70" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="K70" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F71" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G71" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J71" s="25"/>
+      <c r="K71" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F72" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G72" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J72" s="25"/>
+      <c r="K72" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F73" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G73" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J73" s="25"/>
+      <c r="K73" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F74" s="24" t="n">
+        <v>46019</v>
+      </c>
+      <c r="G74" s="24" t="n">
+        <v>46022</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J74" s="25"/>
+      <c r="K74" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E52" r:id="rId1" display="!@AS12"/>

</xml_diff>

<commit_message>
refactor - Code complexity feedback have been done for create method
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="402">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -860,6 +860,453 @@
   </si>
   <si>
     <t>993541096</t>
+  </si>
+  <si>
+    <t>123520366</t>
+  </si>
+  <si>
+    <t>123584949</t>
+  </si>
+  <si>
+    <t>125603202</t>
+  </si>
+  <si>
+    <t>126123779</t>
+  </si>
+  <si>
+    <t>126217023</t>
+  </si>
+  <si>
+    <t>126994473</t>
+  </si>
+  <si>
+    <t>127037447</t>
+  </si>
+  <si>
+    <t>127180521</t>
+  </si>
+  <si>
+    <t>128400910</t>
+  </si>
+  <si>
+    <t>128787382</t>
+  </si>
+  <si>
+    <t>128808585</t>
+  </si>
+  <si>
+    <t>129005604</t>
+  </si>
+  <si>
+    <t>129364320</t>
+  </si>
+  <si>
+    <t>130215758</t>
+  </si>
+  <si>
+    <t>130277886</t>
+  </si>
+  <si>
+    <t>130897737</t>
+  </si>
+  <si>
+    <t>130918492</t>
+  </si>
+  <si>
+    <t>130964391</t>
+  </si>
+  <si>
+    <t>130966377</t>
+  </si>
+  <si>
+    <t>131234640</t>
+  </si>
+  <si>
+    <t>131237156</t>
+  </si>
+  <si>
+    <t>131455511</t>
+  </si>
+  <si>
+    <t>131458093</t>
+  </si>
+  <si>
+    <t>131625124</t>
+  </si>
+  <si>
+    <t>131627917</t>
+  </si>
+  <si>
+    <t>131773737</t>
+  </si>
+  <si>
+    <t>131783183</t>
+  </si>
+  <si>
+    <t>131784020</t>
+  </si>
+  <si>
+    <t>131784756</t>
+  </si>
+  <si>
+    <t>131786021</t>
+  </si>
+  <si>
+    <t>131786997</t>
+  </si>
+  <si>
+    <t>131788269</t>
+  </si>
+  <si>
+    <t>131789243</t>
+  </si>
+  <si>
+    <t>131790552</t>
+  </si>
+  <si>
+    <t>131791369</t>
+  </si>
+  <si>
+    <t>131792782</t>
+  </si>
+  <si>
+    <t>131793594</t>
+  </si>
+  <si>
+    <t>131794724</t>
+  </si>
+  <si>
+    <t>131795587</t>
+  </si>
+  <si>
+    <t>131796457</t>
+  </si>
+  <si>
+    <t>131797354</t>
+  </si>
+  <si>
+    <t>131798569</t>
+  </si>
+  <si>
+    <t>131799420</t>
+  </si>
+  <si>
+    <t>131800314</t>
+  </si>
+  <si>
+    <t>131801186</t>
+  </si>
+  <si>
+    <t>131802448</t>
+  </si>
+  <si>
+    <t>131803328</t>
+  </si>
+  <si>
+    <t>131804183</t>
+  </si>
+  <si>
+    <t>131805091</t>
+  </si>
+  <si>
+    <t>131805999</t>
+  </si>
+  <si>
+    <t>131806871</t>
+  </si>
+  <si>
+    <t>131807806</t>
+  </si>
+  <si>
+    <t>131808703</t>
+  </si>
+  <si>
+    <t>131810179</t>
+  </si>
+  <si>
+    <t>131811089</t>
+  </si>
+  <si>
+    <t>131812740</t>
+  </si>
+  <si>
+    <t>131813711</t>
+  </si>
+  <si>
+    <t>131814638</t>
+  </si>
+  <si>
+    <t>131815593</t>
+  </si>
+  <si>
+    <t>131816549</t>
+  </si>
+  <si>
+    <t>131817883</t>
+  </si>
+  <si>
+    <t>131819483</t>
+  </si>
+  <si>
+    <t>131820478</t>
+  </si>
+  <si>
+    <t>131821419</t>
+  </si>
+  <si>
+    <t>131822736</t>
+  </si>
+  <si>
+    <t>131823793</t>
+  </si>
+  <si>
+    <t>131824767</t>
+  </si>
+  <si>
+    <t>131826290</t>
+  </si>
+  <si>
+    <t>131827457</t>
+  </si>
+  <si>
+    <t>131828824</t>
+  </si>
+  <si>
+    <t>131830096</t>
+  </si>
+  <si>
+    <t>131831160</t>
+  </si>
+  <si>
+    <t>131832193</t>
+  </si>
+  <si>
+    <t>131833276</t>
+  </si>
+  <si>
+    <t>131834638</t>
+  </si>
+  <si>
+    <t>131836227</t>
+  </si>
+  <si>
+    <t>131837454</t>
+  </si>
+  <si>
+    <t>131839124</t>
+  </si>
+  <si>
+    <t>131841303</t>
+  </si>
+  <si>
+    <t>135227283</t>
+  </si>
+  <si>
+    <t>135233922</t>
+  </si>
+  <si>
+    <t>135234813</t>
+  </si>
+  <si>
+    <t>135235529</t>
+  </si>
+  <si>
+    <t>135236586</t>
+  </si>
+  <si>
+    <t>135237682</t>
+  </si>
+  <si>
+    <t>135238991</t>
+  </si>
+  <si>
+    <t>135239782</t>
+  </si>
+  <si>
+    <t>135240579</t>
+  </si>
+  <si>
+    <t>135241876</t>
+  </si>
+  <si>
+    <t>135242777</t>
+  </si>
+  <si>
+    <t>135243635</t>
+  </si>
+  <si>
+    <t>135244516</t>
+  </si>
+  <si>
+    <t>135245687</t>
+  </si>
+  <si>
+    <t>135246537</t>
+  </si>
+  <si>
+    <t>135247676</t>
+  </si>
+  <si>
+    <t>135249272</t>
+  </si>
+  <si>
+    <t>135250107</t>
+  </si>
+  <si>
+    <t>135251274</t>
+  </si>
+  <si>
+    <t>135252142</t>
+  </si>
+  <si>
+    <t>135253051</t>
+  </si>
+  <si>
+    <t>135254413</t>
+  </si>
+  <si>
+    <t>135255344</t>
+  </si>
+  <si>
+    <t>135256237</t>
+  </si>
+  <si>
+    <t>135257121</t>
+  </si>
+  <si>
+    <t>135258058</t>
+  </si>
+  <si>
+    <t>135258970</t>
+  </si>
+  <si>
+    <t>135259854</t>
+  </si>
+  <si>
+    <t>135261182</t>
+  </si>
+  <si>
+    <t>135262135</t>
+  </si>
+  <si>
+    <t>135263459</t>
+  </si>
+  <si>
+    <t>135264778</t>
+  </si>
+  <si>
+    <t>135265726</t>
+  </si>
+  <si>
+    <t>135266672</t>
+  </si>
+  <si>
+    <t>135267878</t>
+  </si>
+  <si>
+    <t>135268863</t>
+  </si>
+  <si>
+    <t>135270320</t>
+  </si>
+  <si>
+    <t>135271508</t>
+  </si>
+  <si>
+    <t>135272485</t>
+  </si>
+  <si>
+    <t>135273742</t>
+  </si>
+  <si>
+    <t>135274796</t>
+  </si>
+  <si>
+    <t>135275834</t>
+  </si>
+  <si>
+    <t>135276902</t>
+  </si>
+  <si>
+    <t>135277942</t>
+  </si>
+  <si>
+    <t>135279211</t>
+  </si>
+  <si>
+    <t>135280290</t>
+  </si>
+  <si>
+    <t>135281352</t>
+  </si>
+  <si>
+    <t>135282756</t>
+  </si>
+  <si>
+    <t>135284005</t>
+  </si>
+  <si>
+    <t>135285109</t>
+  </si>
+  <si>
+    <t>135286633</t>
+  </si>
+  <si>
+    <t>135287719</t>
+  </si>
+  <si>
+    <t>135289199</t>
+  </si>
+  <si>
+    <t>135291154</t>
+  </si>
+  <si>
+    <t>135292956</t>
+  </si>
+  <si>
+    <t>135296970</t>
+  </si>
+  <si>
+    <t>135300821</t>
+  </si>
+  <si>
+    <t>135303727</t>
+  </si>
+  <si>
+    <t>135305006</t>
+  </si>
+  <si>
+    <t>135308093</t>
+  </si>
+  <si>
+    <t>135309839</t>
+  </si>
+  <si>
+    <t>135311114</t>
+  </si>
+  <si>
+    <t>135312849</t>
+  </si>
+  <si>
+    <t>135315348</t>
+  </si>
+  <si>
+    <t>135317647</t>
+  </si>
+  <si>
+    <t>135320828</t>
+  </si>
+  <si>
+    <t>135323641</t>
+  </si>
+  <si>
+    <t>135326620</t>
+  </si>
+  <si>
+    <t>135328886</t>
+  </si>
+  <si>
+    <t>135331458</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1938,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>184</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,7 +2178,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>185</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +2214,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>186</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,7 +2250,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>187</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +2286,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>188</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1875,7 +2322,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>189</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,7 +2356,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>190</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1943,7 +2390,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>191</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,7 +2426,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>192</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,7 +2462,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>193</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,7 +2498,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>194</v>
+        <v>342</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,7 +2534,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>195</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,7 +2570,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>196</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2159,7 +2606,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>197</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2195,7 +2642,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>198</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,7 +2678,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>199</v>
+        <v>347</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,7 +2714,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>200</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2303,7 +2750,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>201</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2337,7 +2784,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>202</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,7 +2818,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>203</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,7 +2854,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>204</v>
+        <v>352</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,7 +2890,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>205</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2479,7 +2926,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>206</v>
+        <v>354</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2515,7 +2962,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>207</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2551,7 +2998,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>208</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,7 +3034,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>209</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2621,7 +3068,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>210</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2657,7 +3104,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>211</v>
+        <v>359</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2693,7 +3140,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>212</v>
+        <v>360</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2729,7 +3176,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>213</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2765,7 +3212,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>214</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2801,7 +3248,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>215</v>
+        <v>363</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2837,7 +3284,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>216</v>
+        <v>364</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,7 +3320,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>217</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2907,7 +3354,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>218</v>
+        <v>366</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2941,7 +3388,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>219</v>
+        <v>367</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2977,7 +3424,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>220</v>
+        <v>368</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,7 +3460,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>221</v>
+        <v>369</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,7 +3496,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>222</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3085,7 +3532,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>223</v>
+        <v>371</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3121,7 +3568,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>224</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3157,7 +3604,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>225</v>
+        <v>373</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3193,7 +3640,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>227</v>
+        <v>375</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3229,7 +3676,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>228</v>
+        <v>376</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3265,7 +3712,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>229</v>
+        <v>377</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3301,7 +3748,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>226</v>
+        <v>374</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3337,7 +3784,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>230</v>
+        <v>378</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3373,7 +3820,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>231</v>
+        <v>379</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3409,7 +3856,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>232</v>
+        <v>380</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3445,7 +3892,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>233</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3479,7 +3926,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>234</v>
+        <v>382</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3515,7 +3962,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>235</v>
+        <v>383</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3547,7 +3994,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>236</v>
+        <v>384</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3583,7 +4030,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>245</v>
+        <v>394</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3615,7 +4062,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>246</v>
+        <v>395</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3647,7 +4094,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>247</v>
+        <v>396</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3679,7 +4126,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>248</v>
+        <v>397</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3711,7 +4158,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>249</v>
+        <v>398</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3743,7 +4190,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>250</v>
+        <v>399</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3775,7 +4222,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>251</v>
+        <v>400</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3807,7 +4254,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>252</v>
+        <v>401</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3841,7 +4288,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>237</v>
+        <v>385</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3877,7 +4324,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>241</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3910,7 +4357,9 @@
       <c r="K71" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="L71" s="8"/>
+      <c r="L71" s="8" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="13" t="s">
@@ -3943,7 +4392,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>238</v>
+        <v>386</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3977,7 +4426,7 @@
         <v>171</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>239</v>
+        <v>387</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4011,7 +4460,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>240</v>
+        <v>388</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4043,7 +4492,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>242</v>
+        <v>391</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4075,7 +4524,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>243</v>
+        <v>392</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4107,7 +4556,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>244</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor -Separate stepdifinition created for E2EBooking Scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="472">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -1307,6 +1307,216 @@
   </si>
   <si>
     <t>135331458</t>
+  </si>
+  <si>
+    <t>145623992</t>
+  </si>
+  <si>
+    <t>145667377</t>
+  </si>
+  <si>
+    <t>145668886</t>
+  </si>
+  <si>
+    <t>145669683</t>
+  </si>
+  <si>
+    <t>145671046</t>
+  </si>
+  <si>
+    <t>145671834</t>
+  </si>
+  <si>
+    <t>145673290</t>
+  </si>
+  <si>
+    <t>145674099</t>
+  </si>
+  <si>
+    <t>145675553</t>
+  </si>
+  <si>
+    <t>145676335</t>
+  </si>
+  <si>
+    <t>145677249</t>
+  </si>
+  <si>
+    <t>145678447</t>
+  </si>
+  <si>
+    <t>145679304</t>
+  </si>
+  <si>
+    <t>145680158</t>
+  </si>
+  <si>
+    <t>145681042</t>
+  </si>
+  <si>
+    <t>145681920</t>
+  </si>
+  <si>
+    <t>145683322</t>
+  </si>
+  <si>
+    <t>145684596</t>
+  </si>
+  <si>
+    <t>145685891</t>
+  </si>
+  <si>
+    <t>145686765</t>
+  </si>
+  <si>
+    <t>145687612</t>
+  </si>
+  <si>
+    <t>145688794</t>
+  </si>
+  <si>
+    <t>145690093</t>
+  </si>
+  <si>
+    <t>145690987</t>
+  </si>
+  <si>
+    <t>145691900</t>
+  </si>
+  <si>
+    <t>145692843</t>
+  </si>
+  <si>
+    <t>145694239</t>
+  </si>
+  <si>
+    <t>145695151</t>
+  </si>
+  <si>
+    <t>145696482</t>
+  </si>
+  <si>
+    <t>145697425</t>
+  </si>
+  <si>
+    <t>145698751</t>
+  </si>
+  <si>
+    <t>145699804</t>
+  </si>
+  <si>
+    <t>145700806</t>
+  </si>
+  <si>
+    <t>145701839</t>
+  </si>
+  <si>
+    <t>145702994</t>
+  </si>
+  <si>
+    <t>145704207</t>
+  </si>
+  <si>
+    <t>145705500</t>
+  </si>
+  <si>
+    <t>145706528</t>
+  </si>
+  <si>
+    <t>145707532</t>
+  </si>
+  <si>
+    <t>145708809</t>
+  </si>
+  <si>
+    <t>145710013</t>
+  </si>
+  <si>
+    <t>145711064</t>
+  </si>
+  <si>
+    <t>145712186</t>
+  </si>
+  <si>
+    <t>145713265</t>
+  </si>
+  <si>
+    <t>145714355</t>
+  </si>
+  <si>
+    <t>145715788</t>
+  </si>
+  <si>
+    <t>145717097</t>
+  </si>
+  <si>
+    <t>145718197</t>
+  </si>
+  <si>
+    <t>145719284</t>
+  </si>
+  <si>
+    <t>145720623</t>
+  </si>
+  <si>
+    <t>145722214</t>
+  </si>
+  <si>
+    <t>145723298</t>
+  </si>
+  <si>
+    <t>145724227</t>
+  </si>
+  <si>
+    <t>145726625</t>
+  </si>
+  <si>
+    <t>145728795</t>
+  </si>
+  <si>
+    <t>145732411</t>
+  </si>
+  <si>
+    <t>145736394</t>
+  </si>
+  <si>
+    <t>145739303</t>
+  </si>
+  <si>
+    <t>145740556</t>
+  </si>
+  <si>
+    <t>145741768</t>
+  </si>
+  <si>
+    <t>145743112</t>
+  </si>
+  <si>
+    <t>145744426</t>
+  </si>
+  <si>
+    <t>145746260</t>
+  </si>
+  <si>
+    <t>145748824</t>
+  </si>
+  <si>
+    <t>145751400</t>
+  </si>
+  <si>
+    <t>145754287</t>
+  </si>
+  <si>
+    <t>145757051</t>
+  </si>
+  <si>
+    <t>145760313</t>
+  </si>
+  <si>
+    <t>145762803</t>
+  </si>
+  <si>
+    <t>145765720</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +2148,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>332</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,7 +2388,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>333</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,7 +2424,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>334</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,7 +2460,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>335</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,7 +2496,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>336</v>
+        <v>406</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2532,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>337</v>
+        <v>407</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,7 +2566,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>338</v>
+        <v>408</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,7 +2600,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>339</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,7 +2636,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>340</v>
+        <v>410</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,7 +2672,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>341</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,7 +2708,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>342</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2534,7 +2744,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>343</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,7 +2780,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>344</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,7 +2816,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>345</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2642,7 +2852,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>346</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2678,7 +2888,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>347</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,7 +2924,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>348</v>
+        <v>418</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,7 +2960,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>349</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,7 +2994,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>350</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,7 +3028,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>351</v>
+        <v>421</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,7 +3064,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>352</v>
+        <v>422</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2890,7 +3100,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>353</v>
+        <v>423</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,7 +3136,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>354</v>
+        <v>424</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +3172,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>355</v>
+        <v>425</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2998,7 +3208,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>356</v>
+        <v>426</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3034,7 +3244,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>357</v>
+        <v>427</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,7 +3278,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>358</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3104,7 +3314,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>359</v>
+        <v>429</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3140,7 +3350,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>360</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3176,7 +3386,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>361</v>
+        <v>431</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3212,7 +3422,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>362</v>
+        <v>432</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3248,7 +3458,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>363</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3284,7 +3494,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>364</v>
+        <v>434</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3320,7 +3530,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>365</v>
+        <v>435</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,7 +3564,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>366</v>
+        <v>436</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3388,7 +3598,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>367</v>
+        <v>437</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3424,7 +3634,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>368</v>
+        <v>438</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3460,7 +3670,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>369</v>
+        <v>439</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3496,7 +3706,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>370</v>
+        <v>440</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3532,7 +3742,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>371</v>
+        <v>441</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3568,7 +3778,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>372</v>
+        <v>442</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3604,7 +3814,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>373</v>
+        <v>443</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3640,7 +3850,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>375</v>
+        <v>445</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3676,7 +3886,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>376</v>
+        <v>446</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3712,7 +3922,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>377</v>
+        <v>447</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3748,7 +3958,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>374</v>
+        <v>444</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,7 +3994,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>378</v>
+        <v>448</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,7 +4030,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>379</v>
+        <v>449</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3856,7 +4066,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>380</v>
+        <v>450</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3892,7 +4102,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>381</v>
+        <v>451</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,7 +4136,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>382</v>
+        <v>452</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3962,7 +4172,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>383</v>
+        <v>453</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3994,7 +4204,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>384</v>
+        <v>454</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4030,7 +4240,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>394</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4062,7 +4272,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>395</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4094,7 +4304,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>396</v>
+        <v>466</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4126,7 +4336,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>397</v>
+        <v>467</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4158,7 +4368,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>398</v>
+        <v>468</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4190,7 +4400,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>399</v>
+        <v>469</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4222,7 +4432,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>400</v>
+        <v>470</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4254,7 +4464,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>401</v>
+        <v>471</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4288,7 +4498,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>385</v>
+        <v>455</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4324,7 +4534,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>389</v>
+        <v>459</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4358,7 +4568,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>390</v>
+        <v>460</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4392,7 +4602,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>386</v>
+        <v>456</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4426,7 +4636,7 @@
         <v>171</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>387</v>
+        <v>457</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4460,7 +4670,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>388</v>
+        <v>458</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4492,7 +4702,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>391</v>
+        <v>461</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4524,7 +4734,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>392</v>
+        <v>462</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4556,7 +4766,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>393</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor – cyclomatic complexity discovered
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="682">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -1517,6 +1517,636 @@
   </si>
   <si>
     <t>145765720</t>
+  </si>
+  <si>
+    <t>173195877</t>
+  </si>
+  <si>
+    <t>173239118</t>
+  </si>
+  <si>
+    <t>173240778</t>
+  </si>
+  <si>
+    <t>173241563</t>
+  </si>
+  <si>
+    <t>173242690</t>
+  </si>
+  <si>
+    <t>173243482</t>
+  </si>
+  <si>
+    <t>173244254</t>
+  </si>
+  <si>
+    <t>173245285</t>
+  </si>
+  <si>
+    <t>173246352</t>
+  </si>
+  <si>
+    <t>173247150</t>
+  </si>
+  <si>
+    <t>173248047</t>
+  </si>
+  <si>
+    <t>173248920</t>
+  </si>
+  <si>
+    <t>173250104</t>
+  </si>
+  <si>
+    <t>173251011</t>
+  </si>
+  <si>
+    <t>173251951</t>
+  </si>
+  <si>
+    <t>173252855</t>
+  </si>
+  <si>
+    <t>173254362</t>
+  </si>
+  <si>
+    <t>173255570</t>
+  </si>
+  <si>
+    <t>173256876</t>
+  </si>
+  <si>
+    <t>173257747</t>
+  </si>
+  <si>
+    <t>173259109</t>
+  </si>
+  <si>
+    <t>173260068</t>
+  </si>
+  <si>
+    <t>173261286</t>
+  </si>
+  <si>
+    <t>173262202</t>
+  </si>
+  <si>
+    <t>173263148</t>
+  </si>
+  <si>
+    <t>173264109</t>
+  </si>
+  <si>
+    <t>173265069</t>
+  </si>
+  <si>
+    <t>173266056</t>
+  </si>
+  <si>
+    <t>173267505</t>
+  </si>
+  <si>
+    <t>173268527</t>
+  </si>
+  <si>
+    <t>173269769</t>
+  </si>
+  <si>
+    <t>173271081</t>
+  </si>
+  <si>
+    <t>173272356</t>
+  </si>
+  <si>
+    <t>173273329</t>
+  </si>
+  <si>
+    <t>173274342</t>
+  </si>
+  <si>
+    <t>173275354</t>
+  </si>
+  <si>
+    <t>173276835</t>
+  </si>
+  <si>
+    <t>173277916</t>
+  </si>
+  <si>
+    <t>173278911</t>
+  </si>
+  <si>
+    <t>173280174</t>
+  </si>
+  <si>
+    <t>173281429</t>
+  </si>
+  <si>
+    <t>173282488</t>
+  </si>
+  <si>
+    <t>173283553</t>
+  </si>
+  <si>
+    <t>173284603</t>
+  </si>
+  <si>
+    <t>173285683</t>
+  </si>
+  <si>
+    <t>173287139</t>
+  </si>
+  <si>
+    <t>173288230</t>
+  </si>
+  <si>
+    <t>173289732</t>
+  </si>
+  <si>
+    <t>173290848</t>
+  </si>
+  <si>
+    <t>173291941</t>
+  </si>
+  <si>
+    <t>173293588</t>
+  </si>
+  <si>
+    <t>173294765</t>
+  </si>
+  <si>
+    <t>173296486</t>
+  </si>
+  <si>
+    <t>173298782</t>
+  </si>
+  <si>
+    <t>173300968</t>
+  </si>
+  <si>
+    <t>173304885</t>
+  </si>
+  <si>
+    <t>173308617</t>
+  </si>
+  <si>
+    <t>173310905</t>
+  </si>
+  <si>
+    <t>173312155</t>
+  </si>
+  <si>
+    <t>173313529</t>
+  </si>
+  <si>
+    <t>173315194</t>
+  </si>
+  <si>
+    <t>173316514</t>
+  </si>
+  <si>
+    <t>173318300</t>
+  </si>
+  <si>
+    <t>173320974</t>
+  </si>
+  <si>
+    <t>173323206</t>
+  </si>
+  <si>
+    <t>173325856</t>
+  </si>
+  <si>
+    <t>173327590</t>
+  </si>
+  <si>
+    <t>173330369</t>
+  </si>
+  <si>
+    <t>173332943</t>
+  </si>
+  <si>
+    <t>173335267</t>
+  </si>
+  <si>
+    <t>173439740</t>
+  </si>
+  <si>
+    <t>173447188</t>
+  </si>
+  <si>
+    <t>173448024</t>
+  </si>
+  <si>
+    <t>173448759</t>
+  </si>
+  <si>
+    <t>173450041</t>
+  </si>
+  <si>
+    <t>173450796</t>
+  </si>
+  <si>
+    <t>173451634</t>
+  </si>
+  <si>
+    <t>173452579</t>
+  </si>
+  <si>
+    <t>173453912</t>
+  </si>
+  <si>
+    <t>173454731</t>
+  </si>
+  <si>
+    <t>173456185</t>
+  </si>
+  <si>
+    <t>173457511</t>
+  </si>
+  <si>
+    <t>173458367</t>
+  </si>
+  <si>
+    <t>173459237</t>
+  </si>
+  <si>
+    <t>173460253</t>
+  </si>
+  <si>
+    <t>173461119</t>
+  </si>
+  <si>
+    <t>173462301</t>
+  </si>
+  <si>
+    <t>173463163</t>
+  </si>
+  <si>
+    <t>173464061</t>
+  </si>
+  <si>
+    <t>173465216</t>
+  </si>
+  <si>
+    <t>173466490</t>
+  </si>
+  <si>
+    <t>173467538</t>
+  </si>
+  <si>
+    <t>173468774</t>
+  </si>
+  <si>
+    <t>173469697</t>
+  </si>
+  <si>
+    <t>173470659</t>
+  </si>
+  <si>
+    <t>173471605</t>
+  </si>
+  <si>
+    <t>173472714</t>
+  </si>
+  <si>
+    <t>173473679</t>
+  </si>
+  <si>
+    <t>173475203</t>
+  </si>
+  <si>
+    <t>173476159</t>
+  </si>
+  <si>
+    <t>173477492</t>
+  </si>
+  <si>
+    <t>173478477</t>
+  </si>
+  <si>
+    <t>173479466</t>
+  </si>
+  <si>
+    <t>173480434</t>
+  </si>
+  <si>
+    <t>173481444</t>
+  </si>
+  <si>
+    <t>173482603</t>
+  </si>
+  <si>
+    <t>173483889</t>
+  </si>
+  <si>
+    <t>173484942</t>
+  </si>
+  <si>
+    <t>173485969</t>
+  </si>
+  <si>
+    <t>173487456</t>
+  </si>
+  <si>
+    <t>173488562</t>
+  </si>
+  <si>
+    <t>173489667</t>
+  </si>
+  <si>
+    <t>173490758</t>
+  </si>
+  <si>
+    <t>173491851</t>
+  </si>
+  <si>
+    <t>173492937</t>
+  </si>
+  <si>
+    <t>173494192</t>
+  </si>
+  <si>
+    <t>173495274</t>
+  </si>
+  <si>
+    <t>173496365</t>
+  </si>
+  <si>
+    <t>173497749</t>
+  </si>
+  <si>
+    <t>173499033</t>
+  </si>
+  <si>
+    <t>173500318</t>
+  </si>
+  <si>
+    <t>173501943</t>
+  </si>
+  <si>
+    <t>173503095</t>
+  </si>
+  <si>
+    <t>173505517</t>
+  </si>
+  <si>
+    <t>173507775</t>
+  </si>
+  <si>
+    <t>173511109</t>
+  </si>
+  <si>
+    <t>173514776</t>
+  </si>
+  <si>
+    <t>173517069</t>
+  </si>
+  <si>
+    <t>173518331</t>
+  </si>
+  <si>
+    <t>173519549</t>
+  </si>
+  <si>
+    <t>173521313</t>
+  </si>
+  <si>
+    <t>173522824</t>
+  </si>
+  <si>
+    <t>173524975</t>
+  </si>
+  <si>
+    <t>173527480</t>
+  </si>
+  <si>
+    <t>173529680</t>
+  </si>
+  <si>
+    <t>173532950</t>
+  </si>
+  <si>
+    <t>173535253</t>
+  </si>
+  <si>
+    <t>173538013</t>
+  </si>
+  <si>
+    <t>173540519</t>
+  </si>
+  <si>
+    <t>173542965</t>
+  </si>
+  <si>
+    <t>173663304</t>
+  </si>
+  <si>
+    <t>173673069</t>
+  </si>
+  <si>
+    <t>173674180</t>
+  </si>
+  <si>
+    <t>173675111</t>
+  </si>
+  <si>
+    <t>173676578</t>
+  </si>
+  <si>
+    <t>173677565</t>
+  </si>
+  <si>
+    <t>173679219</t>
+  </si>
+  <si>
+    <t>173680239</t>
+  </si>
+  <si>
+    <t>173681729</t>
+  </si>
+  <si>
+    <t>173682812</t>
+  </si>
+  <si>
+    <t>173684339</t>
+  </si>
+  <si>
+    <t>173685410</t>
+  </si>
+  <si>
+    <t>173686946</t>
+  </si>
+  <si>
+    <t>173688180</t>
+  </si>
+  <si>
+    <t>173689384</t>
+  </si>
+  <si>
+    <t>173690359</t>
+  </si>
+  <si>
+    <t>173691683</t>
+  </si>
+  <si>
+    <t>173692632</t>
+  </si>
+  <si>
+    <t>173693887</t>
+  </si>
+  <si>
+    <t>173694863</t>
+  </si>
+  <si>
+    <t>173696152</t>
+  </si>
+  <si>
+    <t>173697195</t>
+  </si>
+  <si>
+    <t>173698631</t>
+  </si>
+  <si>
+    <t>173699686</t>
+  </si>
+  <si>
+    <t>173700706</t>
+  </si>
+  <si>
+    <t>173701697</t>
+  </si>
+  <si>
+    <t>173702776</t>
+  </si>
+  <si>
+    <t>173704008</t>
+  </si>
+  <si>
+    <t>173705476</t>
+  </si>
+  <si>
+    <t>173706742</t>
+  </si>
+  <si>
+    <t>173708108</t>
+  </si>
+  <si>
+    <t>173709307</t>
+  </si>
+  <si>
+    <t>173710406</t>
+  </si>
+  <si>
+    <t>173711727</t>
+  </si>
+  <si>
+    <t>173713154</t>
+  </si>
+  <si>
+    <t>173714563</t>
+  </si>
+  <si>
+    <t>173716230</t>
+  </si>
+  <si>
+    <t>173717623</t>
+  </si>
+  <si>
+    <t>173719056</t>
+  </si>
+  <si>
+    <t>173720880</t>
+  </si>
+  <si>
+    <t>173722930</t>
+  </si>
+  <si>
+    <t>173724391</t>
+  </si>
+  <si>
+    <t>173725989</t>
+  </si>
+  <si>
+    <t>173727702</t>
+  </si>
+  <si>
+    <t>173729324</t>
+  </si>
+  <si>
+    <t>173731027</t>
+  </si>
+  <si>
+    <t>173732735</t>
+  </si>
+  <si>
+    <t>173734352</t>
+  </si>
+  <si>
+    <t>173736022</t>
+  </si>
+  <si>
+    <t>173737528</t>
+  </si>
+  <si>
+    <t>173739732</t>
+  </si>
+  <si>
+    <t>173741172</t>
+  </si>
+  <si>
+    <t>173743335</t>
+  </si>
+  <si>
+    <t>173746659</t>
+  </si>
+  <si>
+    <t>173749294</t>
+  </si>
+  <si>
+    <t>173753402</t>
+  </si>
+  <si>
+    <t>173757607</t>
+  </si>
+  <si>
+    <t>173760538</t>
+  </si>
+  <si>
+    <t>173762405</t>
+  </si>
+  <si>
+    <t>173764376</t>
+  </si>
+  <si>
+    <t>173766104</t>
+  </si>
+  <si>
+    <t>173768297</t>
+  </si>
+  <si>
+    <t>173770414</t>
+  </si>
+  <si>
+    <t>173773580</t>
+  </si>
+  <si>
+    <t>173776590</t>
+  </si>
+  <si>
+    <t>173779664</t>
+  </si>
+  <si>
+    <t>173782710</t>
+  </si>
+  <si>
+    <t>173785874</t>
+  </si>
+  <si>
+    <t>173789044</t>
+  </si>
+  <si>
+    <t>173791909</t>
   </si>
 </sst>
 </file>
@@ -2148,7 +2778,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>402</v>
+        <v>612</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2388,7 +3018,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>403</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2424,7 +3054,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>404</v>
+        <v>614</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,7 +3090,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>405</v>
+        <v>615</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,7 +3126,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>406</v>
+        <v>616</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,7 +3162,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>407</v>
+        <v>617</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2566,7 +3196,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>408</v>
+        <v>618</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2600,7 +3230,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>409</v>
+        <v>619</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2636,7 +3266,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>410</v>
+        <v>620</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2672,7 +3302,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>411</v>
+        <v>621</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2708,7 +3338,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>412</v>
+        <v>622</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2744,7 +3374,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>413</v>
+        <v>623</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2780,7 +3410,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>414</v>
+        <v>624</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,7 +3446,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>415</v>
+        <v>625</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,7 +3482,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>416</v>
+        <v>626</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2888,7 +3518,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>417</v>
+        <v>627</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,7 +3554,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>418</v>
+        <v>628</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2960,7 +3590,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>419</v>
+        <v>629</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2994,7 +3624,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>420</v>
+        <v>630</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,7 +3658,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>421</v>
+        <v>631</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,7 +3694,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>422</v>
+        <v>632</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3100,7 +3730,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>423</v>
+        <v>633</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3136,7 +3766,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>424</v>
+        <v>634</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3172,7 +3802,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>425</v>
+        <v>635</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3208,7 +3838,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>426</v>
+        <v>636</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,7 +3874,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>427</v>
+        <v>637</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3278,7 +3908,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>428</v>
+        <v>638</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3314,7 +3944,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>429</v>
+        <v>639</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3350,7 +3980,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>430</v>
+        <v>640</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,7 +4016,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>431</v>
+        <v>641</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3422,7 +4052,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>432</v>
+        <v>642</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,7 +4088,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>433</v>
+        <v>643</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3494,7 +4124,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>434</v>
+        <v>644</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3530,7 +4160,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>435</v>
+        <v>645</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3564,7 +4194,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>436</v>
+        <v>646</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3598,7 +4228,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>437</v>
+        <v>647</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3634,7 +4264,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>438</v>
+        <v>648</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,7 +4300,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>439</v>
+        <v>649</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3706,7 +4336,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>440</v>
+        <v>650</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3742,7 +4372,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>441</v>
+        <v>651</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3778,7 +4408,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>442</v>
+        <v>652</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,7 +4444,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>443</v>
+        <v>653</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3850,7 +4480,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>445</v>
+        <v>655</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3886,7 +4516,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>446</v>
+        <v>656</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3922,7 +4552,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>447</v>
+        <v>657</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3958,7 +4588,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>444</v>
+        <v>654</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3994,7 +4624,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>448</v>
+        <v>658</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4030,7 +4660,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>449</v>
+        <v>659</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4066,7 +4696,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>450</v>
+        <v>660</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4102,7 +4732,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>451</v>
+        <v>661</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4136,7 +4766,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>452</v>
+        <v>662</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4172,7 +4802,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>453</v>
+        <v>663</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4204,7 +4834,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>454</v>
+        <v>664</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4240,7 +4870,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>464</v>
+        <v>674</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4272,7 +4902,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>465</v>
+        <v>675</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4304,7 +4934,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>466</v>
+        <v>676</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4336,7 +4966,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>467</v>
+        <v>677</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4368,7 +4998,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>468</v>
+        <v>678</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4400,7 +5030,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>469</v>
+        <v>679</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4432,7 +5062,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>470</v>
+        <v>680</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4464,7 +5094,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>471</v>
+        <v>681</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4498,7 +5128,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>455</v>
+        <v>665</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4534,7 +5164,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>459</v>
+        <v>669</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4568,7 +5198,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>460</v>
+        <v>670</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4602,7 +5232,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>456</v>
+        <v>666</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4636,7 +5266,7 @@
         <v>171</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>457</v>
+        <v>667</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4670,7 +5300,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>458</v>
+        <v>668</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4702,7 +5332,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>461</v>
+        <v>671</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4734,7 +5364,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>462</v>
+        <v>672</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4766,7 +5396,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>463</v>
+        <v>673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor - Add GitHub Actions workflow for scheduled API tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="892">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -2147,6 +2147,636 @@
   </si>
   <si>
     <t>173791909</t>
+  </si>
+  <si>
+    <t>175647380</t>
+  </si>
+  <si>
+    <t>175691672</t>
+  </si>
+  <si>
+    <t>175693053</t>
+  </si>
+  <si>
+    <t>175693797</t>
+  </si>
+  <si>
+    <t>175694874</t>
+  </si>
+  <si>
+    <t>175695662</t>
+  </si>
+  <si>
+    <t>175696471</t>
+  </si>
+  <si>
+    <t>175697272</t>
+  </si>
+  <si>
+    <t>175698684</t>
+  </si>
+  <si>
+    <t>175699528</t>
+  </si>
+  <si>
+    <t>175700419</t>
+  </si>
+  <si>
+    <t>175701209</t>
+  </si>
+  <si>
+    <t>175702059</t>
+  </si>
+  <si>
+    <t>175703277</t>
+  </si>
+  <si>
+    <t>175704589</t>
+  </si>
+  <si>
+    <t>175705460</t>
+  </si>
+  <si>
+    <t>175706816</t>
+  </si>
+  <si>
+    <t>175708105</t>
+  </si>
+  <si>
+    <t>175709731</t>
+  </si>
+  <si>
+    <t>175711001</t>
+  </si>
+  <si>
+    <t>175712297</t>
+  </si>
+  <si>
+    <t>175713576</t>
+  </si>
+  <si>
+    <t>175714871</t>
+  </si>
+  <si>
+    <t>175716205</t>
+  </si>
+  <si>
+    <t>175717403</t>
+  </si>
+  <si>
+    <t>175718418</t>
+  </si>
+  <si>
+    <t>175719714</t>
+  </si>
+  <si>
+    <t>175720731</t>
+  </si>
+  <si>
+    <t>175722276</t>
+  </si>
+  <si>
+    <t>175723577</t>
+  </si>
+  <si>
+    <t>175724886</t>
+  </si>
+  <si>
+    <t>175725965</t>
+  </si>
+  <si>
+    <t>175727152</t>
+  </si>
+  <si>
+    <t>175728423</t>
+  </si>
+  <si>
+    <t>175729449</t>
+  </si>
+  <si>
+    <t>175730561</t>
+  </si>
+  <si>
+    <t>175731966</t>
+  </si>
+  <si>
+    <t>175733110</t>
+  </si>
+  <si>
+    <t>175734192</t>
+  </si>
+  <si>
+    <t>175735550</t>
+  </si>
+  <si>
+    <t>175736677</t>
+  </si>
+  <si>
+    <t>175737831</t>
+  </si>
+  <si>
+    <t>175739006</t>
+  </si>
+  <si>
+    <t>175740156</t>
+  </si>
+  <si>
+    <t>175741277</t>
+  </si>
+  <si>
+    <t>175742432</t>
+  </si>
+  <si>
+    <t>175743891</t>
+  </si>
+  <si>
+    <t>175745077</t>
+  </si>
+  <si>
+    <t>175746200</t>
+  </si>
+  <si>
+    <t>175747389</t>
+  </si>
+  <si>
+    <t>175748837</t>
+  </si>
+  <si>
+    <t>175750276</t>
+  </si>
+  <si>
+    <t>175751901</t>
+  </si>
+  <si>
+    <t>175754089</t>
+  </si>
+  <si>
+    <t>175756146</t>
+  </si>
+  <si>
+    <t>175759623</t>
+  </si>
+  <si>
+    <t>175762995</t>
+  </si>
+  <si>
+    <t>175765792</t>
+  </si>
+  <si>
+    <t>175767172</t>
+  </si>
+  <si>
+    <t>175768668</t>
+  </si>
+  <si>
+    <t>175770361</t>
+  </si>
+  <si>
+    <t>175771715</t>
+  </si>
+  <si>
+    <t>175774174</t>
+  </si>
+  <si>
+    <t>175776902</t>
+  </si>
+  <si>
+    <t>175779474</t>
+  </si>
+  <si>
+    <t>175782092</t>
+  </si>
+  <si>
+    <t>175784542</t>
+  </si>
+  <si>
+    <t>175787823</t>
+  </si>
+  <si>
+    <t>175790219</t>
+  </si>
+  <si>
+    <t>175792606</t>
+  </si>
+  <si>
+    <t>175893753</t>
+  </si>
+  <si>
+    <t>175901019</t>
+  </si>
+  <si>
+    <t>175901888</t>
+  </si>
+  <si>
+    <t>175902665</t>
+  </si>
+  <si>
+    <t>175903860</t>
+  </si>
+  <si>
+    <t>175904661</t>
+  </si>
+  <si>
+    <t>175905498</t>
+  </si>
+  <si>
+    <t>175906465</t>
+  </si>
+  <si>
+    <t>175907730</t>
+  </si>
+  <si>
+    <t>175908667</t>
+  </si>
+  <si>
+    <t>175910325</t>
+  </si>
+  <si>
+    <t>175911199</t>
+  </si>
+  <si>
+    <t>175912095</t>
+  </si>
+  <si>
+    <t>175912978</t>
+  </si>
+  <si>
+    <t>175913892</t>
+  </si>
+  <si>
+    <t>175915181</t>
+  </si>
+  <si>
+    <t>175916464</t>
+  </si>
+  <si>
+    <t>175917358</t>
+  </si>
+  <si>
+    <t>175918714</t>
+  </si>
+  <si>
+    <t>175919643</t>
+  </si>
+  <si>
+    <t>175920977</t>
+  </si>
+  <si>
+    <t>175921916</t>
+  </si>
+  <si>
+    <t>175923237</t>
+  </si>
+  <si>
+    <t>175924194</t>
+  </si>
+  <si>
+    <t>175925199</t>
+  </si>
+  <si>
+    <t>175926373</t>
+  </si>
+  <si>
+    <t>175927761</t>
+  </si>
+  <si>
+    <t>175928775</t>
+  </si>
+  <si>
+    <t>175930288</t>
+  </si>
+  <si>
+    <t>175931486</t>
+  </si>
+  <si>
+    <t>175932886</t>
+  </si>
+  <si>
+    <t>175933938</t>
+  </si>
+  <si>
+    <t>175934976</t>
+  </si>
+  <si>
+    <t>175936402</t>
+  </si>
+  <si>
+    <t>175937495</t>
+  </si>
+  <si>
+    <t>175938718</t>
+  </si>
+  <si>
+    <t>175940247</t>
+  </si>
+  <si>
+    <t>175941353</t>
+  </si>
+  <si>
+    <t>175942465</t>
+  </si>
+  <si>
+    <t>175943886</t>
+  </si>
+  <si>
+    <t>175945012</t>
+  </si>
+  <si>
+    <t>175946154</t>
+  </si>
+  <si>
+    <t>175947340</t>
+  </si>
+  <si>
+    <t>175948496</t>
+  </si>
+  <si>
+    <t>175949966</t>
+  </si>
+  <si>
+    <t>175951120</t>
+  </si>
+  <si>
+    <t>175952316</t>
+  </si>
+  <si>
+    <t>175953867</t>
+  </si>
+  <si>
+    <t>175955098</t>
+  </si>
+  <si>
+    <t>175956419</t>
+  </si>
+  <si>
+    <t>175958058</t>
+  </si>
+  <si>
+    <t>175959312</t>
+  </si>
+  <si>
+    <t>175961248</t>
+  </si>
+  <si>
+    <t>175963747</t>
+  </si>
+  <si>
+    <t>175966103</t>
+  </si>
+  <si>
+    <t>175970399</t>
+  </si>
+  <si>
+    <t>175974530</t>
+  </si>
+  <si>
+    <t>175977528</t>
+  </si>
+  <si>
+    <t>175979564</t>
+  </si>
+  <si>
+    <t>175981277</t>
+  </si>
+  <si>
+    <t>175983078</t>
+  </si>
+  <si>
+    <t>175984983</t>
+  </si>
+  <si>
+    <t>175987466</t>
+  </si>
+  <si>
+    <t>175990277</t>
+  </si>
+  <si>
+    <t>175993028</t>
+  </si>
+  <si>
+    <t>175996207</t>
+  </si>
+  <si>
+    <t>175999387</t>
+  </si>
+  <si>
+    <t>176002900</t>
+  </si>
+  <si>
+    <t>176006173</t>
+  </si>
+  <si>
+    <t>176008980</t>
+  </si>
+  <si>
+    <t>177861526</t>
+  </si>
+  <si>
+    <t>177869450</t>
+  </si>
+  <si>
+    <t>177870589</t>
+  </si>
+  <si>
+    <t>177871359</t>
+  </si>
+  <si>
+    <t>177872238</t>
+  </si>
+  <si>
+    <t>177873027</t>
+  </si>
+  <si>
+    <t>177874134</t>
+  </si>
+  <si>
+    <t>177875124</t>
+  </si>
+  <si>
+    <t>177876084</t>
+  </si>
+  <si>
+    <t>177877138</t>
+  </si>
+  <si>
+    <t>177878043</t>
+  </si>
+  <si>
+    <t>177878871</t>
+  </si>
+  <si>
+    <t>177879792</t>
+  </si>
+  <si>
+    <t>177880935</t>
+  </si>
+  <si>
+    <t>177881825</t>
+  </si>
+  <si>
+    <t>177882871</t>
+  </si>
+  <si>
+    <t>177884123</t>
+  </si>
+  <si>
+    <t>177885042</t>
+  </si>
+  <si>
+    <t>177886401</t>
+  </si>
+  <si>
+    <t>177887497</t>
+  </si>
+  <si>
+    <t>177888659</t>
+  </si>
+  <si>
+    <t>177889601</t>
+  </si>
+  <si>
+    <t>177890942</t>
+  </si>
+  <si>
+    <t>177891921</t>
+  </si>
+  <si>
+    <t>177893184</t>
+  </si>
+  <si>
+    <t>177894152</t>
+  </si>
+  <si>
+    <t>177895450</t>
+  </si>
+  <si>
+    <t>177896744</t>
+  </si>
+  <si>
+    <t>177897996</t>
+  </si>
+  <si>
+    <t>177899185</t>
+  </si>
+  <si>
+    <t>177900496</t>
+  </si>
+  <si>
+    <t>177901540</t>
+  </si>
+  <si>
+    <t>177902590</t>
+  </si>
+  <si>
+    <t>177903799</t>
+  </si>
+  <si>
+    <t>177905107</t>
+  </si>
+  <si>
+    <t>177906130</t>
+  </si>
+  <si>
+    <t>177907671</t>
+  </si>
+  <si>
+    <t>177908995</t>
+  </si>
+  <si>
+    <t>177910062</t>
+  </si>
+  <si>
+    <t>177911873</t>
+  </si>
+  <si>
+    <t>177913169</t>
+  </si>
+  <si>
+    <t>177914496</t>
+  </si>
+  <si>
+    <t>177916123</t>
+  </si>
+  <si>
+    <t>177917323</t>
+  </si>
+  <si>
+    <t>177918503</t>
+  </si>
+  <si>
+    <t>177919687</t>
+  </si>
+  <si>
+    <t>177921235</t>
+  </si>
+  <si>
+    <t>177922464</t>
+  </si>
+  <si>
+    <t>177923715</t>
+  </si>
+  <si>
+    <t>177925066</t>
+  </si>
+  <si>
+    <t>177926718</t>
+  </si>
+  <si>
+    <t>177928143</t>
+  </si>
+  <si>
+    <t>177929941</t>
+  </si>
+  <si>
+    <t>177932247</t>
+  </si>
+  <si>
+    <t>177934528</t>
+  </si>
+  <si>
+    <t>177938061</t>
+  </si>
+  <si>
+    <t>177941915</t>
+  </si>
+  <si>
+    <t>177944383</t>
+  </si>
+  <si>
+    <t>177945811</t>
+  </si>
+  <si>
+    <t>177947167</t>
+  </si>
+  <si>
+    <t>177948637</t>
+  </si>
+  <si>
+    <t>177950299</t>
+  </si>
+  <si>
+    <t>177952324</t>
+  </si>
+  <si>
+    <t>177954731</t>
+  </si>
+  <si>
+    <t>177957165</t>
+  </si>
+  <si>
+    <t>177960012</t>
+  </si>
+  <si>
+    <t>177962949</t>
+  </si>
+  <si>
+    <t>177965624</t>
+  </si>
+  <si>
+    <t>177968292</t>
+  </si>
+  <si>
+    <t>177970967</t>
   </si>
 </sst>
 </file>
@@ -2778,7 +3408,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>612</v>
+        <v>822</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3018,7 +3648,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>613</v>
+        <v>823</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3054,7 +3684,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>614</v>
+        <v>824</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3090,7 +3720,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>615</v>
+        <v>825</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3126,7 +3756,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>616</v>
+        <v>826</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3162,7 +3792,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>617</v>
+        <v>827</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,7 +3826,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>618</v>
+        <v>828</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3230,7 +3860,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>619</v>
+        <v>829</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,7 +3896,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>620</v>
+        <v>830</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3302,7 +3932,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>621</v>
+        <v>831</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3338,7 +3968,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>622</v>
+        <v>832</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3374,7 +4004,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>623</v>
+        <v>833</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,7 +4040,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>624</v>
+        <v>834</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3446,7 +4076,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>625</v>
+        <v>835</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3482,7 +4112,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>626</v>
+        <v>836</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3518,7 +4148,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>627</v>
+        <v>837</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3554,7 +4184,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>628</v>
+        <v>838</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3590,7 +4220,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>629</v>
+        <v>839</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3624,7 +4254,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>630</v>
+        <v>840</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3658,7 +4288,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>631</v>
+        <v>841</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,7 +4324,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>632</v>
+        <v>842</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3730,7 +4360,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>633</v>
+        <v>843</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3766,7 +4396,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>634</v>
+        <v>844</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3802,7 +4432,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>635</v>
+        <v>845</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3838,7 +4468,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>636</v>
+        <v>846</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3874,7 +4504,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>637</v>
+        <v>847</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3908,7 +4538,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>638</v>
+        <v>848</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3944,7 +4574,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>639</v>
+        <v>849</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3980,7 +4610,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>640</v>
+        <v>850</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4016,7 +4646,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>641</v>
+        <v>851</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4052,7 +4682,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>642</v>
+        <v>852</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4088,7 +4718,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>643</v>
+        <v>853</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,7 +4754,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>644</v>
+        <v>854</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4160,7 +4790,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>645</v>
+        <v>855</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,7 +4824,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>646</v>
+        <v>856</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4228,7 +4858,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>647</v>
+        <v>857</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4264,7 +4894,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>648</v>
+        <v>858</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4300,7 +4930,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>649</v>
+        <v>859</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4336,7 +4966,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>650</v>
+        <v>860</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4372,7 +5002,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>651</v>
+        <v>861</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4408,7 +5038,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>652</v>
+        <v>862</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4444,7 +5074,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>653</v>
+        <v>863</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,7 +5110,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>655</v>
+        <v>865</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4516,7 +5146,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>656</v>
+        <v>866</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4552,7 +5182,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>657</v>
+        <v>867</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4588,7 +5218,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>654</v>
+        <v>864</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4624,7 +5254,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>658</v>
+        <v>868</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4660,7 +5290,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>659</v>
+        <v>869</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4696,7 +5326,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>660</v>
+        <v>870</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4732,7 +5362,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>661</v>
+        <v>871</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4766,7 +5396,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>662</v>
+        <v>872</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4802,7 +5432,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>663</v>
+        <v>873</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4834,7 +5464,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>664</v>
+        <v>874</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4870,7 +5500,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>674</v>
+        <v>884</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4902,7 +5532,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>675</v>
+        <v>885</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4934,7 +5564,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>676</v>
+        <v>886</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4966,7 +5596,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>677</v>
+        <v>887</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4998,7 +5628,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>678</v>
+        <v>888</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5030,7 +5660,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>679</v>
+        <v>889</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5062,7 +5692,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>680</v>
+        <v>890</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5094,7 +5724,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>681</v>
+        <v>891</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5128,7 +5758,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>665</v>
+        <v>875</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5164,7 +5794,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>669</v>
+        <v>879</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5198,7 +5828,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>670</v>
+        <v>880</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5232,7 +5862,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>666</v>
+        <v>876</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5266,7 +5896,7 @@
         <v>171</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>667</v>
+        <v>877</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5300,7 +5930,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>668</v>
+        <v>878</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5332,7 +5962,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>671</v>
+        <v>881</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5364,7 +5994,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>672</v>
+        <v>882</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5396,7 +6026,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>673</v>
+        <v>883</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs - latest verison used in the yaml file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="961">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -2777,6 +2777,213 @@
   </si>
   <si>
     <t>177970967</t>
+  </si>
+  <si>
+    <t>220930916</t>
+  </si>
+  <si>
+    <t>220973741</t>
+  </si>
+  <si>
+    <t>220975277</t>
+  </si>
+  <si>
+    <t>220976305</t>
+  </si>
+  <si>
+    <t>220977462</t>
+  </si>
+  <si>
+    <t>220978293</t>
+  </si>
+  <si>
+    <t>220979139</t>
+  </si>
+  <si>
+    <t>220979975</t>
+  </si>
+  <si>
+    <t>220981368</t>
+  </si>
+  <si>
+    <t>220982239</t>
+  </si>
+  <si>
+    <t>220983646</t>
+  </si>
+  <si>
+    <t>220984585</t>
+  </si>
+  <si>
+    <t>220985453</t>
+  </si>
+  <si>
+    <t>220986403</t>
+  </si>
+  <si>
+    <t>220987351</t>
+  </si>
+  <si>
+    <t>220988325</t>
+  </si>
+  <si>
+    <t>220989709</t>
+  </si>
+  <si>
+    <t>220990610</t>
+  </si>
+  <si>
+    <t>220991836</t>
+  </si>
+  <si>
+    <t>220992806</t>
+  </si>
+  <si>
+    <t>220994313</t>
+  </si>
+  <si>
+    <t>220995468</t>
+  </si>
+  <si>
+    <t>220996679</t>
+  </si>
+  <si>
+    <t>220998173</t>
+  </si>
+  <si>
+    <t>220999186</t>
+  </si>
+  <si>
+    <t>221000230</t>
+  </si>
+  <si>
+    <t>221001231</t>
+  </si>
+  <si>
+    <t>221002261</t>
+  </si>
+  <si>
+    <t>221003626</t>
+  </si>
+  <si>
+    <t>221004891</t>
+  </si>
+  <si>
+    <t>221006205</t>
+  </si>
+  <si>
+    <t>221007307</t>
+  </si>
+  <si>
+    <t>221008377</t>
+  </si>
+  <si>
+    <t>221009595</t>
+  </si>
+  <si>
+    <t>221010878</t>
+  </si>
+  <si>
+    <t>221011972</t>
+  </si>
+  <si>
+    <t>221013481</t>
+  </si>
+  <si>
+    <t>221014725</t>
+  </si>
+  <si>
+    <t>221015875</t>
+  </si>
+  <si>
+    <t>221017508</t>
+  </si>
+  <si>
+    <t>221018693</t>
+  </si>
+  <si>
+    <t>221019896</t>
+  </si>
+  <si>
+    <t>221021129</t>
+  </si>
+  <si>
+    <t>221022650</t>
+  </si>
+  <si>
+    <t>221023854</t>
+  </si>
+  <si>
+    <t>221025211</t>
+  </si>
+  <si>
+    <t>221026505</t>
+  </si>
+  <si>
+    <t>221028022</t>
+  </si>
+  <si>
+    <t>221029891</t>
+  </si>
+  <si>
+    <t>221032144</t>
+  </si>
+  <si>
+    <t>221034744</t>
+  </si>
+  <si>
+    <t>221036395</t>
+  </si>
+  <si>
+    <t>221039201</t>
+  </si>
+  <si>
+    <t>221042579</t>
+  </si>
+  <si>
+    <t>221045176</t>
+  </si>
+  <si>
+    <t>221050316</t>
+  </si>
+  <si>
+    <t>221055188</t>
+  </si>
+  <si>
+    <t>221058023</t>
+  </si>
+  <si>
+    <t>221059818</t>
+  </si>
+  <si>
+    <t>221061587</t>
+  </si>
+  <si>
+    <t>221063270</t>
+  </si>
+  <si>
+    <t>221065001</t>
+  </si>
+  <si>
+    <t>221067352</t>
+  </si>
+  <si>
+    <t>221069911</t>
+  </si>
+  <si>
+    <t>221073130</t>
+  </si>
+  <si>
+    <t>221076549</t>
+  </si>
+  <si>
+    <t>221079281</t>
+  </si>
+  <si>
+    <t>221082353</t>
+  </si>
+  <si>
+    <t>221085186</t>
   </si>
 </sst>
 </file>
@@ -3408,7 +3615,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>822</v>
+        <v>892</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3648,7 +3855,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>823</v>
+        <v>893</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3684,7 +3891,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>824</v>
+        <v>894</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3720,7 +3927,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>825</v>
+        <v>895</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3756,7 +3963,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>826</v>
+        <v>896</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,7 +3999,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>827</v>
+        <v>897</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3826,7 +4033,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>828</v>
+        <v>898</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3860,7 +4067,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>829</v>
+        <v>899</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3896,7 +4103,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>830</v>
+        <v>900</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3932,7 +4139,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>831</v>
+        <v>901</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3968,7 +4175,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>832</v>
+        <v>902</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4004,7 +4211,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>833</v>
+        <v>903</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4040,7 +4247,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>834</v>
+        <v>904</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4076,7 +4283,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>835</v>
+        <v>905</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4112,7 +4319,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>836</v>
+        <v>906</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4148,7 +4355,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>837</v>
+        <v>907</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,7 +4391,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>838</v>
+        <v>908</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,7 +4427,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>839</v>
+        <v>909</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,7 +4461,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>840</v>
+        <v>910</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4288,7 +4495,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>841</v>
+        <v>911</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4324,7 +4531,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>842</v>
+        <v>912</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4360,7 +4567,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>843</v>
+        <v>913</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4396,7 +4603,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>844</v>
+        <v>914</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4432,7 +4639,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>845</v>
+        <v>915</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4468,7 +4675,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>846</v>
+        <v>916</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4504,7 +4711,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>847</v>
+        <v>917</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4538,7 +4745,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>848</v>
+        <v>918</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4574,7 +4781,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>849</v>
+        <v>919</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4610,7 +4817,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>850</v>
+        <v>920</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4646,7 +4853,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>851</v>
+        <v>921</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4682,7 +4889,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>852</v>
+        <v>922</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4718,7 +4925,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>853</v>
+        <v>923</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4754,7 +4961,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>854</v>
+        <v>924</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4790,7 +4997,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>855</v>
+        <v>925</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4824,7 +5031,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>856</v>
+        <v>926</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4858,7 +5065,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>857</v>
+        <v>927</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4894,7 +5101,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>858</v>
+        <v>928</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,7 +5137,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>859</v>
+        <v>929</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4966,7 +5173,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>860</v>
+        <v>930</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5002,7 +5209,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>861</v>
+        <v>931</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5038,7 +5245,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>862</v>
+        <v>932</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5074,7 +5281,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>863</v>
+        <v>933</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5110,7 +5317,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>865</v>
+        <v>935</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5146,7 +5353,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>866</v>
+        <v>936</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5182,7 +5389,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>867</v>
+        <v>937</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5218,7 +5425,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>864</v>
+        <v>934</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5254,7 +5461,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>868</v>
+        <v>938</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5290,7 +5497,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>869</v>
+        <v>939</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5326,7 +5533,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>870</v>
+        <v>940</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5362,7 +5569,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>871</v>
+        <v>941</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5396,7 +5603,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>872</v>
+        <v>942</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5432,7 +5639,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>873</v>
+        <v>943</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5464,7 +5671,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>874</v>
+        <v>944</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5500,7 +5707,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>884</v>
+        <v>954</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5532,7 +5739,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>885</v>
+        <v>955</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5564,7 +5771,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>886</v>
+        <v>956</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5628,7 +5835,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>888</v>
+        <v>957</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5660,7 +5867,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>889</v>
+        <v>958</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5692,7 +5899,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>890</v>
+        <v>959</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5724,7 +5931,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>891</v>
+        <v>960</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5758,7 +5965,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>875</v>
+        <v>945</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5794,7 +6001,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>879</v>
+        <v>949</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5828,7 +6035,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>880</v>
+        <v>950</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5862,7 +6069,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5896,7 +6103,7 @@
         <v>171</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>877</v>
+        <v>947</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5930,7 +6137,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>878</v>
+        <v>948</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5962,7 +6169,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>881</v>
+        <v>951</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5994,7 +6201,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>882</v>
+        <v>952</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6026,7 +6233,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>883</v>
+        <v>953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore - email format and attachment setting have done in the yaml file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="1031">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -2984,6 +2984,216 @@
   </si>
   <si>
     <t>221085186</t>
+  </si>
+  <si>
+    <t>263470844</t>
+  </si>
+  <si>
+    <t>263478454</t>
+  </si>
+  <si>
+    <t>263479841</t>
+  </si>
+  <si>
+    <t>263481152</t>
+  </si>
+  <si>
+    <t>263482411</t>
+  </si>
+  <si>
+    <t>263483258</t>
+  </si>
+  <si>
+    <t>263484672</t>
+  </si>
+  <si>
+    <t>263485677</t>
+  </si>
+  <si>
+    <t>263486869</t>
+  </si>
+  <si>
+    <t>263487716</t>
+  </si>
+  <si>
+    <t>263488667</t>
+  </si>
+  <si>
+    <t>263489735</t>
+  </si>
+  <si>
+    <t>263490665</t>
+  </si>
+  <si>
+    <t>263491579</t>
+  </si>
+  <si>
+    <t>263492575</t>
+  </si>
+  <si>
+    <t>263493487</t>
+  </si>
+  <si>
+    <t>263495020</t>
+  </si>
+  <si>
+    <t>263495977</t>
+  </si>
+  <si>
+    <t>263497601</t>
+  </si>
+  <si>
+    <t>263498608</t>
+  </si>
+  <si>
+    <t>263499900</t>
+  </si>
+  <si>
+    <t>263500770</t>
+  </si>
+  <si>
+    <t>263502177</t>
+  </si>
+  <si>
+    <t>263503395</t>
+  </si>
+  <si>
+    <t>263504687</t>
+  </si>
+  <si>
+    <t>263505764</t>
+  </si>
+  <si>
+    <t>263506898</t>
+  </si>
+  <si>
+    <t>263507966</t>
+  </si>
+  <si>
+    <t>263509239</t>
+  </si>
+  <si>
+    <t>263510354</t>
+  </si>
+  <si>
+    <t>263511684</t>
+  </si>
+  <si>
+    <t>263513086</t>
+  </si>
+  <si>
+    <t>263514187</t>
+  </si>
+  <si>
+    <t>263515276</t>
+  </si>
+  <si>
+    <t>263516565</t>
+  </si>
+  <si>
+    <t>263517778</t>
+  </si>
+  <si>
+    <t>263519166</t>
+  </si>
+  <si>
+    <t>263520234</t>
+  </si>
+  <si>
+    <t>263521315</t>
+  </si>
+  <si>
+    <t>263522919</t>
+  </si>
+  <si>
+    <t>263524429</t>
+  </si>
+  <si>
+    <t>263525839</t>
+  </si>
+  <si>
+    <t>263527101</t>
+  </si>
+  <si>
+    <t>263528473</t>
+  </si>
+  <si>
+    <t>263529715</t>
+  </si>
+  <si>
+    <t>263530954</t>
+  </si>
+  <si>
+    <t>263532173</t>
+  </si>
+  <si>
+    <t>263533606</t>
+  </si>
+  <si>
+    <t>263534859</t>
+  </si>
+  <si>
+    <t>263536116</t>
+  </si>
+  <si>
+    <t>263537894</t>
+  </si>
+  <si>
+    <t>263539512</t>
+  </si>
+  <si>
+    <t>263541161</t>
+  </si>
+  <si>
+    <t>263543793</t>
+  </si>
+  <si>
+    <t>263546085</t>
+  </si>
+  <si>
+    <t>263550218</t>
+  </si>
+  <si>
+    <t>263553959</t>
+  </si>
+  <si>
+    <t>263556898</t>
+  </si>
+  <si>
+    <t>263558397</t>
+  </si>
+  <si>
+    <t>263559829</t>
+  </si>
+  <si>
+    <t>263561477</t>
+  </si>
+  <si>
+    <t>263563419</t>
+  </si>
+  <si>
+    <t>263565290</t>
+  </si>
+  <si>
+    <t>263568735</t>
+  </si>
+  <si>
+    <t>263571081</t>
+  </si>
+  <si>
+    <t>263574398</t>
+  </si>
+  <si>
+    <t>263576798</t>
+  </si>
+  <si>
+    <t>263580486</t>
+  </si>
+  <si>
+    <t>263583431</t>
+  </si>
+  <si>
+    <t>263586110</t>
   </si>
 </sst>
 </file>
@@ -3615,7 +3825,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>892</v>
+        <v>961</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3855,7 +4065,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>893</v>
+        <v>962</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,7 +4101,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>894</v>
+        <v>963</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3927,7 +4137,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>895</v>
+        <v>964</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3963,7 +4173,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>896</v>
+        <v>965</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,7 +4209,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>897</v>
+        <v>966</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4033,7 +4243,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>898</v>
+        <v>967</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4067,7 +4277,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>899</v>
+        <v>968</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4103,7 +4313,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>900</v>
+        <v>969</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4139,7 +4349,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>901</v>
+        <v>970</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4175,7 +4385,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>902</v>
+        <v>971</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4211,7 +4421,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>903</v>
+        <v>972</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4247,7 +4457,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>904</v>
+        <v>973</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4283,7 +4493,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>905</v>
+        <v>974</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4319,7 +4529,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>906</v>
+        <v>975</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4355,7 +4565,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>907</v>
+        <v>976</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4391,7 +4601,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>908</v>
+        <v>977</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4427,7 +4637,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>909</v>
+        <v>978</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4461,7 +4671,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>910</v>
+        <v>979</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4495,7 +4705,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>911</v>
+        <v>980</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4531,7 +4741,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>912</v>
+        <v>981</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4567,7 +4777,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>913</v>
+        <v>982</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4603,7 +4813,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>914</v>
+        <v>983</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4639,7 +4849,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>915</v>
+        <v>984</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4675,7 +4885,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>916</v>
+        <v>985</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4711,7 +4921,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>917</v>
+        <v>986</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4745,7 +4955,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>918</v>
+        <v>987</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4781,7 +4991,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>919</v>
+        <v>988</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4817,7 +5027,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>920</v>
+        <v>989</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4853,7 +5063,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>921</v>
+        <v>990</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4889,7 +5099,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>922</v>
+        <v>991</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4925,7 +5135,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>923</v>
+        <v>992</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4961,7 +5171,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>924</v>
+        <v>993</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4997,7 +5207,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>925</v>
+        <v>994</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5031,7 +5241,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>926</v>
+        <v>995</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5065,7 +5275,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>927</v>
+        <v>996</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5101,7 +5311,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>928</v>
+        <v>997</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5137,7 +5347,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>929</v>
+        <v>998</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5173,7 +5383,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>930</v>
+        <v>999</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5209,7 +5419,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>931</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5245,7 +5455,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>932</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5281,7 +5491,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>933</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5317,7 +5527,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>935</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5353,7 +5563,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>936</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5389,7 +5599,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>937</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5425,7 +5635,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>934</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5461,7 +5671,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>938</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5497,7 +5707,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>939</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5533,7 +5743,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>940</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5569,7 +5779,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>941</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5603,7 +5813,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>942</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5639,7 +5849,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>943</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5671,7 +5881,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>944</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5707,7 +5917,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>954</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5739,7 +5949,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>955</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5771,7 +5981,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>956</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5803,7 +6013,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>887</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5835,7 +6045,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>957</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5867,7 +6077,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>958</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5899,7 +6109,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>959</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5931,7 +6141,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>960</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5965,7 +6175,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>945</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6001,7 +6211,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>949</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6035,7 +6245,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>950</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6069,7 +6279,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>946</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6103,7 +6313,7 @@
         <v>171</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>947</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6137,7 +6347,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>948</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6169,7 +6379,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>951</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6201,7 +6411,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>952</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6233,7 +6443,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>953</v>
+        <v>1022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat - ChainTest Report(Extent Report)
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="1099">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -3194,6 +3194,210 @@
   </si>
   <si>
     <t>263586110</t>
+  </si>
+  <si>
+    <t>312395410</t>
+  </si>
+  <si>
+    <t>312404733</t>
+  </si>
+  <si>
+    <t>312405817</t>
+  </si>
+  <si>
+    <t>312406936</t>
+  </si>
+  <si>
+    <t>312408284</t>
+  </si>
+  <si>
+    <t>312409403</t>
+  </si>
+  <si>
+    <t>312410885</t>
+  </si>
+  <si>
+    <t>312412014</t>
+  </si>
+  <si>
+    <t>312413581</t>
+  </si>
+  <si>
+    <t>312414686</t>
+  </si>
+  <si>
+    <t>312416195</t>
+  </si>
+  <si>
+    <t>312417421</t>
+  </si>
+  <si>
+    <t>312418427</t>
+  </si>
+  <si>
+    <t>312419971</t>
+  </si>
+  <si>
+    <t>312421123</t>
+  </si>
+  <si>
+    <t>312422394</t>
+  </si>
+  <si>
+    <t>312423865</t>
+  </si>
+  <si>
+    <t>312425100</t>
+  </si>
+  <si>
+    <t>312426775</t>
+  </si>
+  <si>
+    <t>312427830</t>
+  </si>
+  <si>
+    <t>312429238</t>
+  </si>
+  <si>
+    <t>312430919</t>
+  </si>
+  <si>
+    <t>312432460</t>
+  </si>
+  <si>
+    <t>312434079</t>
+  </si>
+  <si>
+    <t>312435367</t>
+  </si>
+  <si>
+    <t>312436649</t>
+  </si>
+  <si>
+    <t>312438144</t>
+  </si>
+  <si>
+    <t>312439590</t>
+  </si>
+  <si>
+    <t>312441490</t>
+  </si>
+  <si>
+    <t>312442965</t>
+  </si>
+  <si>
+    <t>312444700</t>
+  </si>
+  <si>
+    <t>312446387</t>
+  </si>
+  <si>
+    <t>312447788</t>
+  </si>
+  <si>
+    <t>312449474</t>
+  </si>
+  <si>
+    <t>312451037</t>
+  </si>
+  <si>
+    <t>312452344</t>
+  </si>
+  <si>
+    <t>312454094</t>
+  </si>
+  <si>
+    <t>312456103</t>
+  </si>
+  <si>
+    <t>312457552</t>
+  </si>
+  <si>
+    <t>312459623</t>
+  </si>
+  <si>
+    <t>312461188</t>
+  </si>
+  <si>
+    <t>312462621</t>
+  </si>
+  <si>
+    <t>312464563</t>
+  </si>
+  <si>
+    <t>312466110</t>
+  </si>
+  <si>
+    <t>312467630</t>
+  </si>
+  <si>
+    <t>312469247</t>
+  </si>
+  <si>
+    <t>312471138</t>
+  </si>
+  <si>
+    <t>312473072</t>
+  </si>
+  <si>
+    <t>312474844</t>
+  </si>
+  <si>
+    <t>312476718</t>
+  </si>
+  <si>
+    <t>312479412</t>
+  </si>
+  <si>
+    <t>312481447</t>
+  </si>
+  <si>
+    <t>312483736</t>
+  </si>
+  <si>
+    <t>312487099</t>
+  </si>
+  <si>
+    <t>312489698</t>
+  </si>
+  <si>
+    <t>312494272</t>
+  </si>
+  <si>
+    <t>312499325</t>
+  </si>
+  <si>
+    <t>312502773</t>
+  </si>
+  <si>
+    <t>312504626</t>
+  </si>
+  <si>
+    <t>312506669</t>
+  </si>
+  <si>
+    <t>312510026</t>
+  </si>
+  <si>
+    <t>312513563</t>
+  </si>
+  <si>
+    <t>312517017</t>
+  </si>
+  <si>
+    <t>312520996</t>
+  </si>
+  <si>
+    <t>312523886</t>
+  </si>
+  <si>
+    <t>312527584</t>
+  </si>
+  <si>
+    <t>312531015</t>
+  </si>
+  <si>
+    <t>312534611</t>
   </si>
 </sst>
 </file>
@@ -3825,7 +4029,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>961</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4065,7 +4269,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>962</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4101,7 +4305,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>963</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4137,7 +4341,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>964</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4173,7 +4377,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>965</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,7 +4413,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>966</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4243,7 +4447,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>967</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4277,7 +4481,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>968</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4313,7 +4517,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>969</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4349,7 +4553,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>970</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,7 +4589,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>971</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4421,7 +4625,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>972</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4457,7 +4661,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>973</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4493,7 +4697,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>974</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4529,7 +4733,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>975</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4565,7 +4769,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>976</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4601,7 +4805,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>977</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4637,7 +4841,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>978</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4671,7 +4875,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>979</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4705,7 +4909,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>980</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4741,7 +4945,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>981</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4777,7 +4981,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>982</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4813,7 +5017,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>983</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4849,7 +5053,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>984</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4885,7 +5089,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>985</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4921,7 +5125,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>986</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4955,7 +5159,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>987</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4991,7 +5195,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>988</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,7 +5231,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>989</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5063,7 +5267,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>990</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5099,7 +5303,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>991</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5135,7 +5339,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>992</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5171,7 +5375,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>993</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5207,7 +5411,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>994</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5241,7 +5445,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>995</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5275,7 +5479,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>996</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5311,7 +5515,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>997</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5347,7 +5551,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>998</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5383,7 +5587,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>999</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5419,7 +5623,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>1000</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5455,7 +5659,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>1001</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5491,7 +5695,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>1002</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5527,7 +5731,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>1004</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5563,7 +5767,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>1005</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5599,7 +5803,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>1006</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5635,7 +5839,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>1003</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5671,7 +5875,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>1007</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5707,7 +5911,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>1008</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5743,7 +5947,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>1009</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5779,7 +5983,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>1010</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5813,7 +6017,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>1011</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5849,7 +6053,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>1012</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5881,7 +6085,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>1013</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5917,7 +6121,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>1023</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5949,7 +6153,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>1024</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5981,7 +6185,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>1025</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6013,7 +6217,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>1026</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6045,7 +6249,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>1027</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6077,7 +6281,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>1028</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6109,7 +6313,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>1029</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6141,7 +6345,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>1030</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6175,7 +6379,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>1014</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6279,7 +6483,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>1015</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6313,7 +6517,7 @@
         <v>171</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>1016</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6347,7 +6551,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>1017</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6379,7 +6583,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>1020</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6411,7 +6615,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>1021</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6443,7 +6647,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>1022</v>
+        <v>1090</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat - Chaintest resport has added. Common reusablity methods added for response validation
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="1631">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -3398,6 +3398,1602 @@
   </si>
   <si>
     <t>312534611</t>
+  </si>
+  <si>
+    <t>314089213</t>
+  </si>
+  <si>
+    <t>314120642</t>
+  </si>
+  <si>
+    <t>314122499</t>
+  </si>
+  <si>
+    <t>314124111</t>
+  </si>
+  <si>
+    <t>314126137</t>
+  </si>
+  <si>
+    <t>314127882</t>
+  </si>
+  <si>
+    <t>314130002</t>
+  </si>
+  <si>
+    <t>314131608</t>
+  </si>
+  <si>
+    <t>314133791</t>
+  </si>
+  <si>
+    <t>314135537</t>
+  </si>
+  <si>
+    <t>314137429</t>
+  </si>
+  <si>
+    <t>314138823</t>
+  </si>
+  <si>
+    <t>314140602</t>
+  </si>
+  <si>
+    <t>314141854</t>
+  </si>
+  <si>
+    <t>314143439</t>
+  </si>
+  <si>
+    <t>314144887</t>
+  </si>
+  <si>
+    <t>314146563</t>
+  </si>
+  <si>
+    <t>314147869</t>
+  </si>
+  <si>
+    <t>314149352</t>
+  </si>
+  <si>
+    <t>314150893</t>
+  </si>
+  <si>
+    <t>314152718</t>
+  </si>
+  <si>
+    <t>314154515</t>
+  </si>
+  <si>
+    <t>314156722</t>
+  </si>
+  <si>
+    <t>314158306</t>
+  </si>
+  <si>
+    <t>314159676</t>
+  </si>
+  <si>
+    <t>314161476</t>
+  </si>
+  <si>
+    <t>314163139</t>
+  </si>
+  <si>
+    <t>314164797</t>
+  </si>
+  <si>
+    <t>314166662</t>
+  </si>
+  <si>
+    <t>314168627</t>
+  </si>
+  <si>
+    <t>314170582</t>
+  </si>
+  <si>
+    <t>314172117</t>
+  </si>
+  <si>
+    <t>314173761</t>
+  </si>
+  <si>
+    <t>314175464</t>
+  </si>
+  <si>
+    <t>314176952</t>
+  </si>
+  <si>
+    <t>314178400</t>
+  </si>
+  <si>
+    <t>314180567</t>
+  </si>
+  <si>
+    <t>314181989</t>
+  </si>
+  <si>
+    <t>314183729</t>
+  </si>
+  <si>
+    <t>314185575</t>
+  </si>
+  <si>
+    <t>314187303</t>
+  </si>
+  <si>
+    <t>314189229</t>
+  </si>
+  <si>
+    <t>314190985</t>
+  </si>
+  <si>
+    <t>314192737</t>
+  </si>
+  <si>
+    <t>314194378</t>
+  </si>
+  <si>
+    <t>314196362</t>
+  </si>
+  <si>
+    <t>314198302</t>
+  </si>
+  <si>
+    <t>314200323</t>
+  </si>
+  <si>
+    <t>314202299</t>
+  </si>
+  <si>
+    <t>314204482</t>
+  </si>
+  <si>
+    <t>314206339</t>
+  </si>
+  <si>
+    <t>314208249</t>
+  </si>
+  <si>
+    <t>314210317</t>
+  </si>
+  <si>
+    <t>314213668</t>
+  </si>
+  <si>
+    <t>314216573</t>
+  </si>
+  <si>
+    <t>314221287</t>
+  </si>
+  <si>
+    <t>314226526</t>
+  </si>
+  <si>
+    <t>314229929</t>
+  </si>
+  <si>
+    <t>314231927</t>
+  </si>
+  <si>
+    <t>314233708</t>
+  </si>
+  <si>
+    <t>314235654</t>
+  </si>
+  <si>
+    <t>314237828</t>
+  </si>
+  <si>
+    <t>314240380</t>
+  </si>
+  <si>
+    <t>314243789</t>
+  </si>
+  <si>
+    <t>314247470</t>
+  </si>
+  <si>
+    <t>314251239</t>
+  </si>
+  <si>
+    <t>314254413</t>
+  </si>
+  <si>
+    <t>314257932</t>
+  </si>
+  <si>
+    <t>314262227</t>
+  </si>
+  <si>
+    <t>314267280</t>
+  </si>
+  <si>
+    <t>316832435</t>
+  </si>
+  <si>
+    <t>316848571</t>
+  </si>
+  <si>
+    <t>316850119</t>
+  </si>
+  <si>
+    <t>316852020</t>
+  </si>
+  <si>
+    <t>316853453</t>
+  </si>
+  <si>
+    <t>316855169</t>
+  </si>
+  <si>
+    <t>316856673</t>
+  </si>
+  <si>
+    <t>316857889</t>
+  </si>
+  <si>
+    <t>316860409</t>
+  </si>
+  <si>
+    <t>316861822</t>
+  </si>
+  <si>
+    <t>316863408</t>
+  </si>
+  <si>
+    <t>316864685</t>
+  </si>
+  <si>
+    <t>316865818</t>
+  </si>
+  <si>
+    <t>316866915</t>
+  </si>
+  <si>
+    <t>316867977</t>
+  </si>
+  <si>
+    <t>316869382</t>
+  </si>
+  <si>
+    <t>316870875</t>
+  </si>
+  <si>
+    <t>316872016</t>
+  </si>
+  <si>
+    <t>316873486</t>
+  </si>
+  <si>
+    <t>316875039</t>
+  </si>
+  <si>
+    <t>316876656</t>
+  </si>
+  <si>
+    <t>316877954</t>
+  </si>
+  <si>
+    <t>316879586</t>
+  </si>
+  <si>
+    <t>316881219</t>
+  </si>
+  <si>
+    <t>316883421</t>
+  </si>
+  <si>
+    <t>316884596</t>
+  </si>
+  <si>
+    <t>316886071</t>
+  </si>
+  <si>
+    <t>316887322</t>
+  </si>
+  <si>
+    <t>316889042</t>
+  </si>
+  <si>
+    <t>316890567</t>
+  </si>
+  <si>
+    <t>316892144</t>
+  </si>
+  <si>
+    <t>316893439</t>
+  </si>
+  <si>
+    <t>316894702</t>
+  </si>
+  <si>
+    <t>316896377</t>
+  </si>
+  <si>
+    <t>316897826</t>
+  </si>
+  <si>
+    <t>316899119</t>
+  </si>
+  <si>
+    <t>316900842</t>
+  </si>
+  <si>
+    <t>316902514</t>
+  </si>
+  <si>
+    <t>316904098</t>
+  </si>
+  <si>
+    <t>316905999</t>
+  </si>
+  <si>
+    <t>316907615</t>
+  </si>
+  <si>
+    <t>316909200</t>
+  </si>
+  <si>
+    <t>316910561</t>
+  </si>
+  <si>
+    <t>316911949</t>
+  </si>
+  <si>
+    <t>316913712</t>
+  </si>
+  <si>
+    <t>316915324</t>
+  </si>
+  <si>
+    <t>316916727</t>
+  </si>
+  <si>
+    <t>316918583</t>
+  </si>
+  <si>
+    <t>316920493</t>
+  </si>
+  <si>
+    <t>316921937</t>
+  </si>
+  <si>
+    <t>316923670</t>
+  </si>
+  <si>
+    <t>316925138</t>
+  </si>
+  <si>
+    <t>316927265</t>
+  </si>
+  <si>
+    <t>317606925</t>
+  </si>
+  <si>
+    <t>317778466</t>
+  </si>
+  <si>
+    <t>318079088</t>
+  </si>
+  <si>
+    <t>318166841</t>
+  </si>
+  <si>
+    <t>318558079</t>
+  </si>
+  <si>
+    <t>318562454</t>
+  </si>
+  <si>
+    <t>318563532</t>
+  </si>
+  <si>
+    <t>318565107</t>
+  </si>
+  <si>
+    <t>318566075</t>
+  </si>
+  <si>
+    <t>318567362</t>
+  </si>
+  <si>
+    <t>318568266</t>
+  </si>
+  <si>
+    <t>318569938</t>
+  </si>
+  <si>
+    <t>318570878</t>
+  </si>
+  <si>
+    <t>318572519</t>
+  </si>
+  <si>
+    <t>318573502</t>
+  </si>
+  <si>
+    <t>318574544</t>
+  </si>
+  <si>
+    <t>318655535</t>
+  </si>
+  <si>
+    <t>318659549</t>
+  </si>
+  <si>
+    <t>318660993</t>
+  </si>
+  <si>
+    <t>318662353</t>
+  </si>
+  <si>
+    <t>318663299</t>
+  </si>
+  <si>
+    <t>318664639</t>
+  </si>
+  <si>
+    <t>318665538</t>
+  </si>
+  <si>
+    <t>318666867</t>
+  </si>
+  <si>
+    <t>318668099</t>
+  </si>
+  <si>
+    <t>318669497</t>
+  </si>
+  <si>
+    <t>318670453</t>
+  </si>
+  <si>
+    <t>318671444</t>
+  </si>
+  <si>
+    <t>318899138</t>
+  </si>
+  <si>
+    <t>318903406</t>
+  </si>
+  <si>
+    <t>318904819</t>
+  </si>
+  <si>
+    <t>318906405</t>
+  </si>
+  <si>
+    <t>318907513</t>
+  </si>
+  <si>
+    <t>318908873</t>
+  </si>
+  <si>
+    <t>318909940</t>
+  </si>
+  <si>
+    <t>318911522</t>
+  </si>
+  <si>
+    <t>318912628</t>
+  </si>
+  <si>
+    <t>318914422</t>
+  </si>
+  <si>
+    <t>318915563</t>
+  </si>
+  <si>
+    <t>318916738</t>
+  </si>
+  <si>
+    <t>319093949</t>
+  </si>
+  <si>
+    <t>319098489</t>
+  </si>
+  <si>
+    <t>319100074</t>
+  </si>
+  <si>
+    <t>319101748</t>
+  </si>
+  <si>
+    <t>319103012</t>
+  </si>
+  <si>
+    <t>319184736</t>
+  </si>
+  <si>
+    <t>319189151</t>
+  </si>
+  <si>
+    <t>319190763</t>
+  </si>
+  <si>
+    <t>319192820</t>
+  </si>
+  <si>
+    <t>319194546</t>
+  </si>
+  <si>
+    <t>319395403</t>
+  </si>
+  <si>
+    <t>319400588</t>
+  </si>
+  <si>
+    <t>319402217</t>
+  </si>
+  <si>
+    <t>319404126</t>
+  </si>
+  <si>
+    <t>319405421</t>
+  </si>
+  <si>
+    <t>319442950</t>
+  </si>
+  <si>
+    <t>319446947</t>
+  </si>
+  <si>
+    <t>319448486</t>
+  </si>
+  <si>
+    <t>319450214</t>
+  </si>
+  <si>
+    <t>319451811</t>
+  </si>
+  <si>
+    <t>319571105</t>
+  </si>
+  <si>
+    <t>319575342</t>
+  </si>
+  <si>
+    <t>319576916</t>
+  </si>
+  <si>
+    <t>319578575</t>
+  </si>
+  <si>
+    <t>319579860</t>
+  </si>
+  <si>
+    <t>319720227</t>
+  </si>
+  <si>
+    <t>319724917</t>
+  </si>
+  <si>
+    <t>319726739</t>
+  </si>
+  <si>
+    <t>319728498</t>
+  </si>
+  <si>
+    <t>319730101</t>
+  </si>
+  <si>
+    <t>319835560</t>
+  </si>
+  <si>
+    <t>319840071</t>
+  </si>
+  <si>
+    <t>319841732</t>
+  </si>
+  <si>
+    <t>319843054</t>
+  </si>
+  <si>
+    <t>319844451</t>
+  </si>
+  <si>
+    <t>319846172</t>
+  </si>
+  <si>
+    <t>319848066</t>
+  </si>
+  <si>
+    <t>319849548</t>
+  </si>
+  <si>
+    <t>319850953</t>
+  </si>
+  <si>
+    <t>319852912</t>
+  </si>
+  <si>
+    <t>319952487</t>
+  </si>
+  <si>
+    <t>319956905</t>
+  </si>
+  <si>
+    <t>319958505</t>
+  </si>
+  <si>
+    <t>319959858</t>
+  </si>
+  <si>
+    <t>319961208</t>
+  </si>
+  <si>
+    <t>319962515</t>
+  </si>
+  <si>
+    <t>319964236</t>
+  </si>
+  <si>
+    <t>319966576</t>
+  </si>
+  <si>
+    <t>319967999</t>
+  </si>
+  <si>
+    <t>319969700</t>
+  </si>
+  <si>
+    <t>321901834</t>
+  </si>
+  <si>
+    <t>321906265</t>
+  </si>
+  <si>
+    <t>321907954</t>
+  </si>
+  <si>
+    <t>321909303</t>
+  </si>
+  <si>
+    <t>321910639</t>
+  </si>
+  <si>
+    <t>321911948</t>
+  </si>
+  <si>
+    <t>321913213</t>
+  </si>
+  <si>
+    <t>321914611</t>
+  </si>
+  <si>
+    <t>321915954</t>
+  </si>
+  <si>
+    <t>321917580</t>
+  </si>
+  <si>
+    <t>322016515</t>
+  </si>
+  <si>
+    <t>322020858</t>
+  </si>
+  <si>
+    <t>322022575</t>
+  </si>
+  <si>
+    <t>322024076</t>
+  </si>
+  <si>
+    <t>322025477</t>
+  </si>
+  <si>
+    <t>322027108</t>
+  </si>
+  <si>
+    <t>322029025</t>
+  </si>
+  <si>
+    <t>322030379</t>
+  </si>
+  <si>
+    <t>322031972</t>
+  </si>
+  <si>
+    <t>322033640</t>
+  </si>
+  <si>
+    <t>322079297</t>
+  </si>
+  <si>
+    <t>322083123</t>
+  </si>
+  <si>
+    <t>322084744</t>
+  </si>
+  <si>
+    <t>322086126</t>
+  </si>
+  <si>
+    <t>322087488</t>
+  </si>
+  <si>
+    <t>322088795</t>
+  </si>
+  <si>
+    <t>322090563</t>
+  </si>
+  <si>
+    <t>322091908</t>
+  </si>
+  <si>
+    <t>322093288</t>
+  </si>
+  <si>
+    <t>322094971</t>
+  </si>
+  <si>
+    <t>322254760</t>
+  </si>
+  <si>
+    <t>322259037</t>
+  </si>
+  <si>
+    <t>322260513</t>
+  </si>
+  <si>
+    <t>322261913</t>
+  </si>
+  <si>
+    <t>322263303</t>
+  </si>
+  <si>
+    <t>322264935</t>
+  </si>
+  <si>
+    <t>322266562</t>
+  </si>
+  <si>
+    <t>322267957</t>
+  </si>
+  <si>
+    <t>322269653</t>
+  </si>
+  <si>
+    <t>322271360</t>
+  </si>
+  <si>
+    <t>322322799</t>
+  </si>
+  <si>
+    <t>322326354</t>
+  </si>
+  <si>
+    <t>322328143</t>
+  </si>
+  <si>
+    <t>322329979</t>
+  </si>
+  <si>
+    <t>322331423</t>
+  </si>
+  <si>
+    <t>322333176</t>
+  </si>
+  <si>
+    <t>322555106</t>
+  </si>
+  <si>
+    <t>322559616</t>
+  </si>
+  <si>
+    <t>322561442</t>
+  </si>
+  <si>
+    <t>322563252</t>
+  </si>
+  <si>
+    <t>322565348</t>
+  </si>
+  <si>
+    <t>322865842</t>
+  </si>
+  <si>
+    <t>322876153</t>
+  </si>
+  <si>
+    <t>322877535</t>
+  </si>
+  <si>
+    <t>322878597</t>
+  </si>
+  <si>
+    <t>322880050</t>
+  </si>
+  <si>
+    <t>322880958</t>
+  </si>
+  <si>
+    <t>322882330</t>
+  </si>
+  <si>
+    <t>322883220</t>
+  </si>
+  <si>
+    <t>322884594</t>
+  </si>
+  <si>
+    <t>322885891</t>
+  </si>
+  <si>
+    <t>322887208</t>
+  </si>
+  <si>
+    <t>322888502</t>
+  </si>
+  <si>
+    <t>322889711</t>
+  </si>
+  <si>
+    <t>322890849</t>
+  </si>
+  <si>
+    <t>322891971</t>
+  </si>
+  <si>
+    <t>322893017</t>
+  </si>
+  <si>
+    <t>322894625</t>
+  </si>
+  <si>
+    <t>322895690</t>
+  </si>
+  <si>
+    <t>322897028</t>
+  </si>
+  <si>
+    <t>322898132</t>
+  </si>
+  <si>
+    <t>322899105</t>
+  </si>
+  <si>
+    <t>322900773</t>
+  </si>
+  <si>
+    <t>322901930</t>
+  </si>
+  <si>
+    <t>322903103</t>
+  </si>
+  <si>
+    <t>322904269</t>
+  </si>
+  <si>
+    <t>322905424</t>
+  </si>
+  <si>
+    <t>322906665</t>
+  </si>
+  <si>
+    <t>322908008</t>
+  </si>
+  <si>
+    <t>322909485</t>
+  </si>
+  <si>
+    <t>322910729</t>
+  </si>
+  <si>
+    <t>322912370</t>
+  </si>
+  <si>
+    <t>322913653</t>
+  </si>
+  <si>
+    <t>322914870</t>
+  </si>
+  <si>
+    <t>322916073</t>
+  </si>
+  <si>
+    <t>322917357</t>
+  </si>
+  <si>
+    <t>322918839</t>
+  </si>
+  <si>
+    <t>322920472</t>
+  </si>
+  <si>
+    <t>322922066</t>
+  </si>
+  <si>
+    <t>322923668</t>
+  </si>
+  <si>
+    <t>322925344</t>
+  </si>
+  <si>
+    <t>322926933</t>
+  </si>
+  <si>
+    <t>322928273</t>
+  </si>
+  <si>
+    <t>322929853</t>
+  </si>
+  <si>
+    <t>322931224</t>
+  </si>
+  <si>
+    <t>322932574</t>
+  </si>
+  <si>
+    <t>322933997</t>
+  </si>
+  <si>
+    <t>322935411</t>
+  </si>
+  <si>
+    <t>322936890</t>
+  </si>
+  <si>
+    <t>322938513</t>
+  </si>
+  <si>
+    <t>322939950</t>
+  </si>
+  <si>
+    <t>322941506</t>
+  </si>
+  <si>
+    <t>322943351</t>
+  </si>
+  <si>
+    <t>322944861</t>
+  </si>
+  <si>
+    <t>322957356</t>
+  </si>
+  <si>
+    <t>323164690</t>
+  </si>
+  <si>
+    <t>323168213</t>
+  </si>
+  <si>
+    <t>323170782</t>
+  </si>
+  <si>
+    <t>323173206</t>
+  </si>
+  <si>
+    <t>323175580</t>
+  </si>
+  <si>
+    <t>323177821</t>
+  </si>
+  <si>
+    <t>323180230</t>
+  </si>
+  <si>
+    <t>323182606</t>
+  </si>
+  <si>
+    <t>325193106</t>
+  </si>
+  <si>
+    <t>325270400</t>
+  </si>
+  <si>
+    <t>325794879</t>
+  </si>
+  <si>
+    <t>325820735</t>
+  </si>
+  <si>
+    <t>325938721</t>
+  </si>
+  <si>
+    <t>326498072</t>
+  </si>
+  <si>
+    <t>326532451</t>
+  </si>
+  <si>
+    <t>326676058</t>
+  </si>
+  <si>
+    <t>327519443</t>
+  </si>
+  <si>
+    <t>327575926</t>
+  </si>
+  <si>
+    <t>327813541</t>
+  </si>
+  <si>
+    <t>327900068</t>
+  </si>
+  <si>
+    <t>327997382</t>
+  </si>
+  <si>
+    <t>328340119</t>
+  </si>
+  <si>
+    <t>328350177</t>
+  </si>
+  <si>
+    <t>328360279</t>
+  </si>
+  <si>
+    <t>328364098</t>
+  </si>
+  <si>
+    <t>328367930</t>
+  </si>
+  <si>
+    <t>328371102</t>
+  </si>
+  <si>
+    <t>328374615</t>
+  </si>
+  <si>
+    <t>328486671</t>
+  </si>
+  <si>
+    <t>328493947</t>
+  </si>
+  <si>
+    <t>328498311</t>
+  </si>
+  <si>
+    <t>328503727</t>
+  </si>
+  <si>
+    <t>328509526</t>
+  </si>
+  <si>
+    <t>328514380</t>
+  </si>
+  <si>
+    <t>328518040</t>
+  </si>
+  <si>
+    <t>328525833</t>
+  </si>
+  <si>
+    <t>329429965</t>
+  </si>
+  <si>
+    <t>329439094</t>
+  </si>
+  <si>
+    <t>329457788</t>
+  </si>
+  <si>
+    <t>329475579</t>
+  </si>
+  <si>
+    <t>329488547</t>
+  </si>
+  <si>
+    <t>329500413</t>
+  </si>
+  <si>
+    <t>329507501</t>
+  </si>
+  <si>
+    <t>329513339</t>
+  </si>
+  <si>
+    <t>329520548</t>
+  </si>
+  <si>
+    <t>329526071</t>
+  </si>
+  <si>
+    <t>329739433</t>
+  </si>
+  <si>
+    <t>329746597</t>
+  </si>
+  <si>
+    <t>329753871</t>
+  </si>
+  <si>
+    <t>329761494</t>
+  </si>
+  <si>
+    <t>329766576</t>
+  </si>
+  <si>
+    <t>329776899</t>
+  </si>
+  <si>
+    <t>329781389</t>
+  </si>
+  <si>
+    <t>329788507</t>
+  </si>
+  <si>
+    <t>329938805</t>
+  </si>
+  <si>
+    <t>329963582</t>
+  </si>
+  <si>
+    <t>329977689</t>
+  </si>
+  <si>
+    <t>330939366</t>
+  </si>
+  <si>
+    <t>330946214</t>
+  </si>
+  <si>
+    <t>330953049</t>
+  </si>
+  <si>
+    <t>331391466</t>
+  </si>
+  <si>
+    <t>331402205</t>
+  </si>
+  <si>
+    <t>331406512</t>
+  </si>
+  <si>
+    <t>332521421</t>
+  </si>
+  <si>
+    <t>332530215</t>
+  </si>
+  <si>
+    <t>332540377</t>
+  </si>
+  <si>
+    <t>332910578</t>
+  </si>
+  <si>
+    <t>332916301</t>
+  </si>
+  <si>
+    <t>332924991</t>
+  </si>
+  <si>
+    <t>334433539</t>
+  </si>
+  <si>
+    <t>334446674</t>
+  </si>
+  <si>
+    <t>334893626</t>
+  </si>
+  <si>
+    <t>334904885</t>
+  </si>
+  <si>
+    <t>334984703</t>
+  </si>
+  <si>
+    <t>334991957</t>
+  </si>
+  <si>
+    <t>335627853</t>
+  </si>
+  <si>
+    <t>335644135</t>
+  </si>
+  <si>
+    <t>336649496</t>
+  </si>
+  <si>
+    <t>336692438</t>
+  </si>
+  <si>
+    <t>336705642</t>
+  </si>
+  <si>
+    <t>336714938</t>
+  </si>
+  <si>
+    <t>336839903</t>
+  </si>
+  <si>
+    <t>336848437</t>
+  </si>
+  <si>
+    <t>337247288</t>
+  </si>
+  <si>
+    <t>337254267</t>
+  </si>
+  <si>
+    <t>337296573</t>
+  </si>
+  <si>
+    <t>337312829</t>
+  </si>
+  <si>
+    <t>338781017</t>
+  </si>
+  <si>
+    <t>338822901</t>
+  </si>
+  <si>
+    <t>339108152</t>
+  </si>
+  <si>
+    <t>339116380</t>
+  </si>
+  <si>
+    <t>339699671</t>
+  </si>
+  <si>
+    <t>339712335</t>
+  </si>
+  <si>
+    <t>340164272</t>
+  </si>
+  <si>
+    <t>340173436</t>
+  </si>
+  <si>
+    <t>340378566</t>
+  </si>
+  <si>
+    <t>340387414</t>
+  </si>
+  <si>
+    <t>340713309</t>
+  </si>
+  <si>
+    <t>340722214</t>
+  </si>
+  <si>
+    <t>344850602</t>
+  </si>
+  <si>
+    <t>344855565</t>
+  </si>
+  <si>
+    <t>344859612</t>
+  </si>
+  <si>
+    <t>344863679</t>
+  </si>
+  <si>
+    <t>344867458</t>
+  </si>
+  <si>
+    <t>344873538</t>
+  </si>
+  <si>
+    <t>344877175</t>
+  </si>
+  <si>
+    <t>344881104</t>
+  </si>
+  <si>
+    <t>345068300</t>
+  </si>
+  <si>
+    <t>345072996</t>
+  </si>
+  <si>
+    <t>345076848</t>
+  </si>
+  <si>
+    <t>345081396</t>
+  </si>
+  <si>
+    <t>345084898</t>
+  </si>
+  <si>
+    <t>345088761</t>
+  </si>
+  <si>
+    <t>345092361</t>
+  </si>
+  <si>
+    <t>345094894</t>
+  </si>
+  <si>
+    <t>345630527</t>
+  </si>
+  <si>
+    <t>345636097</t>
+  </si>
+  <si>
+    <t>345639715</t>
+  </si>
+  <si>
+    <t>345643614</t>
+  </si>
+  <si>
+    <t>345647351</t>
+  </si>
+  <si>
+    <t>345651006</t>
+  </si>
+  <si>
+    <t>345654342</t>
+  </si>
+  <si>
+    <t>345658231</t>
+  </si>
+  <si>
+    <t>345734953</t>
+  </si>
+  <si>
+    <t>345740254</t>
+  </si>
+  <si>
+    <t>345742683</t>
+  </si>
+  <si>
+    <t>346131799</t>
+  </si>
+  <si>
+    <t>346137103</t>
+  </si>
+  <si>
+    <t>346139849</t>
+  </si>
+  <si>
+    <t>346636988</t>
+  </si>
+  <si>
+    <t>346642293</t>
+  </si>
+  <si>
+    <t>346644521</t>
+  </si>
+  <si>
+    <t>346906459</t>
+  </si>
+  <si>
+    <t>346912114</t>
+  </si>
+  <si>
+    <t>346915115</t>
+  </si>
+  <si>
+    <t>347009361</t>
+  </si>
+  <si>
+    <t>347014432</t>
+  </si>
+  <si>
+    <t>347016954</t>
+  </si>
+  <si>
+    <t>347057639</t>
+  </si>
+  <si>
+    <t>347062474</t>
+  </si>
+  <si>
+    <t>347065042</t>
+  </si>
+  <si>
+    <t>347165686</t>
+  </si>
+  <si>
+    <t>347168743</t>
+  </si>
+  <si>
+    <t>347283791</t>
+  </si>
+  <si>
+    <t>347287286</t>
+  </si>
+  <si>
+    <t>347470354</t>
+  </si>
+  <si>
+    <t>347478804</t>
+  </si>
+  <si>
+    <t>347479889</t>
+  </si>
+  <si>
+    <t>347481448</t>
+  </si>
+  <si>
+    <t>347482998</t>
+  </si>
+  <si>
+    <t>347484033</t>
+  </si>
+  <si>
+    <t>347485394</t>
+  </si>
+  <si>
+    <t>347486403</t>
+  </si>
+  <si>
+    <t>347488052</t>
+  </si>
+  <si>
+    <t>347489525</t>
+  </si>
+  <si>
+    <t>347491050</t>
+  </si>
+  <si>
+    <t>347492341</t>
+  </si>
+  <si>
+    <t>347493650</t>
+  </si>
+  <si>
+    <t>347495274</t>
+  </si>
+  <si>
+    <t>347496646</t>
+  </si>
+  <si>
+    <t>347497833</t>
+  </si>
+  <si>
+    <t>347499534</t>
+  </si>
+  <si>
+    <t>347501610</t>
+  </si>
+  <si>
+    <t>347503395</t>
+  </si>
+  <si>
+    <t>347504746</t>
+  </si>
+  <si>
+    <t>347506569</t>
+  </si>
+  <si>
+    <t>347508023</t>
+  </si>
+  <si>
+    <t>347510160</t>
+  </si>
+  <si>
+    <t>347511576</t>
+  </si>
+  <si>
+    <t>347512863</t>
+  </si>
+  <si>
+    <t>347514238</t>
+  </si>
+  <si>
+    <t>347515480</t>
+  </si>
+  <si>
+    <t>347517316</t>
+  </si>
+  <si>
+    <t>347519457</t>
+  </si>
+  <si>
+    <t>347521134</t>
+  </si>
+  <si>
+    <t>347523067</t>
+  </si>
+  <si>
+    <t>347525065</t>
+  </si>
+  <si>
+    <t>347526502</t>
+  </si>
+  <si>
+    <t>347528077</t>
+  </si>
+  <si>
+    <t>347529597</t>
+  </si>
+  <si>
+    <t>347531034</t>
+  </si>
+  <si>
+    <t>347533070</t>
+  </si>
+  <si>
+    <t>347535184</t>
+  </si>
+  <si>
+    <t>347536696</t>
+  </si>
+  <si>
+    <t>347538445</t>
+  </si>
+  <si>
+    <t>347540386</t>
+  </si>
+  <si>
+    <t>347542062</t>
+  </si>
+  <si>
+    <t>347544052</t>
+  </si>
+  <si>
+    <t>347546042</t>
+  </si>
+  <si>
+    <t>347547832</t>
+  </si>
+  <si>
+    <t>347549496</t>
+  </si>
+  <si>
+    <t>347551489</t>
+  </si>
+  <si>
+    <t>347553720</t>
+  </si>
+  <si>
+    <t>347555488</t>
+  </si>
+  <si>
+    <t>347557520</t>
+  </si>
+  <si>
+    <t>347559818</t>
+  </si>
+  <si>
+    <t>347561370</t>
+  </si>
+  <si>
+    <t>347563331</t>
+  </si>
+  <si>
+    <t>347566013</t>
+  </si>
+  <si>
+    <t>347568552</t>
+  </si>
+  <si>
+    <t>347574637</t>
+  </si>
+  <si>
+    <t>347577822</t>
+  </si>
+  <si>
+    <t>347579963</t>
+  </si>
+  <si>
+    <t>347583358</t>
+  </si>
+  <si>
+    <t>347585540</t>
+  </si>
+  <si>
+    <t>347587683</t>
+  </si>
+  <si>
+    <t>347590574</t>
+  </si>
+  <si>
+    <t>347595100</t>
+  </si>
+  <si>
+    <t>347598334</t>
+  </si>
+  <si>
+    <t>347602018</t>
+  </si>
+  <si>
+    <t>347604958</t>
+  </si>
+  <si>
+    <t>347608477</t>
+  </si>
+  <si>
+    <t>347611850</t>
+  </si>
+  <si>
+    <t>347615034</t>
   </si>
 </sst>
 </file>
@@ -4029,7 +5625,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>1031</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4269,7 +5865,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>1032</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4305,7 +5901,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>1033</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4341,7 +5937,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>1034</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4377,7 +5973,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>1035</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4413,7 +6009,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>1036</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4447,7 +6043,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>1037</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4481,7 +6077,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>1038</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,7 +6113,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>1039</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4553,7 +6149,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>1040</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4589,7 +6185,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>1041</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4625,7 +6221,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>1042</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4661,7 +6257,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>1043</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4697,7 +6293,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>1044</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4733,7 +6329,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>1045</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4769,7 +6365,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>1046</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4805,7 +6401,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>1047</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4841,7 +6437,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>1048</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4875,7 +6471,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>1049</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4909,7 +6505,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>1050</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4945,7 +6541,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>1051</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4981,7 +6577,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>1052</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5017,7 +6613,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>1053</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5053,7 +6649,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>1054</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5089,7 +6685,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>1055</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5125,7 +6721,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>1056</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5159,7 +6755,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>1057</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5195,7 +6791,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>1058</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5231,7 +6827,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>1059</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,7 +6863,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>1060</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5303,7 +6899,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>1061</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5339,7 +6935,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>1062</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5375,7 +6971,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>1063</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5411,7 +7007,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>1064</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5445,7 +7041,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>1065</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5479,7 +7075,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>1066</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5515,7 +7111,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>1067</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5551,7 +7147,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>1068</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5587,7 +7183,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>1069</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5623,7 +7219,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>1070</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5659,7 +7255,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>1071</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5695,7 +7291,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>1072</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5731,7 +7327,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>1074</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5767,7 +7363,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>1075</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5803,7 +7399,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>1076</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5839,7 +7435,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>1073</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5875,7 +7471,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>1077</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5911,7 +7507,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>1078</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5947,7 +7543,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>1079</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5983,7 +7579,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>1080</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6017,7 +7613,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>1081</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6053,7 +7649,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>1082</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6085,7 +7681,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>1083</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6121,7 +7717,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>1091</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6153,7 +7749,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>1092</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6185,7 +7781,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>1093</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6217,7 +7813,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>1094</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6249,7 +7845,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>1095</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6281,7 +7877,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>1096</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6313,7 +7909,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>1097</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6345,7 +7941,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>1098</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6379,7 +7975,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>1084</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6415,7 +8011,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>1018</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6449,7 +8045,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>1019</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6483,7 +8079,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>1085</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6517,7 +8113,7 @@
         <v>171</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>1086</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6551,7 +8147,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>1087</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6583,7 +8179,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>1088</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6615,7 +8211,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>1089</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6647,7 +8243,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>1090</v>
+        <v>1622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore - ChainTest Report(Extent Report)Email send configuration modified in the yaml file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="1631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="1769">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -4994,6 +4994,420 @@
   </si>
   <si>
     <t>347615034</t>
+  </si>
+  <si>
+    <t>353191492</t>
+  </si>
+  <si>
+    <t>353221200</t>
+  </si>
+  <si>
+    <t>353222546</t>
+  </si>
+  <si>
+    <t>353223838</t>
+  </si>
+  <si>
+    <t>353225582</t>
+  </si>
+  <si>
+    <t>353226748</t>
+  </si>
+  <si>
+    <t>353228348</t>
+  </si>
+  <si>
+    <t>353229579</t>
+  </si>
+  <si>
+    <t>353231121</t>
+  </si>
+  <si>
+    <t>353232233</t>
+  </si>
+  <si>
+    <t>353233669</t>
+  </si>
+  <si>
+    <t>353234667</t>
+  </si>
+  <si>
+    <t>353235763</t>
+  </si>
+  <si>
+    <t>353236821</t>
+  </si>
+  <si>
+    <t>353238066</t>
+  </si>
+  <si>
+    <t>353239114</t>
+  </si>
+  <si>
+    <t>353240854</t>
+  </si>
+  <si>
+    <t>353242322</t>
+  </si>
+  <si>
+    <t>353244356</t>
+  </si>
+  <si>
+    <t>353245785</t>
+  </si>
+  <si>
+    <t>353247514</t>
+  </si>
+  <si>
+    <t>353249469</t>
+  </si>
+  <si>
+    <t>353251326</t>
+  </si>
+  <si>
+    <t>353252895</t>
+  </si>
+  <si>
+    <t>353254442</t>
+  </si>
+  <si>
+    <t>353256301</t>
+  </si>
+  <si>
+    <t>353258115</t>
+  </si>
+  <si>
+    <t>353259624</t>
+  </si>
+  <si>
+    <t>353261550</t>
+  </si>
+  <si>
+    <t>353263164</t>
+  </si>
+  <si>
+    <t>353265401</t>
+  </si>
+  <si>
+    <t>353267345</t>
+  </si>
+  <si>
+    <t>353268719</t>
+  </si>
+  <si>
+    <t>353270030</t>
+  </si>
+  <si>
+    <t>353271413</t>
+  </si>
+  <si>
+    <t>353273074</t>
+  </si>
+  <si>
+    <t>353274877</t>
+  </si>
+  <si>
+    <t>353276285</t>
+  </si>
+  <si>
+    <t>353277634</t>
+  </si>
+  <si>
+    <t>353279485</t>
+  </si>
+  <si>
+    <t>353280909</t>
+  </si>
+  <si>
+    <t>353282775</t>
+  </si>
+  <si>
+    <t>353284513</t>
+  </si>
+  <si>
+    <t>353286132</t>
+  </si>
+  <si>
+    <t>353287739</t>
+  </si>
+  <si>
+    <t>353289620</t>
+  </si>
+  <si>
+    <t>353291076</t>
+  </si>
+  <si>
+    <t>353292755</t>
+  </si>
+  <si>
+    <t>353294515</t>
+  </si>
+  <si>
+    <t>353296413</t>
+  </si>
+  <si>
+    <t>353298823</t>
+  </si>
+  <si>
+    <t>353301454</t>
+  </si>
+  <si>
+    <t>353303927</t>
+  </si>
+  <si>
+    <t>353306741</t>
+  </si>
+  <si>
+    <t>353309805</t>
+  </si>
+  <si>
+    <t>353315527</t>
+  </si>
+  <si>
+    <t>353319006</t>
+  </si>
+  <si>
+    <t>353321244</t>
+  </si>
+  <si>
+    <t>353325988</t>
+  </si>
+  <si>
+    <t>353328861</t>
+  </si>
+  <si>
+    <t>353331201</t>
+  </si>
+  <si>
+    <t>353334343</t>
+  </si>
+  <si>
+    <t>353337746</t>
+  </si>
+  <si>
+    <t>353341633</t>
+  </si>
+  <si>
+    <t>353346029</t>
+  </si>
+  <si>
+    <t>353350409</t>
+  </si>
+  <si>
+    <t>353356101</t>
+  </si>
+  <si>
+    <t>353360603</t>
+  </si>
+  <si>
+    <t>353365481</t>
+  </si>
+  <si>
+    <t>371631627</t>
+  </si>
+  <si>
+    <t>371640818</t>
+  </si>
+  <si>
+    <t>371642025</t>
+  </si>
+  <si>
+    <t>371644202</t>
+  </si>
+  <si>
+    <t>371645828</t>
+  </si>
+  <si>
+    <t>371647623</t>
+  </si>
+  <si>
+    <t>371649750</t>
+  </si>
+  <si>
+    <t>371651581</t>
+  </si>
+  <si>
+    <t>371653991</t>
+  </si>
+  <si>
+    <t>371656514</t>
+  </si>
+  <si>
+    <t>371658985</t>
+  </si>
+  <si>
+    <t>371661119</t>
+  </si>
+  <si>
+    <t>371663195</t>
+  </si>
+  <si>
+    <t>371665433</t>
+  </si>
+  <si>
+    <t>371667826</t>
+  </si>
+  <si>
+    <t>371670152</t>
+  </si>
+  <si>
+    <t>371672413</t>
+  </si>
+  <si>
+    <t>371674533</t>
+  </si>
+  <si>
+    <t>371676873</t>
+  </si>
+  <si>
+    <t>371678789</t>
+  </si>
+  <si>
+    <t>371681038</t>
+  </si>
+  <si>
+    <t>371682883</t>
+  </si>
+  <si>
+    <t>371685346</t>
+  </si>
+  <si>
+    <t>371687707</t>
+  </si>
+  <si>
+    <t>371690251</t>
+  </si>
+  <si>
+    <t>371692692</t>
+  </si>
+  <si>
+    <t>371695211</t>
+  </si>
+  <si>
+    <t>371697568</t>
+  </si>
+  <si>
+    <t>371700383</t>
+  </si>
+  <si>
+    <t>371703200</t>
+  </si>
+  <si>
+    <t>371706061</t>
+  </si>
+  <si>
+    <t>371708817</t>
+  </si>
+  <si>
+    <t>371711252</t>
+  </si>
+  <si>
+    <t>371713780</t>
+  </si>
+  <si>
+    <t>371716517</t>
+  </si>
+  <si>
+    <t>371719131</t>
+  </si>
+  <si>
+    <t>371722204</t>
+  </si>
+  <si>
+    <t>371725446</t>
+  </si>
+  <si>
+    <t>371728063</t>
+  </si>
+  <si>
+    <t>371731331</t>
+  </si>
+  <si>
+    <t>371734385</t>
+  </si>
+  <si>
+    <t>371737330</t>
+  </si>
+  <si>
+    <t>371739943</t>
+  </si>
+  <si>
+    <t>371742861</t>
+  </si>
+  <si>
+    <t>371745215</t>
+  </si>
+  <si>
+    <t>371747658</t>
+  </si>
+  <si>
+    <t>371750418</t>
+  </si>
+  <si>
+    <t>371753544</t>
+  </si>
+  <si>
+    <t>371756738</t>
+  </si>
+  <si>
+    <t>371759777</t>
+  </si>
+  <si>
+    <t>371763133</t>
+  </si>
+  <si>
+    <t>371766891</t>
+  </si>
+  <si>
+    <t>371770649</t>
+  </si>
+  <si>
+    <t>371775903</t>
+  </si>
+  <si>
+    <t>371780971</t>
+  </si>
+  <si>
+    <t>371789910</t>
+  </si>
+  <si>
+    <t>371795751</t>
+  </si>
+  <si>
+    <t>371799769</t>
+  </si>
+  <si>
+    <t>371805370</t>
+  </si>
+  <si>
+    <t>371809330</t>
+  </si>
+  <si>
+    <t>371813977</t>
+  </si>
+  <si>
+    <t>371818172</t>
+  </si>
+  <si>
+    <t>371822730</t>
+  </si>
+  <si>
+    <t>371827373</t>
+  </si>
+  <si>
+    <t>371832135</t>
+  </si>
+  <si>
+    <t>371836971</t>
+  </si>
+  <si>
+    <t>371842097</t>
+  </si>
+  <si>
+    <t>371846845</t>
+  </si>
+  <si>
+    <t>371851201</t>
   </si>
 </sst>
 </file>
@@ -5625,7 +6039,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>1562</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5865,7 +6279,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>1563</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5901,7 +6315,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>1564</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5937,7 +6351,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>1565</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5973,7 +6387,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>1566</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6009,7 +6423,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>1567</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6043,7 +6457,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>1568</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6077,7 +6491,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>1569</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6113,7 +6527,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>1570</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6149,7 +6563,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>1571</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6185,7 +6599,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>1572</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6221,7 +6635,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>1573</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6257,7 +6671,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>1574</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6293,7 +6707,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>1575</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6329,7 +6743,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>1576</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6365,7 +6779,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>1577</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6401,7 +6815,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>1578</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6437,7 +6851,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>1579</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,7 +6885,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>1580</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6505,7 +6919,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>1581</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6541,7 +6955,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>1582</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6577,7 +6991,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>1583</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6613,7 +7027,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>1584</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6649,7 +7063,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>1585</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6685,7 +7099,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>1586</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6721,7 +7135,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>1587</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6755,7 +7169,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>1588</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6791,7 +7205,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>1589</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6827,7 +7241,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>1590</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6863,7 +7277,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>1591</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6899,7 +7313,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>1592</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6935,7 +7349,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>1593</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6971,7 +7385,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>1594</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7007,7 +7421,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>1595</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7041,7 +7455,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>1596</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7075,7 +7489,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>1597</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7111,7 +7525,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>1598</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7147,7 +7561,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>1599</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7183,7 +7597,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>1600</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7219,7 +7633,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>1601</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7255,7 +7669,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>1602</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7291,7 +7705,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>1603</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7327,7 +7741,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>1605</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7363,7 +7777,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>1606</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7399,7 +7813,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>1607</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7435,7 +7849,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>1604</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7471,7 +7885,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>1608</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7507,7 +7921,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>1609</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7543,7 +7957,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>1610</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7579,7 +7993,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>1611</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7613,7 +8027,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>1612</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7649,7 +8063,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>1613</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7681,7 +8095,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>1614</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7717,7 +8131,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>1623</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7749,7 +8163,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>1624</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7781,7 +8195,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>1625</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7813,7 +8227,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>1626</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7845,7 +8259,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>1627</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7877,7 +8291,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>1628</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7909,7 +8323,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>1629</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7941,7 +8355,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>1630</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7975,7 +8389,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>1615</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8011,7 +8425,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>1618</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8045,7 +8459,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>1619</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8079,7 +8493,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>1616</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8147,7 +8561,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>1617</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8179,7 +8593,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>1620</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8211,7 +8625,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>1621</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8243,7 +8657,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>1622</v>
+        <v>1760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore - final commit README.md doc updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="1769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2331" uniqueCount="1842">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -5408,6 +5408,225 @@
   </si>
   <si>
     <t>371851201</t>
+  </si>
+  <si>
+    <t>408963178</t>
+  </si>
+  <si>
+    <t>409008376</t>
+  </si>
+  <si>
+    <t>409011021</t>
+  </si>
+  <si>
+    <t>409012047</t>
+  </si>
+  <si>
+    <t>409014214</t>
+  </si>
+  <si>
+    <t>409015423</t>
+  </si>
+  <si>
+    <t>409016976</t>
+  </si>
+  <si>
+    <t>409018259</t>
+  </si>
+  <si>
+    <t>409020258</t>
+  </si>
+  <si>
+    <t>409021501</t>
+  </si>
+  <si>
+    <t>409023094</t>
+  </si>
+  <si>
+    <t>409024368</t>
+  </si>
+  <si>
+    <t>409025818</t>
+  </si>
+  <si>
+    <t>409027452</t>
+  </si>
+  <si>
+    <t>409029432</t>
+  </si>
+  <si>
+    <t>409030837</t>
+  </si>
+  <si>
+    <t>409032517</t>
+  </si>
+  <si>
+    <t>409033933</t>
+  </si>
+  <si>
+    <t>409035690</t>
+  </si>
+  <si>
+    <t>409037217</t>
+  </si>
+  <si>
+    <t>409039250</t>
+  </si>
+  <si>
+    <t>409040907</t>
+  </si>
+  <si>
+    <t>409043004</t>
+  </si>
+  <si>
+    <t>409045034</t>
+  </si>
+  <si>
+    <t>409046766</t>
+  </si>
+  <si>
+    <t>409048500</t>
+  </si>
+  <si>
+    <t>409050292</t>
+  </si>
+  <si>
+    <t>409052175</t>
+  </si>
+  <si>
+    <t>409054094</t>
+  </si>
+  <si>
+    <t>409055907</t>
+  </si>
+  <si>
+    <t>409058006</t>
+  </si>
+  <si>
+    <t>409060455</t>
+  </si>
+  <si>
+    <t>409062319</t>
+  </si>
+  <si>
+    <t>409064320</t>
+  </si>
+  <si>
+    <t>409066313</t>
+  </si>
+  <si>
+    <t>409067961</t>
+  </si>
+  <si>
+    <t>409070099</t>
+  </si>
+  <si>
+    <t>409072270</t>
+  </si>
+  <si>
+    <t>409074235</t>
+  </si>
+  <si>
+    <t>409076459</t>
+  </si>
+  <si>
+    <t>409078642</t>
+  </si>
+  <si>
+    <t>409080654</t>
+  </si>
+  <si>
+    <t>409083072</t>
+  </si>
+  <si>
+    <t>409085076</t>
+  </si>
+  <si>
+    <t>409087121</t>
+  </si>
+  <si>
+    <t>409089369</t>
+  </si>
+  <si>
+    <t>409091494</t>
+  </si>
+  <si>
+    <t>409093532</t>
+  </si>
+  <si>
+    <t>409095698</t>
+  </si>
+  <si>
+    <t>409097485</t>
+  </si>
+  <si>
+    <t>409099469</t>
+  </si>
+  <si>
+    <t>409101472</t>
+  </si>
+  <si>
+    <t>409103798</t>
+  </si>
+  <si>
+    <t>409106861</t>
+  </si>
+  <si>
+    <t>409109426</t>
+  </si>
+  <si>
+    <t>409114188</t>
+  </si>
+  <si>
+    <t>409116942</t>
+  </si>
+  <si>
+    <t>409119246</t>
+  </si>
+  <si>
+    <t>409122265</t>
+  </si>
+  <si>
+    <t>409124578</t>
+  </si>
+  <si>
+    <t>409126842</t>
+  </si>
+  <si>
+    <t>409129532</t>
+  </si>
+  <si>
+    <t>409132641</t>
+  </si>
+  <si>
+    <t>409135640</t>
+  </si>
+  <si>
+    <t>409139000</t>
+  </si>
+  <si>
+    <t>409141738</t>
+  </si>
+  <si>
+    <t>409144907</t>
+  </si>
+  <si>
+    <t>409147968</t>
+  </si>
+  <si>
+    <t>409151105</t>
+  </si>
+  <si>
+    <t>416793334</t>
+  </si>
+  <si>
+    <t>417009033</t>
+  </si>
+  <si>
+    <t>417653379</t>
+  </si>
+  <si>
+    <t>417718611</t>
   </si>
 </sst>
 </file>
@@ -6039,7 +6258,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>1700</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6279,7 +6498,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>1701</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6315,7 +6534,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>1702</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6351,7 +6570,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>1703</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6387,7 +6606,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>1704</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6423,7 +6642,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>1705</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6457,7 +6676,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>1706</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6491,7 +6710,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>1707</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6527,7 +6746,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>1708</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6563,7 +6782,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>1709</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6599,7 +6818,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>1710</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6635,7 +6854,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>1711</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6671,7 +6890,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>1712</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6707,7 +6926,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>1713</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6743,7 +6962,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>1714</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6779,7 +6998,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>1715</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6815,7 +7034,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>1716</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6851,7 +7070,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>1717</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6885,7 +7104,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>1718</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6919,7 +7138,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>1719</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6955,7 +7174,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>1720</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6991,7 +7210,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>1721</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7027,7 +7246,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>1722</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7063,7 +7282,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>1723</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7099,7 +7318,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>1724</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7135,7 +7354,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>1725</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7169,7 +7388,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>1726</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7205,7 +7424,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>1727</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7241,7 +7460,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>1728</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7277,7 +7496,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>1729</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7313,7 +7532,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>1730</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7349,7 +7568,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>1731</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7385,7 +7604,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>1732</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7421,7 +7640,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>1733</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7455,7 +7674,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>1734</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7489,7 +7708,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>1735</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7525,7 +7744,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>1736</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7561,7 +7780,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>1737</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7597,7 +7816,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>1738</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7633,7 +7852,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>1739</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7669,7 +7888,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>1740</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7705,7 +7924,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>1741</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7741,7 +7960,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>1743</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7777,7 +7996,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>1744</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7813,7 +8032,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>1745</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7849,7 +8068,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>1742</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7885,7 +8104,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>1746</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7921,7 +8140,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>1747</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7957,7 +8176,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>1748</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7993,7 +8212,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>1749</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8027,7 +8246,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>1750</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8063,7 +8282,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>1751</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8095,7 +8314,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>1752</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8131,7 +8350,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>1761</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8163,7 +8382,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>1762</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8195,7 +8414,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>1763</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8227,7 +8446,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>1764</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8259,7 +8478,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>1765</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8291,7 +8510,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>1766</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8323,7 +8542,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>1767</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8355,7 +8574,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>1768</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8389,7 +8608,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>1753</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8425,7 +8644,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>1756</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8459,7 +8678,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>1757</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8493,7 +8712,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>1754</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8561,7 +8780,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>1755</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8593,7 +8812,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>1758</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8625,7 +8844,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>1759</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8657,7 +8876,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>1760</v>
+        <v>1829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore - final commit warnings removed
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2331" uniqueCount="1842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="1980">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -5627,6 +5627,420 @@
   </si>
   <si>
     <t>417718611</t>
+  </si>
+  <si>
+    <t>418703599</t>
+  </si>
+  <si>
+    <t>418709970</t>
+  </si>
+  <si>
+    <t>418710812</t>
+  </si>
+  <si>
+    <t>418711609</t>
+  </si>
+  <si>
+    <t>418712674</t>
+  </si>
+  <si>
+    <t>418713447</t>
+  </si>
+  <si>
+    <t>418714270</t>
+  </si>
+  <si>
+    <t>418715101</t>
+  </si>
+  <si>
+    <t>418716187</t>
+  </si>
+  <si>
+    <t>418717046</t>
+  </si>
+  <si>
+    <t>418717922</t>
+  </si>
+  <si>
+    <t>418718796</t>
+  </si>
+  <si>
+    <t>418719682</t>
+  </si>
+  <si>
+    <t>418720582</t>
+  </si>
+  <si>
+    <t>418721455</t>
+  </si>
+  <si>
+    <t>418722378</t>
+  </si>
+  <si>
+    <t>418723632</t>
+  </si>
+  <si>
+    <t>418724600</t>
+  </si>
+  <si>
+    <t>418725846</t>
+  </si>
+  <si>
+    <t>418726813</t>
+  </si>
+  <si>
+    <t>418728068</t>
+  </si>
+  <si>
+    <t>418729074</t>
+  </si>
+  <si>
+    <t>418730347</t>
+  </si>
+  <si>
+    <t>418731392</t>
+  </si>
+  <si>
+    <t>418732463</t>
+  </si>
+  <si>
+    <t>418733547</t>
+  </si>
+  <si>
+    <t>418734651</t>
+  </si>
+  <si>
+    <t>418735720</t>
+  </si>
+  <si>
+    <t>418737081</t>
+  </si>
+  <si>
+    <t>418738206</t>
+  </si>
+  <si>
+    <t>418739597</t>
+  </si>
+  <si>
+    <t>418740760</t>
+  </si>
+  <si>
+    <t>418741935</t>
+  </si>
+  <si>
+    <t>418743095</t>
+  </si>
+  <si>
+    <t>418744313</t>
+  </si>
+  <si>
+    <t>418745502</t>
+  </si>
+  <si>
+    <t>418747032</t>
+  </si>
+  <si>
+    <t>418748273</t>
+  </si>
+  <si>
+    <t>418749553</t>
+  </si>
+  <si>
+    <t>418751072</t>
+  </si>
+  <si>
+    <t>418752338</t>
+  </si>
+  <si>
+    <t>418753671</t>
+  </si>
+  <si>
+    <t>418755067</t>
+  </si>
+  <si>
+    <t>418756422</t>
+  </si>
+  <si>
+    <t>418757758</t>
+  </si>
+  <si>
+    <t>418759202</t>
+  </si>
+  <si>
+    <t>418760692</t>
+  </si>
+  <si>
+    <t>418762079</t>
+  </si>
+  <si>
+    <t>418763469</t>
+  </si>
+  <si>
+    <t>418764873</t>
+  </si>
+  <si>
+    <t>418766515</t>
+  </si>
+  <si>
+    <t>418767954</t>
+  </si>
+  <si>
+    <t>418769675</t>
+  </si>
+  <si>
+    <t>418771658</t>
+  </si>
+  <si>
+    <t>418773777</t>
+  </si>
+  <si>
+    <t>418777629</t>
+  </si>
+  <si>
+    <t>418780015</t>
+  </si>
+  <si>
+    <t>418781704</t>
+  </si>
+  <si>
+    <t>418784171</t>
+  </si>
+  <si>
+    <t>418785905</t>
+  </si>
+  <si>
+    <t>418787662</t>
+  </si>
+  <si>
+    <t>418789613</t>
+  </si>
+  <si>
+    <t>418791877</t>
+  </si>
+  <si>
+    <t>418794178</t>
+  </si>
+  <si>
+    <t>418796853</t>
+  </si>
+  <si>
+    <t>418799125</t>
+  </si>
+  <si>
+    <t>418801673</t>
+  </si>
+  <si>
+    <t>418804067</t>
+  </si>
+  <si>
+    <t>418806391</t>
+  </si>
+  <si>
+    <t>435539446</t>
+  </si>
+  <si>
+    <t>435581115</t>
+  </si>
+  <si>
+    <t>435582373</t>
+  </si>
+  <si>
+    <t>435583270</t>
+  </si>
+  <si>
+    <t>435584363</t>
+  </si>
+  <si>
+    <t>435585128</t>
+  </si>
+  <si>
+    <t>435585990</t>
+  </si>
+  <si>
+    <t>435586801</t>
+  </si>
+  <si>
+    <t>435588067</t>
+  </si>
+  <si>
+    <t>435588934</t>
+  </si>
+  <si>
+    <t>435589824</t>
+  </si>
+  <si>
+    <t>435590690</t>
+  </si>
+  <si>
+    <t>435591605</t>
+  </si>
+  <si>
+    <t>435592556</t>
+  </si>
+  <si>
+    <t>435593516</t>
+  </si>
+  <si>
+    <t>435594726</t>
+  </si>
+  <si>
+    <t>435595955</t>
+  </si>
+  <si>
+    <t>435596957</t>
+  </si>
+  <si>
+    <t>435598243</t>
+  </si>
+  <si>
+    <t>435599209</t>
+  </si>
+  <si>
+    <t>435600456</t>
+  </si>
+  <si>
+    <t>435601477</t>
+  </si>
+  <si>
+    <t>435602784</t>
+  </si>
+  <si>
+    <t>435603859</t>
+  </si>
+  <si>
+    <t>435604972</t>
+  </si>
+  <si>
+    <t>435606106</t>
+  </si>
+  <si>
+    <t>435607379</t>
+  </si>
+  <si>
+    <t>435608579</t>
+  </si>
+  <si>
+    <t>435610016</t>
+  </si>
+  <si>
+    <t>435611190</t>
+  </si>
+  <si>
+    <t>435612584</t>
+  </si>
+  <si>
+    <t>435613878</t>
+  </si>
+  <si>
+    <t>435615083</t>
+  </si>
+  <si>
+    <t>435616293</t>
+  </si>
+  <si>
+    <t>435617520</t>
+  </si>
+  <si>
+    <t>435618767</t>
+  </si>
+  <si>
+    <t>435620253</t>
+  </si>
+  <si>
+    <t>435621519</t>
+  </si>
+  <si>
+    <t>435622801</t>
+  </si>
+  <si>
+    <t>435624516</t>
+  </si>
+  <si>
+    <t>435625915</t>
+  </si>
+  <si>
+    <t>435627213</t>
+  </si>
+  <si>
+    <t>435628683</t>
+  </si>
+  <si>
+    <t>435630576</t>
+  </si>
+  <si>
+    <t>435632100</t>
+  </si>
+  <si>
+    <t>435633504</t>
+  </si>
+  <si>
+    <t>435634950</t>
+  </si>
+  <si>
+    <t>435636415</t>
+  </si>
+  <si>
+    <t>435638081</t>
+  </si>
+  <si>
+    <t>435639590</t>
+  </si>
+  <si>
+    <t>435641363</t>
+  </si>
+  <si>
+    <t>435642845</t>
+  </si>
+  <si>
+    <t>435645310</t>
+  </si>
+  <si>
+    <t>435649070</t>
+  </si>
+  <si>
+    <t>435651776</t>
+  </si>
+  <si>
+    <t>435656441</t>
+  </si>
+  <si>
+    <t>435659968</t>
+  </si>
+  <si>
+    <t>435662333</t>
+  </si>
+  <si>
+    <t>435665971</t>
+  </si>
+  <si>
+    <t>435668629</t>
+  </si>
+  <si>
+    <t>435671083</t>
+  </si>
+  <si>
+    <t>435674054</t>
+  </si>
+  <si>
+    <t>435676742</t>
+  </si>
+  <si>
+    <t>435679813</t>
+  </si>
+  <si>
+    <t>435683074</t>
+  </si>
+  <si>
+    <t>435685393</t>
+  </si>
+  <si>
+    <t>435687952</t>
+  </si>
+  <si>
+    <t>435690277</t>
+  </si>
+  <si>
+    <t>435692781</t>
   </si>
 </sst>
 </file>
@@ -6258,7 +6672,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>1769</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6498,7 +6912,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>1770</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6534,7 +6948,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>1771</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6570,7 +6984,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>1772</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6606,7 +7020,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>1773</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6642,7 +7056,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>1774</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6676,7 +7090,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>1775</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6710,7 +7124,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>1776</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6746,7 +7160,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>1777</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6782,7 +7196,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>1778</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6818,7 +7232,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>1779</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6854,7 +7268,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>1780</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6890,7 +7304,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>1781</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6926,7 +7340,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>1782</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6962,7 +7376,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>1783</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6998,7 +7412,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>1784</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7034,7 +7448,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>1785</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7070,7 +7484,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>1786</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7104,7 +7518,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>1787</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7138,7 +7552,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>1788</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7174,7 +7588,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>1789</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7210,7 +7624,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>1790</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7246,7 +7660,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>1791</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7282,7 +7696,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>1792</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7318,7 +7732,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>1793</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7354,7 +7768,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>1794</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7388,7 +7802,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>1795</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7424,7 +7838,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>1796</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7460,7 +7874,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>1797</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7496,7 +7910,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>1798</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7532,7 +7946,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>1799</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7568,7 +7982,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>1800</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7604,7 +8018,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>1801</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7640,7 +8054,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>1802</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7674,7 +8088,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>1803</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7708,7 +8122,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>1804</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7744,7 +8158,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>1805</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7780,7 +8194,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>1806</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7816,7 +8230,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>1807</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7852,7 +8266,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>1808</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7888,7 +8302,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>1809</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7924,7 +8338,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>1810</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7960,7 +8374,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>1812</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7996,7 +8410,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>1813</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8032,7 +8446,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>1814</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8068,7 +8482,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>1811</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8104,7 +8518,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>1815</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8140,7 +8554,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>1816</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8176,7 +8590,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>1817</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8212,7 +8626,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>1818</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8246,7 +8660,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>1819</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8282,7 +8696,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>1820</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8314,7 +8728,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>1821</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8350,7 +8764,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>1830</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8382,7 +8796,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>1831</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8414,7 +8828,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>1832</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8446,7 +8860,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>1833</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8478,7 +8892,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>1834</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8510,7 +8924,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>1835</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8542,7 +8956,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>1836</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8574,7 +8988,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>1837</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8608,7 +9022,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>1841</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8644,7 +9058,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>1825</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8678,7 +9092,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>1826</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8712,7 +9126,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>1823</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8780,7 +9194,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>1824</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8812,7 +9226,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>1827</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8844,7 +9258,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>1828</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8876,7 +9290,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>1829</v>
+        <v>1971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix - bug has fixed in the GET endpoint
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="1980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="2894">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -6041,6 +6041,2748 @@
   </si>
   <si>
     <t>435692781</t>
+  </si>
+  <si>
+    <t>459242101</t>
+  </si>
+  <si>
+    <t>459285159</t>
+  </si>
+  <si>
+    <t>459286663</t>
+  </si>
+  <si>
+    <t>459287476</t>
+  </si>
+  <si>
+    <t>459288680</t>
+  </si>
+  <si>
+    <t>459289631</t>
+  </si>
+  <si>
+    <t>459290588</t>
+  </si>
+  <si>
+    <t>459291614</t>
+  </si>
+  <si>
+    <t>459292822</t>
+  </si>
+  <si>
+    <t>459293916</t>
+  </si>
+  <si>
+    <t>459295242</t>
+  </si>
+  <si>
+    <t>459296298</t>
+  </si>
+  <si>
+    <t>459297376</t>
+  </si>
+  <si>
+    <t>459298563</t>
+  </si>
+  <si>
+    <t>459299708</t>
+  </si>
+  <si>
+    <t>459300760</t>
+  </si>
+  <si>
+    <t>459302116</t>
+  </si>
+  <si>
+    <t>459303279</t>
+  </si>
+  <si>
+    <t>459304676</t>
+  </si>
+  <si>
+    <t>459305836</t>
+  </si>
+  <si>
+    <t>459307243</t>
+  </si>
+  <si>
+    <t>459308471</t>
+  </si>
+  <si>
+    <t>459309986</t>
+  </si>
+  <si>
+    <t>459311231</t>
+  </si>
+  <si>
+    <t>459312586</t>
+  </si>
+  <si>
+    <t>459313885</t>
+  </si>
+  <si>
+    <t>459315224</t>
+  </si>
+  <si>
+    <t>459316565</t>
+  </si>
+  <si>
+    <t>459318235</t>
+  </si>
+  <si>
+    <t>459319536</t>
+  </si>
+  <si>
+    <t>459321082</t>
+  </si>
+  <si>
+    <t>459322546</t>
+  </si>
+  <si>
+    <t>459323855</t>
+  </si>
+  <si>
+    <t>459325285</t>
+  </si>
+  <si>
+    <t>459326765</t>
+  </si>
+  <si>
+    <t>459328215</t>
+  </si>
+  <si>
+    <t>459329888</t>
+  </si>
+  <si>
+    <t>459331340</t>
+  </si>
+  <si>
+    <t>459332775</t>
+  </si>
+  <si>
+    <t>459334551</t>
+  </si>
+  <si>
+    <t>459335998</t>
+  </si>
+  <si>
+    <t>459337569</t>
+  </si>
+  <si>
+    <t>459339129</t>
+  </si>
+  <si>
+    <t>459340647</t>
+  </si>
+  <si>
+    <t>459342372</t>
+  </si>
+  <si>
+    <t>459344053</t>
+  </si>
+  <si>
+    <t>459345680</t>
+  </si>
+  <si>
+    <t>459347234</t>
+  </si>
+  <si>
+    <t>459348811</t>
+  </si>
+  <si>
+    <t>459350361</t>
+  </si>
+  <si>
+    <t>459352330</t>
+  </si>
+  <si>
+    <t>459353991</t>
+  </si>
+  <si>
+    <t>459355926</t>
+  </si>
+  <si>
+    <t>459358550</t>
+  </si>
+  <si>
+    <t>459382267</t>
+  </si>
+  <si>
+    <t>459386948</t>
+  </si>
+  <si>
+    <t>459389811</t>
+  </si>
+  <si>
+    <t>459391791</t>
+  </si>
+  <si>
+    <t>459394666</t>
+  </si>
+  <si>
+    <t>459396713</t>
+  </si>
+  <si>
+    <t>459398810</t>
+  </si>
+  <si>
+    <t>459401222</t>
+  </si>
+  <si>
+    <t>459404413</t>
+  </si>
+  <si>
+    <t>459407061</t>
+  </si>
+  <si>
+    <t>459409940</t>
+  </si>
+  <si>
+    <t>459412515</t>
+  </si>
+  <si>
+    <t>459415535</t>
+  </si>
+  <si>
+    <t>459418324</t>
+  </si>
+  <si>
+    <t>459420976</t>
+  </si>
+  <si>
+    <t>459483780</t>
+  </si>
+  <si>
+    <t>459493540</t>
+  </si>
+  <si>
+    <t>459494783</t>
+  </si>
+  <si>
+    <t>459495732</t>
+  </si>
+  <si>
+    <t>459496686</t>
+  </si>
+  <si>
+    <t>459497611</t>
+  </si>
+  <si>
+    <t>459498827</t>
+  </si>
+  <si>
+    <t>459499766</t>
+  </si>
+  <si>
+    <t>459501009</t>
+  </si>
+  <si>
+    <t>459502100</t>
+  </si>
+  <si>
+    <t>459503422</t>
+  </si>
+  <si>
+    <t>459504538</t>
+  </si>
+  <si>
+    <t>459505626</t>
+  </si>
+  <si>
+    <t>459506750</t>
+  </si>
+  <si>
+    <t>459507793</t>
+  </si>
+  <si>
+    <t>459508926</t>
+  </si>
+  <si>
+    <t>459510380</t>
+  </si>
+  <si>
+    <t>459511581</t>
+  </si>
+  <si>
+    <t>459512975</t>
+  </si>
+  <si>
+    <t>459514157</t>
+  </si>
+  <si>
+    <t>459515554</t>
+  </si>
+  <si>
+    <t>459516953</t>
+  </si>
+  <si>
+    <t>459518496</t>
+  </si>
+  <si>
+    <t>459519752</t>
+  </si>
+  <si>
+    <t>459521017</t>
+  </si>
+  <si>
+    <t>459522317</t>
+  </si>
+  <si>
+    <t>459523717</t>
+  </si>
+  <si>
+    <t>459525198</t>
+  </si>
+  <si>
+    <t>459526803</t>
+  </si>
+  <si>
+    <t>459528103</t>
+  </si>
+  <si>
+    <t>459529762</t>
+  </si>
+  <si>
+    <t>459531222</t>
+  </si>
+  <si>
+    <t>459532584</t>
+  </si>
+  <si>
+    <t>459534020</t>
+  </si>
+  <si>
+    <t>459535497</t>
+  </si>
+  <si>
+    <t>459536993</t>
+  </si>
+  <si>
+    <t>459538727</t>
+  </si>
+  <si>
+    <t>459540278</t>
+  </si>
+  <si>
+    <t>459541814</t>
+  </si>
+  <si>
+    <t>459543699</t>
+  </si>
+  <si>
+    <t>459545238</t>
+  </si>
+  <si>
+    <t>459547125</t>
+  </si>
+  <si>
+    <t>459549077</t>
+  </si>
+  <si>
+    <t>459550733</t>
+  </si>
+  <si>
+    <t>459552383</t>
+  </si>
+  <si>
+    <t>459553963</t>
+  </si>
+  <si>
+    <t>459555717</t>
+  </si>
+  <si>
+    <t>459557404</t>
+  </si>
+  <si>
+    <t>459559060</t>
+  </si>
+  <si>
+    <t>459560731</t>
+  </si>
+  <si>
+    <t>459562678</t>
+  </si>
+  <si>
+    <t>459564381</t>
+  </si>
+  <si>
+    <t>459566378</t>
+  </si>
+  <si>
+    <t>459569544</t>
+  </si>
+  <si>
+    <t>459991569</t>
+  </si>
+  <si>
+    <t>460019385</t>
+  </si>
+  <si>
+    <t>460020430</t>
+  </si>
+  <si>
+    <t>460021374</t>
+  </si>
+  <si>
+    <t>460022574</t>
+  </si>
+  <si>
+    <t>460023539</t>
+  </si>
+  <si>
+    <t>460024821</t>
+  </si>
+  <si>
+    <t>460025695</t>
+  </si>
+  <si>
+    <t>460026958</t>
+  </si>
+  <si>
+    <t>460027938</t>
+  </si>
+  <si>
+    <t>460029243</t>
+  </si>
+  <si>
+    <t>460030323</t>
+  </si>
+  <si>
+    <t>460031458</t>
+  </si>
+  <si>
+    <t>460032490</t>
+  </si>
+  <si>
+    <t>460033652</t>
+  </si>
+  <si>
+    <t>460034768</t>
+  </si>
+  <si>
+    <t>460036191</t>
+  </si>
+  <si>
+    <t>460037316</t>
+  </si>
+  <si>
+    <t>460038814</t>
+  </si>
+  <si>
+    <t>460040064</t>
+  </si>
+  <si>
+    <t>460041486</t>
+  </si>
+  <si>
+    <t>460042694</t>
+  </si>
+  <si>
+    <t>460044221</t>
+  </si>
+  <si>
+    <t>460045464</t>
+  </si>
+  <si>
+    <t>460046849</t>
+  </si>
+  <si>
+    <t>460048176</t>
+  </si>
+  <si>
+    <t>460049543</t>
+  </si>
+  <si>
+    <t>460050852</t>
+  </si>
+  <si>
+    <t>460052516</t>
+  </si>
+  <si>
+    <t>460281219</t>
+  </si>
+  <si>
+    <t>460290866</t>
+  </si>
+  <si>
+    <t>460291915</t>
+  </si>
+  <si>
+    <t>460292833</t>
+  </si>
+  <si>
+    <t>460294082</t>
+  </si>
+  <si>
+    <t>460295041</t>
+  </si>
+  <si>
+    <t>460296268</t>
+  </si>
+  <si>
+    <t>460297308</t>
+  </si>
+  <si>
+    <t>460298630</t>
+  </si>
+  <si>
+    <t>460299753</t>
+  </si>
+  <si>
+    <t>460301062</t>
+  </si>
+  <si>
+    <t>460302189</t>
+  </si>
+  <si>
+    <t>460303268</t>
+  </si>
+  <si>
+    <t>460304381</t>
+  </si>
+  <si>
+    <t>460305539</t>
+  </si>
+  <si>
+    <t>460306749</t>
+  </si>
+  <si>
+    <t>460308195</t>
+  </si>
+  <si>
+    <t>460309355</t>
+  </si>
+  <si>
+    <t>460310803</t>
+  </si>
+  <si>
+    <t>460311928</t>
+  </si>
+  <si>
+    <t>460313495</t>
+  </si>
+  <si>
+    <t>460314814</t>
+  </si>
+  <si>
+    <t>460316330</t>
+  </si>
+  <si>
+    <t>460317688</t>
+  </si>
+  <si>
+    <t>460318992</t>
+  </si>
+  <si>
+    <t>460320352</t>
+  </si>
+  <si>
+    <t>460321726</t>
+  </si>
+  <si>
+    <t>460323073</t>
+  </si>
+  <si>
+    <t>460324703</t>
+  </si>
+  <si>
+    <t>460326090</t>
+  </si>
+  <si>
+    <t>460327675</t>
+  </si>
+  <si>
+    <t>460329104</t>
+  </si>
+  <si>
+    <t>460330544</t>
+  </si>
+  <si>
+    <t>460331972</t>
+  </si>
+  <si>
+    <t>460333407</t>
+  </si>
+  <si>
+    <t>460334911</t>
+  </si>
+  <si>
+    <t>460336668</t>
+  </si>
+  <si>
+    <t>460338167</t>
+  </si>
+  <si>
+    <t>460339708</t>
+  </si>
+  <si>
+    <t>460341494</t>
+  </si>
+  <si>
+    <t>460343112</t>
+  </si>
+  <si>
+    <t>460344748</t>
+  </si>
+  <si>
+    <t>460346487</t>
+  </si>
+  <si>
+    <t>460348149</t>
+  </si>
+  <si>
+    <t>460349760</t>
+  </si>
+  <si>
+    <t>460351411</t>
+  </si>
+  <si>
+    <t>460353064</t>
+  </si>
+  <si>
+    <t>460354801</t>
+  </si>
+  <si>
+    <t>460356637</t>
+  </si>
+  <si>
+    <t>460358364</t>
+  </si>
+  <si>
+    <t>460360454</t>
+  </si>
+  <si>
+    <t>460362252</t>
+  </si>
+  <si>
+    <t>460365147</t>
+  </si>
+  <si>
+    <t>460376967</t>
+  </si>
+  <si>
+    <t>461251692</t>
+  </si>
+  <si>
+    <t>461296722</t>
+  </si>
+  <si>
+    <t>461298078</t>
+  </si>
+  <si>
+    <t>461299039</t>
+  </si>
+  <si>
+    <t>461300261</t>
+  </si>
+  <si>
+    <t>461301322</t>
+  </si>
+  <si>
+    <t>461302663</t>
+  </si>
+  <si>
+    <t>461303605</t>
+  </si>
+  <si>
+    <t>461304869</t>
+  </si>
+  <si>
+    <t>461305975</t>
+  </si>
+  <si>
+    <t>461307326</t>
+  </si>
+  <si>
+    <t>461308374</t>
+  </si>
+  <si>
+    <t>461309442</t>
+  </si>
+  <si>
+    <t>461310573</t>
+  </si>
+  <si>
+    <t>461311756</t>
+  </si>
+  <si>
+    <t>461312882</t>
+  </si>
+  <si>
+    <t>461314298</t>
+  </si>
+  <si>
+    <t>461315680</t>
+  </si>
+  <si>
+    <t>461317108</t>
+  </si>
+  <si>
+    <t>461318288</t>
+  </si>
+  <si>
+    <t>461319834</t>
+  </si>
+  <si>
+    <t>461321055</t>
+  </si>
+  <si>
+    <t>461322619</t>
+  </si>
+  <si>
+    <t>461323972</t>
+  </si>
+  <si>
+    <t>461325378</t>
+  </si>
+  <si>
+    <t>461326662</t>
+  </si>
+  <si>
+    <t>461328040</t>
+  </si>
+  <si>
+    <t>461329396</t>
+  </si>
+  <si>
+    <t>461331072</t>
+  </si>
+  <si>
+    <t>461332537</t>
+  </si>
+  <si>
+    <t>461334226</t>
+  </si>
+  <si>
+    <t>461335681</t>
+  </si>
+  <si>
+    <t>461337171</t>
+  </si>
+  <si>
+    <t>461338645</t>
+  </si>
+  <si>
+    <t>461340144</t>
+  </si>
+  <si>
+    <t>461341645</t>
+  </si>
+  <si>
+    <t>461343458</t>
+  </si>
+  <si>
+    <t>461345010</t>
+  </si>
+  <si>
+    <t>461346574</t>
+  </si>
+  <si>
+    <t>461348447</t>
+  </si>
+  <si>
+    <t>461350089</t>
+  </si>
+  <si>
+    <t>461351820</t>
+  </si>
+  <si>
+    <t>461353505</t>
+  </si>
+  <si>
+    <t>461355178</t>
+  </si>
+  <si>
+    <t>461356878</t>
+  </si>
+  <si>
+    <t>461358652</t>
+  </si>
+  <si>
+    <t>461360369</t>
+  </si>
+  <si>
+    <t>461362176</t>
+  </si>
+  <si>
+    <t>461363991</t>
+  </si>
+  <si>
+    <t>461365694</t>
+  </si>
+  <si>
+    <t>461367790</t>
+  </si>
+  <si>
+    <t>461369564</t>
+  </si>
+  <si>
+    <t>461371709</t>
+  </si>
+  <si>
+    <t>461384018</t>
+  </si>
+  <si>
+    <t>462976000</t>
+  </si>
+  <si>
+    <t>463004240</t>
+  </si>
+  <si>
+    <t>463005341</t>
+  </si>
+  <si>
+    <t>463006239</t>
+  </si>
+  <si>
+    <t>463007497</t>
+  </si>
+  <si>
+    <t>463008431</t>
+  </si>
+  <si>
+    <t>463009666</t>
+  </si>
+  <si>
+    <t>463010716</t>
+  </si>
+  <si>
+    <t>463011979</t>
+  </si>
+  <si>
+    <t>463013067</t>
+  </si>
+  <si>
+    <t>463014538</t>
+  </si>
+  <si>
+    <t>463015734</t>
+  </si>
+  <si>
+    <t>463016866</t>
+  </si>
+  <si>
+    <t>463018020</t>
+  </si>
+  <si>
+    <t>463019119</t>
+  </si>
+  <si>
+    <t>463020177</t>
+  </si>
+  <si>
+    <t>463021675</t>
+  </si>
+  <si>
+    <t>463022887</t>
+  </si>
+  <si>
+    <t>463024337</t>
+  </si>
+  <si>
+    <t>463025458</t>
+  </si>
+  <si>
+    <t>463026992</t>
+  </si>
+  <si>
+    <t>463028243</t>
+  </si>
+  <si>
+    <t>463029690</t>
+  </si>
+  <si>
+    <t>463030949</t>
+  </si>
+  <si>
+    <t>463032264</t>
+  </si>
+  <si>
+    <t>463033634</t>
+  </si>
+  <si>
+    <t>463035019</t>
+  </si>
+  <si>
+    <t>463036395</t>
+  </si>
+  <si>
+    <t>463038037</t>
+  </si>
+  <si>
+    <t>463039372</t>
+  </si>
+  <si>
+    <t>463041197</t>
+  </si>
+  <si>
+    <t>463042616</t>
+  </si>
+  <si>
+    <t>463044112</t>
+  </si>
+  <si>
+    <t>463045583</t>
+  </si>
+  <si>
+    <t>463047127</t>
+  </si>
+  <si>
+    <t>463048591</t>
+  </si>
+  <si>
+    <t>463050322</t>
+  </si>
+  <si>
+    <t>463051925</t>
+  </si>
+  <si>
+    <t>463053426</t>
+  </si>
+  <si>
+    <t>463055301</t>
+  </si>
+  <si>
+    <t>463056859</t>
+  </si>
+  <si>
+    <t>463058510</t>
+  </si>
+  <si>
+    <t>463060164</t>
+  </si>
+  <si>
+    <t>463061853</t>
+  </si>
+  <si>
+    <t>463063503</t>
+  </si>
+  <si>
+    <t>463065146</t>
+  </si>
+  <si>
+    <t>463066785</t>
+  </si>
+  <si>
+    <t>463068494</t>
+  </si>
+  <si>
+    <t>463070289</t>
+  </si>
+  <si>
+    <t>463072084</t>
+  </si>
+  <si>
+    <t>463074153</t>
+  </si>
+  <si>
+    <t>463075911</t>
+  </si>
+  <si>
+    <t>463077979</t>
+  </si>
+  <si>
+    <t>463081181</t>
+  </si>
+  <si>
+    <t>463520868</t>
+  </si>
+  <si>
+    <t>463639440</t>
+  </si>
+  <si>
+    <t>463755731</t>
+  </si>
+  <si>
+    <t>464773447</t>
+  </si>
+  <si>
+    <t>465954450</t>
+  </si>
+  <si>
+    <t>466062400</t>
+  </si>
+  <si>
+    <t>466222903</t>
+  </si>
+  <si>
+    <t>466238634</t>
+  </si>
+  <si>
+    <t>466779473</t>
+  </si>
+  <si>
+    <t>466816459</t>
+  </si>
+  <si>
+    <t>466876892</t>
+  </si>
+  <si>
+    <t>466885701</t>
+  </si>
+  <si>
+    <t>468420300</t>
+  </si>
+  <si>
+    <t>468428957</t>
+  </si>
+  <si>
+    <t>468443543</t>
+  </si>
+  <si>
+    <t>468448740</t>
+  </si>
+  <si>
+    <t>469134125</t>
+  </si>
+  <si>
+    <t>469157471</t>
+  </si>
+  <si>
+    <t>469375833</t>
+  </si>
+  <si>
+    <t>469380476</t>
+  </si>
+  <si>
+    <t>469869175</t>
+  </si>
+  <si>
+    <t>469892760</t>
+  </si>
+  <si>
+    <t>470100988</t>
+  </si>
+  <si>
+    <t>470105895</t>
+  </si>
+  <si>
+    <t>470731125</t>
+  </si>
+  <si>
+    <t>470745639</t>
+  </si>
+  <si>
+    <t>471358344</t>
+  </si>
+  <si>
+    <t>471363508</t>
+  </si>
+  <si>
+    <t>471365576</t>
+  </si>
+  <si>
+    <t>471971055</t>
+  </si>
+  <si>
+    <t>471977541</t>
+  </si>
+  <si>
+    <t>471978474</t>
+  </si>
+  <si>
+    <t>471979306</t>
+  </si>
+  <si>
+    <t>471980435</t>
+  </si>
+  <si>
+    <t>471981254</t>
+  </si>
+  <si>
+    <t>471982129</t>
+  </si>
+  <si>
+    <t>471982987</t>
+  </si>
+  <si>
+    <t>472119766</t>
+  </si>
+  <si>
+    <t>472126317</t>
+  </si>
+  <si>
+    <t>472127224</t>
+  </si>
+  <si>
+    <t>472128028</t>
+  </si>
+  <si>
+    <t>472129112</t>
+  </si>
+  <si>
+    <t>472129942</t>
+  </si>
+  <si>
+    <t>472130793</t>
+  </si>
+  <si>
+    <t>472131660</t>
+  </si>
+  <si>
+    <t>472132845</t>
+  </si>
+  <si>
+    <t>472133745</t>
+  </si>
+  <si>
+    <t>472134687</t>
+  </si>
+  <si>
+    <t>472135629</t>
+  </si>
+  <si>
+    <t>472136614</t>
+  </si>
+  <si>
+    <t>472137609</t>
+  </si>
+  <si>
+    <t>472138621</t>
+  </si>
+  <si>
+    <t>472139642</t>
+  </si>
+  <si>
+    <t>472140957</t>
+  </si>
+  <si>
+    <t>472142003</t>
+  </si>
+  <si>
+    <t>472143378</t>
+  </si>
+  <si>
+    <t>472144462</t>
+  </si>
+  <si>
+    <t>472145815</t>
+  </si>
+  <si>
+    <t>472146956</t>
+  </si>
+  <si>
+    <t>472148351</t>
+  </si>
+  <si>
+    <t>472149488</t>
+  </si>
+  <si>
+    <t>472150661</t>
+  </si>
+  <si>
+    <t>472151866</t>
+  </si>
+  <si>
+    <t>472153041</t>
+  </si>
+  <si>
+    <t>472154226</t>
+  </si>
+  <si>
+    <t>472155662</t>
+  </si>
+  <si>
+    <t>472156910</t>
+  </si>
+  <si>
+    <t>472158431</t>
+  </si>
+  <si>
+    <t>472159699</t>
+  </si>
+  <si>
+    <t>472160959</t>
+  </si>
+  <si>
+    <t>472162247</t>
+  </si>
+  <si>
+    <t>472163566</t>
+  </si>
+  <si>
+    <t>472164900</t>
+  </si>
+  <si>
+    <t>472166487</t>
+  </si>
+  <si>
+    <t>472167848</t>
+  </si>
+  <si>
+    <t>472169225</t>
+  </si>
+  <si>
+    <t>472170862</t>
+  </si>
+  <si>
+    <t>472172310</t>
+  </si>
+  <si>
+    <t>472173834</t>
+  </si>
+  <si>
+    <t>472175346</t>
+  </si>
+  <si>
+    <t>472176879</t>
+  </si>
+  <si>
+    <t>472178386</t>
+  </si>
+  <si>
+    <t>472179939</t>
+  </si>
+  <si>
+    <t>472181502</t>
+  </si>
+  <si>
+    <t>472183152</t>
+  </si>
+  <si>
+    <t>472184784</t>
+  </si>
+  <si>
+    <t>472186414</t>
+  </si>
+  <si>
+    <t>472188312</t>
+  </si>
+  <si>
+    <t>472189931</t>
+  </si>
+  <si>
+    <t>472192049</t>
+  </si>
+  <si>
+    <t>472193830</t>
+  </si>
+  <si>
+    <t>472196687</t>
+  </si>
+  <si>
+    <t>472200730</t>
+  </si>
+  <si>
+    <t>472203268</t>
+  </si>
+  <si>
+    <t>472205230</t>
+  </si>
+  <si>
+    <t>472207280</t>
+  </si>
+  <si>
+    <t>472209283</t>
+  </si>
+  <si>
+    <t>472211410</t>
+  </si>
+  <si>
+    <t>472213853</t>
+  </si>
+  <si>
+    <t>472216318</t>
+  </si>
+  <si>
+    <t>472219056</t>
+  </si>
+  <si>
+    <t>472221605</t>
+  </si>
+  <si>
+    <t>472224467</t>
+  </si>
+  <si>
+    <t>472227095</t>
+  </si>
+  <si>
+    <t>472229723</t>
+  </si>
+  <si>
+    <t>472580505</t>
+  </si>
+  <si>
+    <t>472587083</t>
+  </si>
+  <si>
+    <t>472587920</t>
+  </si>
+  <si>
+    <t>472588725</t>
+  </si>
+  <si>
+    <t>472589864</t>
+  </si>
+  <si>
+    <t>472590685</t>
+  </si>
+  <si>
+    <t>472591581</t>
+  </si>
+  <si>
+    <t>472592489</t>
+  </si>
+  <si>
+    <t>472593659</t>
+  </si>
+  <si>
+    <t>472594581</t>
+  </si>
+  <si>
+    <t>472595550</t>
+  </si>
+  <si>
+    <t>472596561</t>
+  </si>
+  <si>
+    <t>472597531</t>
+  </si>
+  <si>
+    <t>472598513</t>
+  </si>
+  <si>
+    <t>472599550</t>
+  </si>
+  <si>
+    <t>472600551</t>
+  </si>
+  <si>
+    <t>472601849</t>
+  </si>
+  <si>
+    <t>472602894</t>
+  </si>
+  <si>
+    <t>472604254</t>
+  </si>
+  <si>
+    <t>472605304</t>
+  </si>
+  <si>
+    <t>472606675</t>
+  </si>
+  <si>
+    <t>472607833</t>
+  </si>
+  <si>
+    <t>472609272</t>
+  </si>
+  <si>
+    <t>472610456</t>
+  </si>
+  <si>
+    <t>472611694</t>
+  </si>
+  <si>
+    <t>472612884</t>
+  </si>
+  <si>
+    <t>472614113</t>
+  </si>
+  <si>
+    <t>472615324</t>
+  </si>
+  <si>
+    <t>472616852</t>
+  </si>
+  <si>
+    <t>472618123</t>
+  </si>
+  <si>
+    <t>472619676</t>
+  </si>
+  <si>
+    <t>472620987</t>
+  </si>
+  <si>
+    <t>472622271</t>
+  </si>
+  <si>
+    <t>472623581</t>
+  </si>
+  <si>
+    <t>472624925</t>
+  </si>
+  <si>
+    <t>472626256</t>
+  </si>
+  <si>
+    <t>472627878</t>
+  </si>
+  <si>
+    <t>472629318</t>
+  </si>
+  <si>
+    <t>472630724</t>
+  </si>
+  <si>
+    <t>472632442</t>
+  </si>
+  <si>
+    <t>472633949</t>
+  </si>
+  <si>
+    <t>472635503</t>
+  </si>
+  <si>
+    <t>472637036</t>
+  </si>
+  <si>
+    <t>472638520</t>
+  </si>
+  <si>
+    <t>472639988</t>
+  </si>
+  <si>
+    <t>472641504</t>
+  </si>
+  <si>
+    <t>472643083</t>
+  </si>
+  <si>
+    <t>472644658</t>
+  </si>
+  <si>
+    <t>472646258</t>
+  </si>
+  <si>
+    <t>472647864</t>
+  </si>
+  <si>
+    <t>472649708</t>
+  </si>
+  <si>
+    <t>472651347</t>
+  </si>
+  <si>
+    <t>472653519</t>
+  </si>
+  <si>
+    <t>472655351</t>
+  </si>
+  <si>
+    <t>472657971</t>
+  </si>
+  <si>
+    <t>472662070</t>
+  </si>
+  <si>
+    <t>472664691</t>
+  </si>
+  <si>
+    <t>472666577</t>
+  </si>
+  <si>
+    <t>472669331</t>
+  </si>
+  <si>
+    <t>472671311</t>
+  </si>
+  <si>
+    <t>472673412</t>
+  </si>
+  <si>
+    <t>472675578</t>
+  </si>
+  <si>
+    <t>472678123</t>
+  </si>
+  <si>
+    <t>472680597</t>
+  </si>
+  <si>
+    <t>472683338</t>
+  </si>
+  <si>
+    <t>472685819</t>
+  </si>
+  <si>
+    <t>472688630</t>
+  </si>
+  <si>
+    <t>472691227</t>
+  </si>
+  <si>
+    <t>472693816</t>
+  </si>
+  <si>
+    <t>473310628</t>
+  </si>
+  <si>
+    <t>473317606</t>
+  </si>
+  <si>
+    <t>473318489</t>
+  </si>
+  <si>
+    <t>473319315</t>
+  </si>
+  <si>
+    <t>473320411</t>
+  </si>
+  <si>
+    <t>473321268</t>
+  </si>
+  <si>
+    <t>473322160</t>
+  </si>
+  <si>
+    <t>473323053</t>
+  </si>
+  <si>
+    <t>473324196</t>
+  </si>
+  <si>
+    <t>473325133</t>
+  </si>
+  <si>
+    <t>473326117</t>
+  </si>
+  <si>
+    <t>473327051</t>
+  </si>
+  <si>
+    <t>473328018</t>
+  </si>
+  <si>
+    <t>473329016</t>
+  </si>
+  <si>
+    <t>473330020</t>
+  </si>
+  <si>
+    <t>473331056</t>
+  </si>
+  <si>
+    <t>473332382</t>
+  </si>
+  <si>
+    <t>473333438</t>
+  </si>
+  <si>
+    <t>473334694</t>
+  </si>
+  <si>
+    <t>473335786</t>
+  </si>
+  <si>
+    <t>473337174</t>
+  </si>
+  <si>
+    <t>473338301</t>
+  </si>
+  <si>
+    <t>473339753</t>
+  </si>
+  <si>
+    <t>473340909</t>
+  </si>
+  <si>
+    <t>473342067</t>
+  </si>
+  <si>
+    <t>473343284</t>
+  </si>
+  <si>
+    <t>473344512</t>
+  </si>
+  <si>
+    <t>473345726</t>
+  </si>
+  <si>
+    <t>473347255</t>
+  </si>
+  <si>
+    <t>473348559</t>
+  </si>
+  <si>
+    <t>473350130</t>
+  </si>
+  <si>
+    <t>473351424</t>
+  </si>
+  <si>
+    <t>473352737</t>
+  </si>
+  <si>
+    <t>473354049</t>
+  </si>
+  <si>
+    <t>473355429</t>
+  </si>
+  <si>
+    <t>473356801</t>
+  </si>
+  <si>
+    <t>473358498</t>
+  </si>
+  <si>
+    <t>473359893</t>
+  </si>
+  <si>
+    <t>473361334</t>
+  </si>
+  <si>
+    <t>473363080</t>
+  </si>
+  <si>
+    <t>473364833</t>
+  </si>
+  <si>
+    <t>473366372</t>
+  </si>
+  <si>
+    <t>473367946</t>
+  </si>
+  <si>
+    <t>473369460</t>
+  </si>
+  <si>
+    <t>473371002</t>
+  </si>
+  <si>
+    <t>473372551</t>
+  </si>
+  <si>
+    <t>473374097</t>
+  </si>
+  <si>
+    <t>473375706</t>
+  </si>
+  <si>
+    <t>473377358</t>
+  </si>
+  <si>
+    <t>473378987</t>
+  </si>
+  <si>
+    <t>473380965</t>
+  </si>
+  <si>
+    <t>473382643</t>
+  </si>
+  <si>
+    <t>473384901</t>
+  </si>
+  <si>
+    <t>473386863</t>
+  </si>
+  <si>
+    <t>473389541</t>
+  </si>
+  <si>
+    <t>473393708</t>
+  </si>
+  <si>
+    <t>473396368</t>
+  </si>
+  <si>
+    <t>473398362</t>
+  </si>
+  <si>
+    <t>473401110</t>
+  </si>
+  <si>
+    <t>473403168</t>
+  </si>
+  <si>
+    <t>473405241</t>
+  </si>
+  <si>
+    <t>473407393</t>
+  </si>
+  <si>
+    <t>473409930</t>
+  </si>
+  <si>
+    <t>473412424</t>
+  </si>
+  <si>
+    <t>473415396</t>
+  </si>
+  <si>
+    <t>473417940</t>
+  </si>
+  <si>
+    <t>473420816</t>
+  </si>
+  <si>
+    <t>473423444</t>
+  </si>
+  <si>
+    <t>473426176</t>
+  </si>
+  <si>
+    <t>474440238</t>
+  </si>
+  <si>
+    <t>474464653</t>
+  </si>
+  <si>
+    <t>474465595</t>
+  </si>
+  <si>
+    <t>474466415</t>
+  </si>
+  <si>
+    <t>474467572</t>
+  </si>
+  <si>
+    <t>474468416</t>
+  </si>
+  <si>
+    <t>474469325</t>
+  </si>
+  <si>
+    <t>474470228</t>
+  </si>
+  <si>
+    <t>474471380</t>
+  </si>
+  <si>
+    <t>474472375</t>
+  </si>
+  <si>
+    <t>474473662</t>
+  </si>
+  <si>
+    <t>474474661</t>
+  </si>
+  <si>
+    <t>474475676</t>
+  </si>
+  <si>
+    <t>474476678</t>
+  </si>
+  <si>
+    <t>474477958</t>
+  </si>
+  <si>
+    <t>474478987</t>
+  </si>
+  <si>
+    <t>474480315</t>
+  </si>
+  <si>
+    <t>474481378</t>
+  </si>
+  <si>
+    <t>474482753</t>
+  </si>
+  <si>
+    <t>474483992</t>
+  </si>
+  <si>
+    <t>474485373</t>
+  </si>
+  <si>
+    <t>474486528</t>
+  </si>
+  <si>
+    <t>474487988</t>
+  </si>
+  <si>
+    <t>474489169</t>
+  </si>
+  <si>
+    <t>474490380</t>
+  </si>
+  <si>
+    <t>474491593</t>
+  </si>
+  <si>
+    <t>474492847</t>
+  </si>
+  <si>
+    <t>474494099</t>
+  </si>
+  <si>
+    <t>474495645</t>
+  </si>
+  <si>
+    <t>474496927</t>
+  </si>
+  <si>
+    <t>474498518</t>
+  </si>
+  <si>
+    <t>474499897</t>
+  </si>
+  <si>
+    <t>474501211</t>
+  </si>
+  <si>
+    <t>474502740</t>
+  </si>
+  <si>
+    <t>474504141</t>
+  </si>
+  <si>
+    <t>474505535</t>
+  </si>
+  <si>
+    <t>474507218</t>
+  </si>
+  <si>
+    <t>474508672</t>
+  </si>
+  <si>
+    <t>474510112</t>
+  </si>
+  <si>
+    <t>474511864</t>
+  </si>
+  <si>
+    <t>474513337</t>
+  </si>
+  <si>
+    <t>474514847</t>
+  </si>
+  <si>
+    <t>474516432</t>
+  </si>
+  <si>
+    <t>474517972</t>
+  </si>
+  <si>
+    <t>474519497</t>
+  </si>
+  <si>
+    <t>474521034</t>
+  </si>
+  <si>
+    <t>474522692</t>
+  </si>
+  <si>
+    <t>474524332</t>
+  </si>
+  <si>
+    <t>474525971</t>
+  </si>
+  <si>
+    <t>474527621</t>
+  </si>
+  <si>
+    <t>474529560</t>
+  </si>
+  <si>
+    <t>474531237</t>
+  </si>
+  <si>
+    <t>474533495</t>
+  </si>
+  <si>
+    <t>474535429</t>
+  </si>
+  <si>
+    <t>474538145</t>
+  </si>
+  <si>
+    <t>474542326</t>
+  </si>
+  <si>
+    <t>474545034</t>
+  </si>
+  <si>
+    <t>474547143</t>
+  </si>
+  <si>
+    <t>474549988</t>
+  </si>
+  <si>
+    <t>474552058</t>
+  </si>
+  <si>
+    <t>474554143</t>
+  </si>
+  <si>
+    <t>474556440</t>
+  </si>
+  <si>
+    <t>474558955</t>
+  </si>
+  <si>
+    <t>474561498</t>
+  </si>
+  <si>
+    <t>474564534</t>
+  </si>
+  <si>
+    <t>474567090</t>
+  </si>
+  <si>
+    <t>474570048</t>
+  </si>
+  <si>
+    <t>474572752</t>
+  </si>
+  <si>
+    <t>474575520</t>
+  </si>
+  <si>
+    <t>475745253</t>
+  </si>
+  <si>
+    <t>475752459</t>
+  </si>
+  <si>
+    <t>475753425</t>
+  </si>
+  <si>
+    <t>475754540</t>
+  </si>
+  <si>
+    <t>475755409</t>
+  </si>
+  <si>
+    <t>475756286</t>
+  </si>
+  <si>
+    <t>475757427</t>
+  </si>
+  <si>
+    <t>475758309</t>
+  </si>
+  <si>
+    <t>475759281</t>
+  </si>
+  <si>
+    <t>475760363</t>
+  </si>
+  <si>
+    <t>475761354</t>
+  </si>
+  <si>
+    <t>475762419</t>
+  </si>
+  <si>
+    <t>475763448</t>
+  </si>
+  <si>
+    <t>475764457</t>
+  </si>
+  <si>
+    <t>475765798</t>
+  </si>
+  <si>
+    <t>475766827</t>
+  </si>
+  <si>
+    <t>475767911</t>
+  </si>
+  <si>
+    <t>475769022</t>
+  </si>
+  <si>
+    <t>475770116</t>
+  </si>
+  <si>
+    <t>475771241</t>
+  </si>
+  <si>
+    <t>475772641</t>
+  </si>
+  <si>
+    <t>475773788</t>
+  </si>
+  <si>
+    <t>475774950</t>
+  </si>
+  <si>
+    <t>475776157</t>
+  </si>
+  <si>
+    <t>475777380</t>
+  </si>
+  <si>
+    <t>475778917</t>
+  </si>
+  <si>
+    <t>475780194</t>
+  </si>
+  <si>
+    <t>475781756</t>
+  </si>
+  <si>
+    <t>475783025</t>
+  </si>
+  <si>
+    <t>475784312</t>
+  </si>
+  <si>
+    <t>475785647</t>
+  </si>
+  <si>
+    <t>475787023</t>
+  </si>
+  <si>
+    <t>475788364</t>
+  </si>
+  <si>
+    <t>475789735</t>
+  </si>
+  <si>
+    <t>475791158</t>
+  </si>
+  <si>
+    <t>475792551</t>
+  </si>
+  <si>
+    <t>475793987</t>
+  </si>
+  <si>
+    <t>475795450</t>
+  </si>
+  <si>
+    <t>475797152</t>
+  </si>
+  <si>
+    <t>475798644</t>
+  </si>
+  <si>
+    <t>475800309</t>
+  </si>
+  <si>
+    <t>475801846</t>
+  </si>
+  <si>
+    <t>475803464</t>
+  </si>
+  <si>
+    <t>475805022</t>
+  </si>
+  <si>
+    <t>475806581</t>
+  </si>
+  <si>
+    <t>475808163</t>
+  </si>
+  <si>
+    <t>475809807</t>
+  </si>
+  <si>
+    <t>475811434</t>
+  </si>
+  <si>
+    <t>475813064</t>
+  </si>
+  <si>
+    <t>475814683</t>
+  </si>
+  <si>
+    <t>475816361</t>
+  </si>
+  <si>
+    <t>475818038</t>
+  </si>
+  <si>
+    <t>475819990</t>
+  </si>
+  <si>
+    <t>475821943</t>
+  </si>
+  <si>
+    <t>475824325</t>
+  </si>
+  <si>
+    <t>475828259</t>
+  </si>
+  <si>
+    <t>475830922</t>
+  </si>
+  <si>
+    <t>475832952</t>
+  </si>
+  <si>
+    <t>475835727</t>
+  </si>
+  <si>
+    <t>475837844</t>
+  </si>
+  <si>
+    <t>475839954</t>
+  </si>
+  <si>
+    <t>475842240</t>
+  </si>
+  <si>
+    <t>475866104</t>
+  </si>
+  <si>
+    <t>475868722</t>
+  </si>
+  <si>
+    <t>475871623</t>
+  </si>
+  <si>
+    <t>475874224</t>
+  </si>
+  <si>
+    <t>475877143</t>
+  </si>
+  <si>
+    <t>475879817</t>
+  </si>
+  <si>
+    <t>475882472</t>
+  </si>
+  <si>
+    <t>476269150</t>
+  </si>
+  <si>
+    <t>477152154</t>
+  </si>
+  <si>
+    <t>477568694</t>
+  </si>
+  <si>
+    <t>477670749</t>
+  </si>
+  <si>
+    <t>477778975</t>
+  </si>
+  <si>
+    <t>477901544</t>
+  </si>
+  <si>
+    <t>478126456</t>
+  </si>
+  <si>
+    <t>478180100</t>
+  </si>
+  <si>
+    <t>478185230</t>
+  </si>
+  <si>
+    <t>478394120</t>
+  </si>
+  <si>
+    <t>478400435</t>
+  </si>
+  <si>
+    <t>478661393</t>
+  </si>
+  <si>
+    <t>478668199</t>
+  </si>
+  <si>
+    <t>479218917</t>
+  </si>
+  <si>
+    <t>479246597</t>
+  </si>
+  <si>
+    <t>479247976</t>
+  </si>
+  <si>
+    <t>479248815</t>
+  </si>
+  <si>
+    <t>479249988</t>
+  </si>
+  <si>
+    <t>479250842</t>
+  </si>
+  <si>
+    <t>479251763</t>
+  </si>
+  <si>
+    <t>479252726</t>
+  </si>
+  <si>
+    <t>479253926</t>
+  </si>
+  <si>
+    <t>479254866</t>
+  </si>
+  <si>
+    <t>479256145</t>
+  </si>
+  <si>
+    <t>479257128</t>
+  </si>
+  <si>
+    <t>479258175</t>
+  </si>
+  <si>
+    <t>479259208</t>
+  </si>
+  <si>
+    <t>479260307</t>
+  </si>
+  <si>
+    <t>479261441</t>
+  </si>
+  <si>
+    <t>479262785</t>
+  </si>
+  <si>
+    <t>479263905</t>
+  </si>
+  <si>
+    <t>479265344</t>
+  </si>
+  <si>
+    <t>479266488</t>
+  </si>
+  <si>
+    <t>479267886</t>
+  </si>
+  <si>
+    <t>479269065</t>
+  </si>
+  <si>
+    <t>479270537</t>
+  </si>
+  <si>
+    <t>479271892</t>
+  </si>
+  <si>
+    <t>479273160</t>
+  </si>
+  <si>
+    <t>479274428</t>
+  </si>
+  <si>
+    <t>479275800</t>
+  </si>
+  <si>
+    <t>479277097</t>
+  </si>
+  <si>
+    <t>479278676</t>
+  </si>
+  <si>
+    <t>479280003</t>
+  </si>
+  <si>
+    <t>479281629</t>
+  </si>
+  <si>
+    <t>479283020</t>
+  </si>
+  <si>
+    <t>479284380</t>
+  </si>
+  <si>
+    <t>479285768</t>
+  </si>
+  <si>
+    <t>479287175</t>
+  </si>
+  <si>
+    <t>479288635</t>
+  </si>
+  <si>
+    <t>479290350</t>
+  </si>
+  <si>
+    <t>479291831</t>
+  </si>
+  <si>
+    <t>479293342</t>
+  </si>
+  <si>
+    <t>479295105</t>
+  </si>
+  <si>
+    <t>479296677</t>
+  </si>
+  <si>
+    <t>479298238</t>
+  </si>
+  <si>
+    <t>479299879</t>
+  </si>
+  <si>
+    <t>479301440</t>
+  </si>
+  <si>
+    <t>479303038</t>
+  </si>
+  <si>
+    <t>479304659</t>
+  </si>
+  <si>
+    <t>479306317</t>
+  </si>
+  <si>
+    <t>479308013</t>
+  </si>
+  <si>
+    <t>479309707</t>
+  </si>
+  <si>
+    <t>479311417</t>
+  </si>
+  <si>
+    <t>479313406</t>
+  </si>
+  <si>
+    <t>479315135</t>
+  </si>
+  <si>
+    <t>479317424</t>
+  </si>
+  <si>
+    <t>479319408</t>
+  </si>
+  <si>
+    <t>479322160</t>
+  </si>
+  <si>
+    <t>479326440</t>
+  </si>
+  <si>
+    <t>479329175</t>
+  </si>
+  <si>
+    <t>479331652</t>
+  </si>
+  <si>
+    <t>479334259</t>
+  </si>
+  <si>
+    <t>479336768</t>
+  </si>
+  <si>
+    <t>479339300</t>
+  </si>
+  <si>
+    <t>479341901</t>
+  </si>
+  <si>
+    <t>479344476</t>
+  </si>
+  <si>
+    <t>479347348</t>
+  </si>
+  <si>
+    <t>479349987</t>
+  </si>
+  <si>
+    <t>479352956</t>
+  </si>
+  <si>
+    <t>479355706</t>
+  </si>
+  <si>
+    <t>479358457</t>
+  </si>
+  <si>
+    <t>479501786</t>
+  </si>
+  <si>
+    <t>479508673</t>
+  </si>
+  <si>
+    <t>479509549</t>
+  </si>
+  <si>
+    <t>479510441</t>
+  </si>
+  <si>
+    <t>479511618</t>
+  </si>
+  <si>
+    <t>479512493</t>
+  </si>
+  <si>
+    <t>479513425</t>
+  </si>
+  <si>
+    <t>479514358</t>
+  </si>
+  <si>
+    <t>479515589</t>
+  </si>
+  <si>
+    <t>479516596</t>
+  </si>
+  <si>
+    <t>479517897</t>
+  </si>
+  <si>
+    <t>479518910</t>
+  </si>
+  <si>
+    <t>479519960</t>
+  </si>
+  <si>
+    <t>479521003</t>
+  </si>
+  <si>
+    <t>479522088</t>
+  </si>
+  <si>
+    <t>479523260</t>
+  </si>
+  <si>
+    <t>479524907</t>
+  </si>
+  <si>
+    <t>479526034</t>
+  </si>
+  <si>
+    <t>479527440</t>
+  </si>
+  <si>
+    <t>479528592</t>
+  </si>
+  <si>
+    <t>479530064</t>
+  </si>
+  <si>
+    <t>479531285</t>
+  </si>
+  <si>
+    <t>479532808</t>
+  </si>
+  <si>
+    <t>479534040</t>
+  </si>
+  <si>
+    <t>479535303</t>
+  </si>
+  <si>
+    <t>479536580</t>
+  </si>
+  <si>
+    <t>479537908</t>
+  </si>
+  <si>
+    <t>479539204</t>
+  </si>
+  <si>
+    <t>479540784</t>
+  </si>
+  <si>
+    <t>479542129</t>
+  </si>
+  <si>
+    <t>479543769</t>
+  </si>
+  <si>
+    <t>479545175</t>
+  </si>
+  <si>
+    <t>479546601</t>
+  </si>
+  <si>
+    <t>479548027</t>
+  </si>
+  <si>
+    <t>479549500</t>
+  </si>
+  <si>
+    <t>479550927</t>
+  </si>
+  <si>
+    <t>479552659</t>
+  </si>
+  <si>
+    <t>479554219</t>
+  </si>
+  <si>
+    <t>479555870</t>
+  </si>
+  <si>
+    <t>479557662</t>
+  </si>
+  <si>
+    <t>479559286</t>
+  </si>
+  <si>
+    <t>479560893</t>
+  </si>
+  <si>
+    <t>479562531</t>
+  </si>
+  <si>
+    <t>479564160</t>
+  </si>
+  <si>
+    <t>479565795</t>
+  </si>
+  <si>
+    <t>479567442</t>
+  </si>
+  <si>
+    <t>479569144</t>
+  </si>
+  <si>
+    <t>479570845</t>
+  </si>
+  <si>
+    <t>479572561</t>
+  </si>
+  <si>
+    <t>479574285</t>
+  </si>
+  <si>
+    <t>479576346</t>
+  </si>
+  <si>
+    <t>479578114</t>
+  </si>
+  <si>
+    <t>479580445</t>
+  </si>
+  <si>
+    <t>479582440</t>
+  </si>
+  <si>
+    <t>479585222</t>
+  </si>
+  <si>
+    <t>479589557</t>
+  </si>
+  <si>
+    <t>479592312</t>
+  </si>
+  <si>
+    <t>479594724</t>
+  </si>
+  <si>
+    <t>479597988</t>
+  </si>
+  <si>
+    <t>479600582</t>
+  </si>
+  <si>
+    <t>479603112</t>
+  </si>
+  <si>
+    <t>479605722</t>
+  </si>
+  <si>
+    <t>479608355</t>
+  </si>
+  <si>
+    <t>479611002</t>
+  </si>
+  <si>
+    <t>479613972</t>
+  </si>
+  <si>
+    <t>479616628</t>
+  </si>
+  <si>
+    <t>479619697</t>
+  </si>
+  <si>
+    <t>479622423</t>
+  </si>
+  <si>
+    <t>479625150</t>
+  </si>
+  <si>
+    <t>479942103</t>
+  </si>
+  <si>
+    <t>479950082</t>
+  </si>
+  <si>
+    <t>479951399</t>
+  </si>
+  <si>
+    <t>479952465</t>
+  </si>
+  <si>
+    <t>479953786</t>
+  </si>
+  <si>
+    <t>479954869</t>
+  </si>
+  <si>
+    <t>479956338</t>
+  </si>
+  <si>
+    <t>479957447</t>
+  </si>
+  <si>
+    <t>479958829</t>
+  </si>
+  <si>
+    <t>479960087</t>
+  </si>
+  <si>
+    <t>479961496</t>
+  </si>
+  <si>
+    <t>479962701</t>
+  </si>
+  <si>
+    <t>479963930</t>
+  </si>
+  <si>
+    <t>479965209</t>
+  </si>
+  <si>
+    <t>479966744</t>
+  </si>
+  <si>
+    <t>479968221</t>
+  </si>
+  <si>
+    <t>479969944</t>
+  </si>
+  <si>
+    <t>479971299</t>
+  </si>
+  <si>
+    <t>479973038</t>
+  </si>
+  <si>
+    <t>479974392</t>
+  </si>
+  <si>
+    <t>479975958</t>
+  </si>
+  <si>
+    <t>479977351</t>
+  </si>
+  <si>
+    <t>479979002</t>
+  </si>
+  <si>
+    <t>479980476</t>
+  </si>
+  <si>
+    <t>479981961</t>
+  </si>
+  <si>
+    <t>479983556</t>
+  </si>
+  <si>
+    <t>479985162</t>
+  </si>
+  <si>
+    <t>479986869</t>
+  </si>
+  <si>
+    <t>479988625</t>
+  </si>
+  <si>
+    <t>479990189</t>
+  </si>
+  <si>
+    <t>479992111</t>
+  </si>
+  <si>
+    <t>479993933</t>
+  </si>
+  <si>
+    <t>479995647</t>
+  </si>
+  <si>
+    <t>479997493</t>
+  </si>
+  <si>
+    <t>479999285</t>
+  </si>
+  <si>
+    <t>480001013</t>
+  </si>
+  <si>
+    <t>480003038</t>
+  </si>
+  <si>
+    <t>480004811</t>
+  </si>
+  <si>
+    <t>480006588</t>
+  </si>
+  <si>
+    <t>480008741</t>
+  </si>
+  <si>
+    <t>480010557</t>
+  </si>
+  <si>
+    <t>480012398</t>
+  </si>
+  <si>
+    <t>480014361</t>
+  </si>
+  <si>
+    <t>480016338</t>
+  </si>
+  <si>
+    <t>480018306</t>
+  </si>
+  <si>
+    <t>480020342</t>
+  </si>
+  <si>
+    <t>480022324</t>
+  </si>
+  <si>
+    <t>480024353</t>
+  </si>
+  <si>
+    <t>480026379</t>
+  </si>
+  <si>
+    <t>480028379</t>
+  </si>
+  <si>
+    <t>480030708</t>
+  </si>
+  <si>
+    <t>480033242</t>
+  </si>
+  <si>
+    <t>480036117</t>
+  </si>
+  <si>
+    <t>480038612</t>
+  </si>
+  <si>
+    <t>480041769</t>
+  </si>
+  <si>
+    <t>480046677</t>
+  </si>
+  <si>
+    <t>480050175</t>
+  </si>
+  <si>
+    <t>480053225</t>
+  </si>
+  <si>
+    <t>480057344</t>
+  </si>
+  <si>
+    <t>480060383</t>
+  </si>
+  <si>
+    <t>480063491</t>
+  </si>
+  <si>
+    <t>480066509</t>
+  </si>
+  <si>
+    <t>480069753</t>
+  </si>
+  <si>
+    <t>480072960</t>
+  </si>
+  <si>
+    <t>480076544</t>
+  </si>
+  <si>
+    <t>480079719</t>
+  </si>
+  <si>
+    <t>480083549</t>
+  </si>
+  <si>
+    <t>480086789</t>
+  </si>
+  <si>
+    <t>480089946</t>
   </si>
 </sst>
 </file>
@@ -6672,7 +9414,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>1911</v>
+        <v>2825</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6912,7 +9654,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>1912</v>
+        <v>2826</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6948,7 +9690,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>1913</v>
+        <v>2827</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6984,7 +9726,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>1914</v>
+        <v>2828</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7020,7 +9762,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>1915</v>
+        <v>2829</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7056,7 +9798,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>1916</v>
+        <v>2830</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7090,7 +9832,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>1917</v>
+        <v>2831</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7124,7 +9866,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>1918</v>
+        <v>2832</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7160,7 +9902,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>1919</v>
+        <v>2833</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7196,7 +9938,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>1920</v>
+        <v>2834</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7232,7 +9974,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>1921</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7268,7 +10010,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>1922</v>
+        <v>2836</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7304,7 +10046,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>1923</v>
+        <v>2837</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7340,7 +10082,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>1924</v>
+        <v>2838</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7376,7 +10118,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>1925</v>
+        <v>2839</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7412,7 +10154,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>1926</v>
+        <v>2840</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7448,7 +10190,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>1927</v>
+        <v>2841</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7484,7 +10226,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>1928</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7518,7 +10260,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>1929</v>
+        <v>2843</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7552,7 +10294,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>1930</v>
+        <v>2844</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7588,7 +10330,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>1931</v>
+        <v>2845</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7624,7 +10366,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>1932</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7660,7 +10402,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>1933</v>
+        <v>2847</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7696,7 +10438,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>1934</v>
+        <v>2848</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7732,7 +10474,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>1935</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7768,7 +10510,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>1936</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7802,7 +10544,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>1937</v>
+        <v>2851</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7838,7 +10580,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>1938</v>
+        <v>2852</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7874,7 +10616,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>1939</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7910,7 +10652,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>1940</v>
+        <v>2854</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7946,7 +10688,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>1941</v>
+        <v>2855</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7982,7 +10724,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>1942</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8018,7 +10760,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>1943</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8054,7 +10796,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>1944</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8088,7 +10830,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>1945</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8122,7 +10864,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>1946</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8158,7 +10900,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>1947</v>
+        <v>2861</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8194,7 +10936,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>1948</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8230,7 +10972,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>1949</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8266,7 +11008,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>1950</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8302,7 +11044,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>1951</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8338,7 +11080,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>1952</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8374,7 +11116,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>1954</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8410,7 +11152,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>1955</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8446,7 +11188,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>1956</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8482,7 +11224,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>1953</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8518,7 +11260,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>1957</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8554,7 +11296,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>1958</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8590,7 +11332,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>1959</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8626,7 +11368,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>1960</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8660,7 +11402,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>1961</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8696,7 +11438,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>1962</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8728,7 +11470,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>1963</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8764,7 +11506,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>1972</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8796,7 +11538,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>1973</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8828,7 +11570,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>1974</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8860,7 +11602,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>1975</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8892,7 +11634,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>1976</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8924,7 +11666,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>1977</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8956,7 +11698,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>1978</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8988,7 +11730,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>1979</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9022,7 +11764,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>1964</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9058,7 +11800,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>1967</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9092,7 +11834,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>1968</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9126,7 +11868,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>1965</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9194,7 +11936,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>1966</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9226,7 +11968,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>1969</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9258,7 +12000,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>1970</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9290,7 +12032,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>1971</v>
+        <v>2885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix - unnecessary tags  removed
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="2894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3521" uniqueCount="3032">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -8783,6 +8783,420 @@
   </si>
   <si>
     <t>480089946</t>
+  </si>
+  <si>
+    <t>482740813</t>
+  </si>
+  <si>
+    <t>482751581</t>
+  </si>
+  <si>
+    <t>482753530</t>
+  </si>
+  <si>
+    <t>482754677</t>
+  </si>
+  <si>
+    <t>482755963</t>
+  </si>
+  <si>
+    <t>482757262</t>
+  </si>
+  <si>
+    <t>482758682</t>
+  </si>
+  <si>
+    <t>482759899</t>
+  </si>
+  <si>
+    <t>482761314</t>
+  </si>
+  <si>
+    <t>482762505</t>
+  </si>
+  <si>
+    <t>482764072</t>
+  </si>
+  <si>
+    <t>482765353</t>
+  </si>
+  <si>
+    <t>482766647</t>
+  </si>
+  <si>
+    <t>482767911</t>
+  </si>
+  <si>
+    <t>482769276</t>
+  </si>
+  <si>
+    <t>482770622</t>
+  </si>
+  <si>
+    <t>482772325</t>
+  </si>
+  <si>
+    <t>482773627</t>
+  </si>
+  <si>
+    <t>482775239</t>
+  </si>
+  <si>
+    <t>482776618</t>
+  </si>
+  <si>
+    <t>482778302</t>
+  </si>
+  <si>
+    <t>482779838</t>
+  </si>
+  <si>
+    <t>482781676</t>
+  </si>
+  <si>
+    <t>482783215</t>
+  </si>
+  <si>
+    <t>482784974</t>
+  </si>
+  <si>
+    <t>482786519</t>
+  </si>
+  <si>
+    <t>482788065</t>
+  </si>
+  <si>
+    <t>482789741</t>
+  </si>
+  <si>
+    <t>482791808</t>
+  </si>
+  <si>
+    <t>482793395</t>
+  </si>
+  <si>
+    <t>482795055</t>
+  </si>
+  <si>
+    <t>482797068</t>
+  </si>
+  <si>
+    <t>482798713</t>
+  </si>
+  <si>
+    <t>482800568</t>
+  </si>
+  <si>
+    <t>482802587</t>
+  </si>
+  <si>
+    <t>482804273</t>
+  </si>
+  <si>
+    <t>482806055</t>
+  </si>
+  <si>
+    <t>482807965</t>
+  </si>
+  <si>
+    <t>482809928</t>
+  </si>
+  <si>
+    <t>482812761</t>
+  </si>
+  <si>
+    <t>482814979</t>
+  </si>
+  <si>
+    <t>482817036</t>
+  </si>
+  <si>
+    <t>482819179</t>
+  </si>
+  <si>
+    <t>482821661</t>
+  </si>
+  <si>
+    <t>482823934</t>
+  </si>
+  <si>
+    <t>482826036</t>
+  </si>
+  <si>
+    <t>482828355</t>
+  </si>
+  <si>
+    <t>482830807</t>
+  </si>
+  <si>
+    <t>482832895</t>
+  </si>
+  <si>
+    <t>482835105</t>
+  </si>
+  <si>
+    <t>482837225</t>
+  </si>
+  <si>
+    <t>482839549</t>
+  </si>
+  <si>
+    <t>482841975</t>
+  </si>
+  <si>
+    <t>482844443</t>
+  </si>
+  <si>
+    <t>482847666</t>
+  </si>
+  <si>
+    <t>482854194</t>
+  </si>
+  <si>
+    <t>482857556</t>
+  </si>
+  <si>
+    <t>482860508</t>
+  </si>
+  <si>
+    <t>482864667</t>
+  </si>
+  <si>
+    <t>482867856</t>
+  </si>
+  <si>
+    <t>482870790</t>
+  </si>
+  <si>
+    <t>482874381</t>
+  </si>
+  <si>
+    <t>482877629</t>
+  </si>
+  <si>
+    <t>482881210</t>
+  </si>
+  <si>
+    <t>482884597</t>
+  </si>
+  <si>
+    <t>482887832</t>
+  </si>
+  <si>
+    <t>482891454</t>
+  </si>
+  <si>
+    <t>482895901</t>
+  </si>
+  <si>
+    <t>482903736</t>
+  </si>
+  <si>
+    <t>501726448</t>
+  </si>
+  <si>
+    <t>501739339</t>
+  </si>
+  <si>
+    <t>501742110</t>
+  </si>
+  <si>
+    <t>501744782</t>
+  </si>
+  <si>
+    <t>501747262</t>
+  </si>
+  <si>
+    <t>501750036</t>
+  </si>
+  <si>
+    <t>501752825</t>
+  </si>
+  <si>
+    <t>501755118</t>
+  </si>
+  <si>
+    <t>501757539</t>
+  </si>
+  <si>
+    <t>501760306</t>
+  </si>
+  <si>
+    <t>501763047</t>
+  </si>
+  <si>
+    <t>501765110</t>
+  </si>
+  <si>
+    <t>501767473</t>
+  </si>
+  <si>
+    <t>501769640</t>
+  </si>
+  <si>
+    <t>501772146</t>
+  </si>
+  <si>
+    <t>501774837</t>
+  </si>
+  <si>
+    <t>501778314</t>
+  </si>
+  <si>
+    <t>501781234</t>
+  </si>
+  <si>
+    <t>501784796</t>
+  </si>
+  <si>
+    <t>501789032</t>
+  </si>
+  <si>
+    <t>501792672</t>
+  </si>
+  <si>
+    <t>501796195</t>
+  </si>
+  <si>
+    <t>501799602</t>
+  </si>
+  <si>
+    <t>501803087</t>
+  </si>
+  <si>
+    <t>501806235</t>
+  </si>
+  <si>
+    <t>501809237</t>
+  </si>
+  <si>
+    <t>501810977</t>
+  </si>
+  <si>
+    <t>501813223</t>
+  </si>
+  <si>
+    <t>501815477</t>
+  </si>
+  <si>
+    <t>501818155</t>
+  </si>
+  <si>
+    <t>501820380</t>
+  </si>
+  <si>
+    <t>501822604</t>
+  </si>
+  <si>
+    <t>501824833</t>
+  </si>
+  <si>
+    <t>501827115</t>
+  </si>
+  <si>
+    <t>501829269</t>
+  </si>
+  <si>
+    <t>501831473</t>
+  </si>
+  <si>
+    <t>501833725</t>
+  </si>
+  <si>
+    <t>501836195</t>
+  </si>
+  <si>
+    <t>501838393</t>
+  </si>
+  <si>
+    <t>501840979</t>
+  </si>
+  <si>
+    <t>501845769</t>
+  </si>
+  <si>
+    <t>501849918</t>
+  </si>
+  <si>
+    <t>501854646</t>
+  </si>
+  <si>
+    <t>501859139</t>
+  </si>
+  <si>
+    <t>501863171</t>
+  </si>
+  <si>
+    <t>501867580</t>
+  </si>
+  <si>
+    <t>501872414</t>
+  </si>
+  <si>
+    <t>501876607</t>
+  </si>
+  <si>
+    <t>501881075</t>
+  </si>
+  <si>
+    <t>501885683</t>
+  </si>
+  <si>
+    <t>501892058</t>
+  </si>
+  <si>
+    <t>501896543</t>
+  </si>
+  <si>
+    <t>501899839</t>
+  </si>
+  <si>
+    <t>501902720</t>
+  </si>
+  <si>
+    <t>501906988</t>
+  </si>
+  <si>
+    <t>501914292</t>
+  </si>
+  <si>
+    <t>501920581</t>
+  </si>
+  <si>
+    <t>501927085</t>
+  </si>
+  <si>
+    <t>501934756</t>
+  </si>
+  <si>
+    <t>501941139</t>
+  </si>
+  <si>
+    <t>501948292</t>
+  </si>
+  <si>
+    <t>501955025</t>
+  </si>
+  <si>
+    <t>501960768</t>
+  </si>
+  <si>
+    <t>501965491</t>
+  </si>
+  <si>
+    <t>501970378</t>
+  </si>
+  <si>
+    <t>501974916</t>
+  </si>
+  <si>
+    <t>501979576</t>
+  </si>
+  <si>
+    <t>501984114</t>
+  </si>
+  <si>
+    <t>501989016</t>
   </si>
 </sst>
 </file>
@@ -9414,7 +9828,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>2825</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9654,7 +10068,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>2826</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9690,7 +10104,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>2827</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9726,7 +10140,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>2828</v>
+        <v>2966</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9762,7 +10176,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>2829</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9798,7 +10212,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>2830</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9832,7 +10246,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>2831</v>
+        <v>2969</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9866,7 +10280,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>2832</v>
+        <v>2970</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9902,7 +10316,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>2833</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9938,7 +10352,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>2834</v>
+        <v>2972</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9974,7 +10388,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>2835</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10010,7 +10424,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>2836</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10046,7 +10460,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>2837</v>
+        <v>2975</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10082,7 +10496,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>2838</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10118,7 +10532,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>2839</v>
+        <v>2977</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10154,7 +10568,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>2840</v>
+        <v>2978</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10190,7 +10604,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>2841</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10226,7 +10640,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>2842</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10260,7 +10674,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>2843</v>
+        <v>2981</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10294,7 +10708,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>2844</v>
+        <v>2982</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10330,7 +10744,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>2845</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10366,7 +10780,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>2846</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10402,7 +10816,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>2847</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10438,7 +10852,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>2848</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10474,7 +10888,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>2849</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10510,7 +10924,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>2850</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10544,7 +10958,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>2851</v>
+        <v>2989</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10580,7 +10994,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>2852</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10616,7 +11030,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>2853</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10652,7 +11066,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>2854</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10688,7 +11102,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>2855</v>
+        <v>2993</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10724,7 +11138,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>2856</v>
+        <v>2994</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10760,7 +11174,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>2857</v>
+        <v>2995</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10796,7 +11210,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>2858</v>
+        <v>2996</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10830,7 +11244,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>2859</v>
+        <v>2997</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10864,7 +11278,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>2860</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10900,7 +11314,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>2861</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10936,7 +11350,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>2862</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10972,7 +11386,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>2863</v>
+        <v>3001</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11008,7 +11422,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>2864</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11044,7 +11458,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>2865</v>
+        <v>3003</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11080,7 +11494,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>2866</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11116,7 +11530,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>2868</v>
+        <v>3006</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11152,7 +11566,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>2869</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11188,7 +11602,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>2870</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11224,7 +11638,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>2867</v>
+        <v>3005</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11260,7 +11674,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>2871</v>
+        <v>3009</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11296,7 +11710,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>2872</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11332,7 +11746,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>2873</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11368,7 +11782,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>2874</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11402,7 +11816,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>2875</v>
+        <v>3013</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11438,7 +11852,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>2876</v>
+        <v>3014</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11470,7 +11884,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>2877</v>
+        <v>3015</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11506,7 +11920,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>2886</v>
+        <v>3024</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11538,7 +11952,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>2887</v>
+        <v>3025</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11570,7 +11984,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>2888</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11602,7 +12016,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>2889</v>
+        <v>3027</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11634,7 +12048,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>2890</v>
+        <v>3028</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11666,7 +12080,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>2891</v>
+        <v>3029</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11698,7 +12112,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>2892</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11730,7 +12144,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>2893</v>
+        <v>3031</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11764,7 +12178,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>2878</v>
+        <v>3016</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11800,7 +12214,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>2881</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11834,7 +12248,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>2882</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11868,7 +12282,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>2879</v>
+        <v>3017</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11936,7 +12350,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>2880</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11968,7 +12382,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>2883</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12000,7 +12414,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>2884</v>
+        <v>3022</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12032,7 +12446,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>2885</v>
+        <v>3023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix - unnecessary system.out.println  removed
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Booking_Creation_DataSet.xlsx
+++ b/src/test/resources/testData/Booking_Creation_DataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3521" uniqueCount="3032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3659" uniqueCount="3170">
   <si>
     <t xml:space="preserve">dataset</t>
   </si>
@@ -9197,6 +9197,420 @@
   </si>
   <si>
     <t>501989016</t>
+  </si>
+  <si>
+    <t>775941275</t>
+  </si>
+  <si>
+    <t>775984304</t>
+  </si>
+  <si>
+    <t>775986152</t>
+  </si>
+  <si>
+    <t>775987080</t>
+  </si>
+  <si>
+    <t>775988344</t>
+  </si>
+  <si>
+    <t>775989397</t>
+  </si>
+  <si>
+    <t>775990772</t>
+  </si>
+  <si>
+    <t>775991762</t>
+  </si>
+  <si>
+    <t>775993135</t>
+  </si>
+  <si>
+    <t>775994168</t>
+  </si>
+  <si>
+    <t>775995616</t>
+  </si>
+  <si>
+    <t>775996803</t>
+  </si>
+  <si>
+    <t>775997926</t>
+  </si>
+  <si>
+    <t>775999047</t>
+  </si>
+  <si>
+    <t>776000288</t>
+  </si>
+  <si>
+    <t>776001358</t>
+  </si>
+  <si>
+    <t>776002886</t>
+  </si>
+  <si>
+    <t>776004197</t>
+  </si>
+  <si>
+    <t>776005760</t>
+  </si>
+  <si>
+    <t>776006978</t>
+  </si>
+  <si>
+    <t>776008512</t>
+  </si>
+  <si>
+    <t>776009912</t>
+  </si>
+  <si>
+    <t>776011608</t>
+  </si>
+  <si>
+    <t>776013063</t>
+  </si>
+  <si>
+    <t>776014459</t>
+  </si>
+  <si>
+    <t>776015876</t>
+  </si>
+  <si>
+    <t>776017421</t>
+  </si>
+  <si>
+    <t>776018828</t>
+  </si>
+  <si>
+    <t>776020622</t>
+  </si>
+  <si>
+    <t>776022069</t>
+  </si>
+  <si>
+    <t>776023833</t>
+  </si>
+  <si>
+    <t>776025425</t>
+  </si>
+  <si>
+    <t>776026950</t>
+  </si>
+  <si>
+    <t>776028523</t>
+  </si>
+  <si>
+    <t>776030429</t>
+  </si>
+  <si>
+    <t>776032014</t>
+  </si>
+  <si>
+    <t>776033849</t>
+  </si>
+  <si>
+    <t>776035527</t>
+  </si>
+  <si>
+    <t>776037184</t>
+  </si>
+  <si>
+    <t>776039179</t>
+  </si>
+  <si>
+    <t>776040922</t>
+  </si>
+  <si>
+    <t>776042671</t>
+  </si>
+  <si>
+    <t>776044482</t>
+  </si>
+  <si>
+    <t>776046290</t>
+  </si>
+  <si>
+    <t>776047948</t>
+  </si>
+  <si>
+    <t>776049832</t>
+  </si>
+  <si>
+    <t>776051697</t>
+  </si>
+  <si>
+    <t>776053531</t>
+  </si>
+  <si>
+    <t>776055517</t>
+  </si>
+  <si>
+    <t>776057361</t>
+  </si>
+  <si>
+    <t>776059518</t>
+  </si>
+  <si>
+    <t>776061721</t>
+  </si>
+  <si>
+    <t>776064415</t>
+  </si>
+  <si>
+    <t>776066726</t>
+  </si>
+  <si>
+    <t>776069940</t>
+  </si>
+  <si>
+    <t>776074492</t>
+  </si>
+  <si>
+    <t>776077447</t>
+  </si>
+  <si>
+    <t>776080105</t>
+  </si>
+  <si>
+    <t>776083513</t>
+  </si>
+  <si>
+    <t>776086441</t>
+  </si>
+  <si>
+    <t>776089186</t>
+  </si>
+  <si>
+    <t>776091896</t>
+  </si>
+  <si>
+    <t>776094766</t>
+  </si>
+  <si>
+    <t>776097646</t>
+  </si>
+  <si>
+    <t>776100912</t>
+  </si>
+  <si>
+    <t>776103870</t>
+  </si>
+  <si>
+    <t>776107225</t>
+  </si>
+  <si>
+    <t>776109977</t>
+  </si>
+  <si>
+    <t>776112721</t>
+  </si>
+  <si>
+    <t>945515761</t>
+  </si>
+  <si>
+    <t>945525749</t>
+  </si>
+  <si>
+    <t>945527232</t>
+  </si>
+  <si>
+    <t>945528070</t>
+  </si>
+  <si>
+    <t>945529254</t>
+  </si>
+  <si>
+    <t>945530144</t>
+  </si>
+  <si>
+    <t>945531062</t>
+  </si>
+  <si>
+    <t>945532327</t>
+  </si>
+  <si>
+    <t>945533515</t>
+  </si>
+  <si>
+    <t>945534481</t>
+  </si>
+  <si>
+    <t>945535764</t>
+  </si>
+  <si>
+    <t>945536778</t>
+  </si>
+  <si>
+    <t>945537874</t>
+  </si>
+  <si>
+    <t>945538935</t>
+  </si>
+  <si>
+    <t>945540444</t>
+  </si>
+  <si>
+    <t>945541514</t>
+  </si>
+  <si>
+    <t>945542936</t>
+  </si>
+  <si>
+    <t>945544108</t>
+  </si>
+  <si>
+    <t>945545512</t>
+  </si>
+  <si>
+    <t>945546935</t>
+  </si>
+  <si>
+    <t>945548368</t>
+  </si>
+  <si>
+    <t>945549544</t>
+  </si>
+  <si>
+    <t>945551047</t>
+  </si>
+  <si>
+    <t>945552363</t>
+  </si>
+  <si>
+    <t>945553649</t>
+  </si>
+  <si>
+    <t>945554921</t>
+  </si>
+  <si>
+    <t>945556217</t>
+  </si>
+  <si>
+    <t>945557536</t>
+  </si>
+  <si>
+    <t>945559139</t>
+  </si>
+  <si>
+    <t>945560799</t>
+  </si>
+  <si>
+    <t>945563169</t>
+  </si>
+  <si>
+    <t>945565733</t>
+  </si>
+  <si>
+    <t>945567813</t>
+  </si>
+  <si>
+    <t>945569997</t>
+  </si>
+  <si>
+    <t>945572217</t>
+  </si>
+  <si>
+    <t>945574354</t>
+  </si>
+  <si>
+    <t>945576889</t>
+  </si>
+  <si>
+    <t>945579701</t>
+  </si>
+  <si>
+    <t>945581921</t>
+  </si>
+  <si>
+    <t>945584513</t>
+  </si>
+  <si>
+    <t>945587045</t>
+  </si>
+  <si>
+    <t>945589275</t>
+  </si>
+  <si>
+    <t>945591951</t>
+  </si>
+  <si>
+    <t>945594326</t>
+  </si>
+  <si>
+    <t>945596595</t>
+  </si>
+  <si>
+    <t>945599073</t>
+  </si>
+  <si>
+    <t>945601484</t>
+  </si>
+  <si>
+    <t>945603891</t>
+  </si>
+  <si>
+    <t>945606359</t>
+  </si>
+  <si>
+    <t>945608963</t>
+  </si>
+  <si>
+    <t>945611269</t>
+  </si>
+  <si>
+    <t>945613802</t>
+  </si>
+  <si>
+    <t>945616388</t>
+  </si>
+  <si>
+    <t>945618547</t>
+  </si>
+  <si>
+    <t>945621825</t>
+  </si>
+  <si>
+    <t>945627257</t>
+  </si>
+  <si>
+    <t>945630129</t>
+  </si>
+  <si>
+    <t>945632654</t>
+  </si>
+  <si>
+    <t>945634857</t>
+  </si>
+  <si>
+    <t>945638021</t>
+  </si>
+  <si>
+    <t>945641427</t>
+  </si>
+  <si>
+    <t>945644313</t>
+  </si>
+  <si>
+    <t>945647859</t>
+  </si>
+  <si>
+    <t>945651259</t>
+  </si>
+  <si>
+    <t>945655334</t>
+  </si>
+  <si>
+    <t>945658997</t>
+  </si>
+  <si>
+    <t>945662545</t>
+  </si>
+  <si>
+    <t>945665474</t>
+  </si>
+  <si>
+    <t>945668234</t>
   </si>
 </sst>
 </file>
@@ -9828,7 +10242,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>2963</v>
+        <v>3101</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10068,7 +10482,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>2964</v>
+        <v>3102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10104,7 +10518,7 @@
         <v>23</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>2965</v>
+        <v>3103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10140,7 +10554,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>2966</v>
+        <v>3104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10176,7 +10590,7 @@
         <v>23</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>2967</v>
+        <v>3105</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10212,7 +10626,7 @@
         <v>20</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>2968</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10246,7 +10660,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>2969</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10280,7 +10694,7 @@
         <v>23</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>2970</v>
+        <v>3108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10316,7 +10730,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>2971</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10352,7 +10766,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>2972</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10388,7 +10802,7 @@
         <v>20</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>2973</v>
+        <v>3111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10424,7 +10838,7 @@
         <v>20</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>2974</v>
+        <v>3112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10460,7 +10874,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>2975</v>
+        <v>3113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10496,7 +10910,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>2976</v>
+        <v>3114</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10532,7 +10946,7 @@
         <v>23</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>2977</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10568,7 +10982,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>2978</v>
+        <v>3116</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10604,7 +11018,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>2979</v>
+        <v>3117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10640,7 +11054,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>2980</v>
+        <v>3118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10674,7 +11088,7 @@
         <v>23</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>2981</v>
+        <v>3119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10708,7 +11122,7 @@
         <v>23</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>2982</v>
+        <v>3120</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10744,7 +11158,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>2983</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10780,7 +11194,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>2984</v>
+        <v>3122</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10816,7 +11230,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>2985</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10852,7 +11266,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>2986</v>
+        <v>3124</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10888,7 +11302,7 @@
         <v>20</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>2987</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10924,7 +11338,7 @@
         <v>20</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>2988</v>
+        <v>3126</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10958,7 +11372,7 @@
         <v>23</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>2989</v>
+        <v>3127</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10994,7 +11408,7 @@
         <v>23</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>2990</v>
+        <v>3128</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11030,7 +11444,7 @@
         <v>23</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>2991</v>
+        <v>3129</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11066,7 +11480,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>2992</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11102,7 +11516,7 @@
         <v>20</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>2993</v>
+        <v>3131</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11138,7 +11552,7 @@
         <v>23</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>2994</v>
+        <v>3132</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11174,7 +11588,7 @@
         <v>23</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>2995</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11210,7 +11624,7 @@
         <v>23</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>2996</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11244,7 +11658,7 @@
         <v>23</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>2997</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11278,7 +11692,7 @@
         <v>23</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>2998</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11314,7 +11728,7 @@
         <v>20</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>2999</v>
+        <v>3137</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11350,7 +11764,7 @@
         <v>23</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>3000</v>
+        <v>3138</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11386,7 +11800,7 @@
         <v>23</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>3001</v>
+        <v>3139</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11422,7 +11836,7 @@
         <v>20</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>3002</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11458,7 +11872,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>3003</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11494,7 +11908,7 @@
         <v>20</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>3004</v>
+        <v>3142</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11530,7 +11944,7 @@
         <v>23</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>3006</v>
+        <v>3144</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11566,7 +11980,7 @@
         <v>23</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>3007</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11602,7 +12016,7 @@
         <v>23</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>3008</v>
+        <v>3146</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11638,7 +12052,7 @@
         <v>23</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>3005</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11674,7 +12088,7 @@
         <v>20</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>3009</v>
+        <v>3147</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11710,7 +12124,7 @@
         <v>20</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>3010</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11746,7 +12160,7 @@
         <v>23</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>3011</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11782,7 +12196,7 @@
         <v>23</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>3012</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11816,7 +12230,7 @@
         <v>23</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>3013</v>
+        <v>3151</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11852,7 +12266,7 @@
         <v>20</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>3014</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11884,7 +12298,7 @@
       <c r="J60" s="26"/>
       <c r="K60" s="7"/>
       <c r="L60" s="8" t="s">
-        <v>3015</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11920,7 +12334,7 @@
         <v>20</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>3024</v>
+        <v>3162</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11952,7 +12366,7 @@
       <c r="J62" s="26"/>
       <c r="K62" s="7"/>
       <c r="L62" s="8" t="s">
-        <v>3025</v>
+        <v>3163</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11984,7 +12398,7 @@
       <c r="J63" s="26"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8" t="s">
-        <v>3026</v>
+        <v>3164</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12016,7 +12430,7 @@
       <c r="J64" s="26"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8" t="s">
-        <v>3027</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12048,7 +12462,7 @@
       <c r="J65" s="26"/>
       <c r="K65" s="7"/>
       <c r="L65" s="8" t="s">
-        <v>3028</v>
+        <v>3166</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12080,7 +12494,7 @@
       <c r="J66" s="26"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8" t="s">
-        <v>3029</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12112,7 +12526,7 @@
       <c r="J67" s="26"/>
       <c r="K67" s="7"/>
       <c r="L67" s="8" t="s">
-        <v>3030</v>
+        <v>3168</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12144,7 +12558,7 @@
       <c r="J68" s="26"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8" t="s">
-        <v>3031</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12178,7 +12592,7 @@
         <v>171</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>3016</v>
+        <v>3154</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12214,7 +12628,7 @@
         <v>20</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>3019</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12248,7 +12662,7 @@
         <v>171</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>3020</v>
+        <v>3158</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12282,7 +12696,7 @@
         <v>171</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>3017</v>
+        <v>3155</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12350,7 +12764,7 @@
         <v>171</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>3018</v>
+        <v>3156</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12382,7 +12796,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="29"/>
       <c r="L75" s="8" t="s">
-        <v>3021</v>
+        <v>3159</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12414,7 +12828,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="29"/>
       <c r="L76" s="8" t="s">
-        <v>3022</v>
+        <v>3160</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12446,7 +12860,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="29"/>
       <c r="L77" s="30" t="s">
-        <v>3023</v>
+        <v>3161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>